<commit_message>
Error metric for automatic calibration now bank position (wetted edge) error. Also various minor bug fixes and improvements to scenario testing.
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@142 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
   <si>
     <t>Stencil</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Slope - higher resolution</t>
+  </si>
+  <si>
+    <t>Bank Height Bank ID - Bank flux prop to toe transport rate</t>
+  </si>
+  <si>
+    <t>9 but higher res</t>
   </si>
 </sst>
 </file>
@@ -253,21 +259,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -555,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L59" sqref="L59"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1014,9 @@
       <c r="M11">
         <v>60</v>
       </c>
+      <c r="N11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1062,6 +1057,9 @@
       </c>
       <c r="M12">
         <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3162,7 +3160,7 @@
     <mergeCell ref="K1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Minor changes to sensitivity analysis (extra scenarios and other tweaks)
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@143 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
   <si>
     <t>Stencil</t>
   </si>
@@ -167,9 +167,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Preffered?</t>
-  </si>
-  <si>
     <t>dT</t>
   </si>
   <si>
@@ -189,6 +186,69 @@
   </si>
   <si>
     <t>9 but higher res</t>
+  </si>
+  <si>
+    <t>Transport/no-transport ID - bank flux proportional to toe transport</t>
+  </si>
+  <si>
+    <t>Delft3D but transport/non-transport ID and stencil</t>
+  </si>
+  <si>
+    <t>9 + stencil</t>
+  </si>
+  <si>
+    <t>9 + stencil + higher res</t>
+  </si>
+  <si>
+    <t>13 but higher res</t>
+  </si>
+  <si>
+    <t>13 but stencil</t>
+  </si>
+  <si>
+    <t>13 + stencil + higher res</t>
+  </si>
+  <si>
+    <t>13 + degrading toe trigger</t>
+  </si>
+  <si>
+    <t>13 + degrading toe trigger + higher res</t>
+  </si>
+  <si>
+    <t>13 + stencil + trigger</t>
+  </si>
+  <si>
+    <t>13 + stencil + trigger + higher res</t>
+  </si>
+  <si>
+    <t>13 + threshold height trigger</t>
+  </si>
+  <si>
+    <t>13 + threshold height trigger + higher res</t>
+  </si>
+  <si>
+    <t>Slope ID - flux proportional to toe transport</t>
+  </si>
+  <si>
+    <t>5 + Higher res</t>
+  </si>
+  <si>
+    <t>5 + stencil</t>
+  </si>
+  <si>
+    <t>5 + stencil + higher res</t>
+  </si>
+  <si>
+    <t>wet/dry ID - Flux proportional to toe transport</t>
+  </si>
+  <si>
+    <t>45 + higher res</t>
+  </si>
+  <si>
+    <t>45 + stencil + higher res</t>
+  </si>
+  <si>
+    <t>45 + stencil</t>
   </si>
 </sst>
 </file>
@@ -259,7 +319,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -543,11 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +667,7 @@
     <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="9.5703125" customWidth="1"/>
-    <col min="14" max="14" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -587,7 +696,7 @@
       </c>
       <c r="L1" s="6"/>
       <c r="M1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -628,7 +737,7 @@
         <v>37</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>5</v>
@@ -719,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -763,7 +872,7 @@
         <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -792,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -807,7 +916,7 @@
         <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -815,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -845,9 +954,12 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M7">
+        <v>60</v>
+      </c>
+      <c r="N7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -856,7 +968,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -877,7 +989,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -886,10 +998,13 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M8">
         <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -897,7 +1012,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -912,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -927,10 +1042,13 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M9">
         <v>60</v>
+      </c>
+      <c r="N9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -938,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -953,13 +1071,13 @@
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
@@ -968,11 +1086,14 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M10">
         <v>20</v>
       </c>
+      <c r="N10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1009,13 +1130,13 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M11">
         <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1044,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -1053,13 +1174,13 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M12">
         <v>20</v>
       </c>
       <c r="N12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1070,13 +1191,13 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1097,10 +1218,13 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M13">
         <v>60</v>
+      </c>
+      <c r="N13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1111,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1129,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J14" t="s">
         <v>9</v>
@@ -1138,10 +1262,13 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M14">
         <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1158,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1179,13 +1306,13 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M15">
         <v>60</v>
       </c>
       <c r="N15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1202,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1214,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J16" t="s">
         <v>9</v>
@@ -1223,21 +1350,21 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M16">
         <v>20</v>
       </c>
       <c r="N16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1246,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1261,24 +1388,27 @@
         <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M17">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1287,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1299,22 +1429,25 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1328,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1349,13 +1482,13 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M19">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1369,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1381,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J20" t="s">
         <v>10</v>
@@ -1390,18 +1523,18 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1410,10 +1543,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
         <v>3</v>
@@ -1425,24 +1558,24 @@
         <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M21">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1451,10 +1584,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
         <v>3</v>
@@ -1463,22 +1596,22 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1492,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>2</v>
@@ -1513,13 +1646,16 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M23">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1533,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -1545,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J24" t="s">
         <v>9</v>
@@ -1554,18 +1690,21 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1574,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -1589,24 +1728,27 @@
         <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M25">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1615,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -1627,22 +1769,25 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1656,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -1677,13 +1822,13 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M27">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1697,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>2</v>
@@ -1709,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J28" t="s">
         <v>10</v>
@@ -1718,18 +1863,18 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M28">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1738,10 +1883,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" s="2">
         <v>3</v>
@@ -1753,24 +1898,24 @@
         <v>35</v>
       </c>
       <c r="J29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M29">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1779,10 +1924,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" s="2">
         <v>3</v>
@@ -1791,22 +1936,22 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M30">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1820,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1841,13 +1986,16 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M31">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1861,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1873,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J32" t="s">
         <v>9</v>
@@ -1882,10 +2030,13 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M32">
         <v>20</v>
+      </c>
+      <c r="N32" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1893,7 +2044,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1902,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1917,16 +2068,19 @@
         <v>35</v>
       </c>
       <c r="J33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M33">
         <v>60</v>
+      </c>
+      <c r="N33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1934,7 +2088,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1943,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1955,19 +2109,22 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M34">
         <v>20</v>
+      </c>
+      <c r="N34" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1984,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2005,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M35">
         <v>60</v>
@@ -2025,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2037,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J36" t="s">
         <v>10</v>
@@ -2046,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M36">
         <v>20</v>
@@ -2066,10 +2223,10 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G37" s="2">
         <v>3</v>
@@ -2081,13 +2238,13 @@
         <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
       <c r="L37">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M37">
         <v>60</v>
@@ -2107,10 +2264,10 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G38" s="2">
         <v>3</v>
@@ -2119,16 +2276,16 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M38">
         <v>20</v>
@@ -2148,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -2169,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M39">
         <v>60</v>
@@ -2189,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <v>3</v>
@@ -2201,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J40" t="s">
         <v>9</v>
@@ -2210,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M40">
         <v>20</v>
@@ -2230,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41">
         <v>3</v>
@@ -2245,13 +2402,13 @@
         <v>35</v>
       </c>
       <c r="J41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M41">
         <v>60</v>
@@ -2271,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42">
         <v>3</v>
@@ -2283,16 +2440,16 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M42">
         <v>20</v>
@@ -2312,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -2333,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="L43">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M43">
         <v>60</v>
@@ -2353,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -2365,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J44" t="s">
         <v>10</v>
@@ -2374,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M44">
         <v>20</v>
@@ -2388,16 +2545,16 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45">
-        <v>999</v>
+        <v>3</v>
       </c>
       <c r="G45" s="2">
         <v>3</v>
@@ -2409,19 +2566,16 @@
         <v>35</v>
       </c>
       <c r="J45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
       <c r="L45">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M45">
         <v>60</v>
-      </c>
-      <c r="N45" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2432,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2441,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="F46">
-        <v>999</v>
+        <v>3</v>
       </c>
       <c r="G46" s="2">
         <v>3</v>
@@ -2450,19 +2604,19 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M46">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2470,7 +2624,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2482,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="G47" s="2">
         <v>3</v>
@@ -2491,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="J47" t="s">
         <v>9</v>
@@ -2500,18 +2654,21 @@
         <v>0</v>
       </c>
       <c r="L47">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M47">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N47" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2520,10 +2677,10 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2">
         <v>3</v>
@@ -2532,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J48" t="s">
         <v>9</v>
@@ -2541,18 +2698,21 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M48">
         <v>20</v>
       </c>
+      <c r="N48" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2561,10 +2721,10 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2">
         <v>3</v>
@@ -2576,19 +2736,19 @@
         <v>35</v>
       </c>
       <c r="J49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M49">
         <v>60</v>
       </c>
       <c r="N49" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2596,7 +2756,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2608,7 +2768,7 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="G50" s="2">
         <v>3</v>
@@ -2617,19 +2777,22 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M50">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N50" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2649,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="G51" s="2">
         <v>3</v>
@@ -2658,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="J51" t="s">
         <v>10</v>
@@ -2667,15 +2830,18 @@
         <v>0</v>
       </c>
       <c r="L51">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M51">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N51" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -2687,10 +2853,10 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="G52" s="2">
         <v>3</v>
@@ -2699,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J52" t="s">
         <v>10</v>
@@ -2708,7 +2874,7 @@
         <v>0</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M52">
         <v>20</v>
@@ -2716,10 +2882,10 @@
     </row>
     <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2728,34 +2894,31 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>35</v>
       </c>
       <c r="J53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M53">
         <v>60</v>
-      </c>
-      <c r="N53" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2763,7 +2926,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2772,34 +2935,31 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54">
         <v>0</v>
       </c>
       <c r="G54" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M54">
         <v>20</v>
-      </c>
-      <c r="N54" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2810,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2837,13 +2997,13 @@
         <v>0</v>
       </c>
       <c r="L55">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M55">
         <v>60</v>
       </c>
       <c r="N55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2854,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2872,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J56" t="s">
         <v>9</v>
@@ -2881,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M56">
         <v>20</v>
       </c>
       <c r="N56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2898,7 +3058,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2913,7 +3073,7 @@
         <v>4</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="s">
         <v>35</v>
@@ -2925,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="L57">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M57">
         <v>60</v>
@@ -2942,7 +3102,7 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2957,10 +3117,10 @@
         <v>4</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J58" t="s">
         <v>9</v>
@@ -2969,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="L58">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M58">
         <v>20</v>
@@ -2998,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3013,13 +3173,13 @@
         <v>0</v>
       </c>
       <c r="L59">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M59">
         <v>60</v>
       </c>
       <c r="N59" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3042,13 +3202,13 @@
         <v>0</v>
       </c>
       <c r="G60" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J60" t="s">
         <v>9</v>
@@ -3057,13 +3217,13 @@
         <v>0</v>
       </c>
       <c r="L60">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M60">
         <v>20</v>
       </c>
       <c r="N60" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3074,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3107,7 +3267,7 @@
         <v>60</v>
       </c>
       <c r="N61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3118,7 +3278,7 @@
         <v>1</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3136,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J62" t="s">
         <v>9</v>
@@ -3151,7 +3311,183 @@
         <v>20</v>
       </c>
       <c r="N62" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="b">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63" s="2">
+        <v>2</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63" t="s">
+        <v>9</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <v>60</v>
+      </c>
+      <c r="N63" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>2</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>42</v>
+      </c>
+      <c r="J64" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>20</v>
+      </c>
+      <c r="N64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="b">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65" s="2">
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" t="s">
+        <v>9</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>60</v>
+      </c>
+      <c r="N65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="b">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" s="2">
+        <v>2</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>42</v>
+      </c>
+      <c r="J66" t="s">
+        <v>9</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>20</v>
+      </c>
+      <c r="N66" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3159,9 +3495,19 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="K1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A3:XFD48 A49:M50 O49:XFD50 A51:XFD1048576">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$B3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N50">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$B49</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N49">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$B49</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Altering structure of input variable to tidy up a bit and modifying ReadModelInputs.m to make ReadAllModelInputs.m obsolete to prevent duplication of code.
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@145 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="70">
   <si>
     <t>Stencil</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>45 + stencil</t>
+  </si>
+  <si>
+    <t>Inputs\Selwyn_XS3_0.25m.csv</t>
+  </si>
+  <si>
+    <t>9 but v high res</t>
   </si>
 </sst>
 </file>
@@ -319,28 +325,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -652,11 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +649,7 @@
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="9.5703125" customWidth="1"/>
     <col min="14" max="14" width="61" bestFit="1" customWidth="1"/>
@@ -1197,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1209,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="J13" t="s">
         <v>9</v>
@@ -1221,10 +1206,10 @@
         <v>0.1</v>
       </c>
       <c r="M13">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="N13" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1253,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
         <v>9</v>
@@ -1265,10 +1250,10 @@
         <v>0.1</v>
       </c>
       <c r="M14">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1279,13 +1264,13 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1297,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
@@ -1309,10 +1294,10 @@
         <v>0.1</v>
       </c>
       <c r="M15">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1341,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
         <v>9</v>
@@ -1353,10 +1338,10 @@
         <v>0.1</v>
       </c>
       <c r="M16">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1373,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1385,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J17" t="s">
         <v>9</v>
@@ -1397,10 +1382,10 @@
         <v>0.1</v>
       </c>
       <c r="M17">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1429,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
         <v>9</v>
@@ -1441,10 +1426,10 @@
         <v>0.1</v>
       </c>
       <c r="M18">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1452,7 +1437,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1461,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1473,10 +1458,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1485,7 +1470,10 @@
         <v>0.1</v>
       </c>
       <c r="M19">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1514,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
         <v>10</v>
@@ -1526,7 +1514,7 @@
         <v>0.1</v>
       </c>
       <c r="M20">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1543,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1555,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J21" t="s">
         <v>10</v>
@@ -1567,7 +1555,7 @@
         <v>0.1</v>
       </c>
       <c r="M21">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1596,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J22" t="s">
         <v>10</v>
@@ -1608,7 +1596,7 @@
         <v>0.1</v>
       </c>
       <c r="M22">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1616,7 +1604,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1625,10 +1613,10 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2">
         <v>3</v>
@@ -1637,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1649,10 +1637,7 @@
         <v>0.1</v>
       </c>
       <c r="M23">
-        <v>60</v>
-      </c>
-      <c r="N23" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1681,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J24" t="s">
         <v>9</v>
@@ -1693,10 +1678,10 @@
         <v>0.1</v>
       </c>
       <c r="M24">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1713,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -1725,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J25" t="s">
         <v>9</v>
@@ -1737,10 +1722,10 @@
         <v>0.1</v>
       </c>
       <c r="M25">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1769,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
         <v>9</v>
@@ -1781,10 +1766,10 @@
         <v>0.1</v>
       </c>
       <c r="M26">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1792,7 +1777,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -1801,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -1813,10 +1798,10 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -1825,7 +1810,10 @@
         <v>0.1</v>
       </c>
       <c r="M27">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N27" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1854,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
         <v>10</v>
@@ -1866,7 +1854,7 @@
         <v>0.1</v>
       </c>
       <c r="M28">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1883,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -1895,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J29" t="s">
         <v>10</v>
@@ -1907,7 +1895,7 @@
         <v>0.1</v>
       </c>
       <c r="M29">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1936,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J30" t="s">
         <v>10</v>
@@ -1948,7 +1936,7 @@
         <v>0.1</v>
       </c>
       <c r="M30">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1956,7 +1944,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1965,10 +1953,10 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" s="2">
         <v>3</v>
@@ -1977,10 +1965,10 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1989,10 +1977,7 @@
         <v>0.1</v>
       </c>
       <c r="M31">
-        <v>60</v>
-      </c>
-      <c r="N31" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2021,7 +2006,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J32" t="s">
         <v>9</v>
@@ -2033,10 +2018,10 @@
         <v>0.1</v>
       </c>
       <c r="M32">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2053,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2065,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J33" t="s">
         <v>9</v>
@@ -2077,10 +2062,10 @@
         <v>0.1</v>
       </c>
       <c r="M33">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N33" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2109,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J34" t="s">
         <v>9</v>
@@ -2121,10 +2106,10 @@
         <v>0.1</v>
       </c>
       <c r="M34">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2132,7 +2117,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2141,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2153,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2165,7 +2150,10 @@
         <v>0.1</v>
       </c>
       <c r="M35">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N35" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2194,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J36" t="s">
         <v>10</v>
@@ -2206,7 +2194,7 @@
         <v>0.1</v>
       </c>
       <c r="M36">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2223,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2235,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J37" t="s">
         <v>10</v>
@@ -2247,7 +2235,7 @@
         <v>0.1</v>
       </c>
       <c r="M37">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2276,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J38" t="s">
         <v>10</v>
@@ -2288,7 +2276,7 @@
         <v>0.1</v>
       </c>
       <c r="M38">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2305,10 +2293,10 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2">
         <v>3</v>
@@ -2317,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2329,7 +2317,7 @@
         <v>0.1</v>
       </c>
       <c r="M39">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2358,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J40" t="s">
         <v>9</v>
@@ -2370,7 +2358,7 @@
         <v>0.1</v>
       </c>
       <c r="M40">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2387,7 +2375,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>3</v>
@@ -2399,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J41" t="s">
         <v>9</v>
@@ -2411,7 +2399,7 @@
         <v>0.1</v>
       </c>
       <c r="M41">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2440,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J42" t="s">
         <v>9</v>
@@ -2452,7 +2440,7 @@
         <v>0.1</v>
       </c>
       <c r="M42">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2469,7 +2457,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -2481,10 +2469,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -2493,7 +2481,7 @@
         <v>0.1</v>
       </c>
       <c r="M43">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2522,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J44" t="s">
         <v>10</v>
@@ -2534,7 +2522,7 @@
         <v>0.1</v>
       </c>
       <c r="M44">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2551,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F45">
         <v>3</v>
@@ -2563,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J45" t="s">
         <v>10</v>
@@ -2575,7 +2563,7 @@
         <v>0.1</v>
       </c>
       <c r="M45">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2604,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J46" t="s">
         <v>10</v>
@@ -2616,7 +2604,7 @@
         <v>0.1</v>
       </c>
       <c r="M46">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2624,19 +2612,19 @@
         <v>45</v>
       </c>
       <c r="B47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G47" s="2">
         <v>3</v>
@@ -2645,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -2657,15 +2645,12 @@
         <v>0.1</v>
       </c>
       <c r="M47">
-        <v>60</v>
-      </c>
-      <c r="N47" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -2689,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J48" t="s">
         <v>9</v>
@@ -2701,15 +2686,15 @@
         <v>0.1</v>
       </c>
       <c r="M48">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
@@ -2721,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2733,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J49" t="s">
         <v>9</v>
@@ -2745,10 +2730,10 @@
         <v>0.1</v>
       </c>
       <c r="M49">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2777,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J50" t="s">
         <v>9</v>
@@ -2789,10 +2774,10 @@
         <v>0.1</v>
       </c>
       <c r="M50">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2800,7 +2785,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2809,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2821,10 +2806,10 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -2833,15 +2818,15 @@
         <v>0.1</v>
       </c>
       <c r="M51">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N51" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -2865,7 +2850,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J52" t="s">
         <v>10</v>
@@ -2877,12 +2862,15 @@
         <v>0.1</v>
       </c>
       <c r="M52">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N52" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
@@ -2894,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2906,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J53" t="s">
         <v>10</v>
@@ -2918,7 +2906,7 @@
         <v>0.1</v>
       </c>
       <c r="M53">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2947,7 +2935,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J54" t="s">
         <v>10</v>
@@ -2959,7 +2947,7 @@
         <v>0.1</v>
       </c>
       <c r="M54">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2967,7 +2955,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2976,22 +2964,22 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -3000,10 +2988,7 @@
         <v>0.1</v>
       </c>
       <c r="M55">
-        <v>60</v>
-      </c>
-      <c r="N55" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3032,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J56" t="s">
         <v>9</v>
@@ -3044,7 +3029,7 @@
         <v>0.1</v>
       </c>
       <c r="M56">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N56" t="s">
         <v>7</v>
@@ -3058,7 +3043,7 @@
         <v>1</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -3076,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J57" t="s">
         <v>9</v>
@@ -3088,10 +3073,10 @@
         <v>0.1</v>
       </c>
       <c r="M57">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3120,7 +3105,7 @@
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J58" t="s">
         <v>9</v>
@@ -3132,7 +3117,7 @@
         <v>0.1</v>
       </c>
       <c r="M58">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N58" t="s">
         <v>8</v>
@@ -3146,7 +3131,7 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3161,10 +3146,10 @@
         <v>4</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J59" t="s">
         <v>9</v>
@@ -3176,7 +3161,7 @@
         <v>0.1</v>
       </c>
       <c r="M59">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N59" t="s">
         <v>8</v>
@@ -3208,7 +3193,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J60" t="s">
         <v>9</v>
@@ -3220,7 +3205,7 @@
         <v>0.1</v>
       </c>
       <c r="M60">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N60" t="s">
         <v>8</v>
@@ -3246,13 +3231,13 @@
         <v>0</v>
       </c>
       <c r="G61" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J61" t="s">
         <v>9</v>
@@ -3261,13 +3246,13 @@
         <v>0</v>
       </c>
       <c r="L61">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M61">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N61" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3296,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J62" t="s">
         <v>9</v>
@@ -3308,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="M62">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N62" t="s">
         <v>29</v>
@@ -3322,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -3340,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J63" t="s">
         <v>9</v>
@@ -3352,10 +3337,10 @@
         <v>1</v>
       </c>
       <c r="M63">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3384,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J64" t="s">
         <v>9</v>
@@ -3396,7 +3381,7 @@
         <v>1</v>
       </c>
       <c r="M64">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N64" t="s">
         <v>30</v>
@@ -3416,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -3428,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J65" t="s">
         <v>9</v>
@@ -3440,10 +3425,10 @@
         <v>1</v>
       </c>
       <c r="M65">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N65" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3472,21 +3457,65 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" t="s">
+        <v>9</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>60</v>
+      </c>
+      <c r="N66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67" s="2">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
         <v>42</v>
       </c>
-      <c r="J66" t="s">
-        <v>9</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-      <c r="M66">
+      <c r="J67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
         <v>20</v>
       </c>
-      <c r="N66" t="s">
+      <c r="N67" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3495,19 +3524,19 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="K1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:XFD48 A49:M50 O49:XFD50 A51:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="2">
+  <conditionalFormatting sqref="B50:M51 O50:XFD51 A68:XFD1048576 A3:XFD13 B14:XFD49 B52:XFD67 A14:A67">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$B49</formula>
+  <conditionalFormatting sqref="N51">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$B50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N49">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$B49</formula>
+  <conditionalFormatting sqref="N50">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$B50</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Additional XS data for higher res and for extra validation XS (XS7)
Adding more high res simulations to run list to allow plots of res vs coefficient

git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@156 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="74">
   <si>
     <t>Stencil</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Bank Height Bank ID - Bank flux prop to toe transport rate</t>
   </si>
   <si>
-    <t>9 but higher res</t>
-  </si>
-  <si>
     <t>Transport/no-transport ID - bank flux proportional to toe transport</t>
   </si>
   <si>
@@ -254,7 +251,22 @@
     <t>Inputs\Selwyn_XS3_0.25m.csv</t>
   </si>
   <si>
-    <t>9 but v high res</t>
+    <t>Slope - 0.25m res</t>
+  </si>
+  <si>
+    <t>Slope - 0.1m res</t>
+  </si>
+  <si>
+    <t>Inputs\Selwyn_XS3_0.10m.csv</t>
+  </si>
+  <si>
+    <t>9 but 0.25m res</t>
+  </si>
+  <si>
+    <t>9 but 1m res</t>
+  </si>
+  <si>
+    <t>9 but 0.1m res</t>
   </si>
 </sst>
 </file>
@@ -325,7 +337,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -637,11 +663,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +930,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -912,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -923,32 +949,32 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="2">
-        <v>3</v>
+      <c r="G7">
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L7">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="M7">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -956,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -967,29 +993,29 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="2">
-        <v>3</v>
+      <c r="G8">
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L8">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="M8">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="N8" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1033,7 +1059,7 @@
         <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1077,7 +1103,7 @@
         <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1088,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1121,7 +1147,7 @@
         <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1132,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1165,7 +1191,7 @@
         <v>20</v>
       </c>
       <c r="N12" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1194,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
         <v>9</v>
@@ -1206,10 +1232,10 @@
         <v>0.1</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1226,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1238,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J14" t="s">
         <v>9</v>
@@ -1250,10 +1276,10 @@
         <v>0.1</v>
       </c>
       <c r="M14">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N14" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1270,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1282,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
@@ -1294,10 +1320,10 @@
         <v>0.1</v>
       </c>
       <c r="M15">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="N15" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1308,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1326,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="J16" t="s">
         <v>9</v>
@@ -1338,10 +1364,10 @@
         <v>0.1</v>
       </c>
       <c r="M16">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="N16" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1352,13 +1378,13 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1370,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
         <v>9</v>
@@ -1382,10 +1408,10 @@
         <v>0.1</v>
       </c>
       <c r="M17">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1396,13 +1422,13 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1414,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J18" t="s">
         <v>9</v>
@@ -1426,10 +1452,10 @@
         <v>0.1</v>
       </c>
       <c r="M18">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1446,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1458,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
         <v>9</v>
@@ -1470,10 +1496,10 @@
         <v>0.1</v>
       </c>
       <c r="M19">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1481,7 +1507,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1502,10 +1528,10 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1514,7 +1540,10 @@
         <v>0.1</v>
       </c>
       <c r="M20">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1522,7 +1551,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1531,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1543,10 +1572,10 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1555,7 +1584,10 @@
         <v>0.1</v>
       </c>
       <c r="M21">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1563,7 +1595,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1572,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1584,10 +1616,10 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1596,7 +1628,10 @@
         <v>0.1</v>
       </c>
       <c r="M22">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1613,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1625,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
         <v>10</v>
@@ -1637,7 +1672,7 @@
         <v>0.1</v>
       </c>
       <c r="M23">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1645,7 +1680,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -1657,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2">
         <v>3</v>
@@ -1666,10 +1701,10 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1678,10 +1713,7 @@
         <v>0.1</v>
       </c>
       <c r="M24">
-        <v>60</v>
-      </c>
-      <c r="N24" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1689,7 +1721,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1698,10 +1730,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2">
         <v>3</v>
@@ -1710,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -1722,10 +1754,7 @@
         <v>0.1</v>
       </c>
       <c r="M25">
-        <v>20</v>
-      </c>
-      <c r="N25" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1733,7 +1762,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1742,10 +1771,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2">
         <v>3</v>
@@ -1754,10 +1783,10 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1766,10 +1795,7 @@
         <v>0.1</v>
       </c>
       <c r="M26">
-        <v>60</v>
-      </c>
-      <c r="N26" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1786,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -1798,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
         <v>9</v>
@@ -1810,10 +1836,10 @@
         <v>0.1</v>
       </c>
       <c r="M27">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1821,7 +1847,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1842,10 +1868,10 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1854,7 +1880,10 @@
         <v>0.1</v>
       </c>
       <c r="M28">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1862,7 +1891,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1871,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -1883,10 +1912,10 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -1895,7 +1924,10 @@
         <v>0.1</v>
       </c>
       <c r="M29">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N29" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1903,7 +1935,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1912,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30">
         <v>2</v>
@@ -1924,10 +1956,10 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1936,7 +1968,10 @@
         <v>0.1</v>
       </c>
       <c r="M30">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1953,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1965,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J31" t="s">
         <v>10</v>
@@ -1977,7 +2012,7 @@
         <v>0.1</v>
       </c>
       <c r="M31">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1985,7 +2020,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1997,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" s="2">
         <v>3</v>
@@ -2006,10 +2041,10 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2018,10 +2053,7 @@
         <v>0.1</v>
       </c>
       <c r="M32">
-        <v>60</v>
-      </c>
-      <c r="N32" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2029,7 +2061,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2038,10 +2070,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="2">
         <v>3</v>
@@ -2050,10 +2082,10 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -2062,10 +2094,7 @@
         <v>0.1</v>
       </c>
       <c r="M33">
-        <v>20</v>
-      </c>
-      <c r="N33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2073,7 +2102,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2082,10 +2111,10 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="2">
         <v>3</v>
@@ -2094,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -2106,10 +2135,7 @@
         <v>0.1</v>
       </c>
       <c r="M34">
-        <v>60</v>
-      </c>
-      <c r="N34" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2126,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2138,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J35" t="s">
         <v>9</v>
@@ -2150,7 +2176,7 @@
         <v>0.1</v>
       </c>
       <c r="M35">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N35" t="s">
         <v>57</v>
@@ -2161,7 +2187,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2182,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -2194,7 +2220,10 @@
         <v>0.1</v>
       </c>
       <c r="M36">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2202,7 +2231,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2211,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2223,10 +2252,10 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -2235,7 +2264,10 @@
         <v>0.1</v>
       </c>
       <c r="M37">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N37" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2243,7 +2275,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2252,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2264,10 +2296,10 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2276,7 +2308,10 @@
         <v>0.1</v>
       </c>
       <c r="M38">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2293,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -2305,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J39" t="s">
         <v>10</v>
@@ -2317,7 +2352,7 @@
         <v>0.1</v>
       </c>
       <c r="M39">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2337,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2">
         <v>3</v>
@@ -2346,10 +2381,10 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -2358,7 +2393,7 @@
         <v>0.1</v>
       </c>
       <c r="M40">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2375,10 +2410,10 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G41" s="2">
         <v>3</v>
@@ -2387,10 +2422,10 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -2399,7 +2434,7 @@
         <v>0.1</v>
       </c>
       <c r="M41">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2416,10 +2451,10 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2">
         <v>3</v>
@@ -2428,10 +2463,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -2440,7 +2475,7 @@
         <v>0.1</v>
       </c>
       <c r="M42">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2457,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -2469,7 +2504,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J43" t="s">
         <v>9</v>
@@ -2481,7 +2516,7 @@
         <v>0.1</v>
       </c>
       <c r="M43">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2510,10 +2545,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -2522,7 +2557,7 @@
         <v>0.1</v>
       </c>
       <c r="M44">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2539,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F45">
         <v>3</v>
@@ -2551,10 +2586,10 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -2563,7 +2598,7 @@
         <v>0.1</v>
       </c>
       <c r="M45">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2580,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46">
         <v>3</v>
@@ -2592,10 +2627,10 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -2604,7 +2639,7 @@
         <v>0.1</v>
       </c>
       <c r="M46">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2621,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F47">
         <v>3</v>
@@ -2633,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J47" t="s">
         <v>10</v>
@@ -2645,7 +2680,7 @@
         <v>0.1</v>
       </c>
       <c r="M47">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2653,10 +2688,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2665,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G48" s="2">
         <v>3</v>
@@ -2674,10 +2709,10 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -2686,10 +2721,7 @@
         <v>0.1</v>
       </c>
       <c r="M48">
-        <v>60</v>
-      </c>
-      <c r="N48" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2697,19 +2729,19 @@
         <v>47</v>
       </c>
       <c r="B49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49" s="2">
         <v>3</v>
@@ -2718,10 +2750,10 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K49">
         <v>0</v>
@@ -2730,10 +2762,7 @@
         <v>0.1</v>
       </c>
       <c r="M49">
-        <v>20</v>
-      </c>
-      <c r="N49" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2741,19 +2770,19 @@
         <v>48</v>
       </c>
       <c r="B50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G50" s="2">
         <v>3</v>
@@ -2762,10 +2791,10 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -2774,10 +2803,7 @@
         <v>0.1</v>
       </c>
       <c r="M50">
-        <v>60</v>
-      </c>
-      <c r="N50" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2794,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2806,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J51" t="s">
         <v>9</v>
@@ -2818,10 +2844,10 @@
         <v>0.1</v>
       </c>
       <c r="M51">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2829,7 +2855,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2850,10 +2876,10 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -2862,10 +2888,10 @@
         <v>0.1</v>
       </c>
       <c r="M52">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N52" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2873,7 +2899,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2882,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2894,10 +2920,10 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -2906,7 +2932,10 @@
         <v>0.1</v>
       </c>
       <c r="M53">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N53" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2914,7 +2943,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2923,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2935,10 +2964,10 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -2947,7 +2976,10 @@
         <v>0.1</v>
       </c>
       <c r="M54">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="N54" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2964,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2976,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J55" t="s">
         <v>10</v>
@@ -2988,7 +3020,10 @@
         <v>0.1</v>
       </c>
       <c r="M55">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="N55" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -2996,7 +3031,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3011,16 +3046,16 @@
         <v>0</v>
       </c>
       <c r="G56" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -3029,10 +3064,7 @@
         <v>0.1</v>
       </c>
       <c r="M56">
-        <v>60</v>
-      </c>
-      <c r="N56" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3040,7 +3072,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3049,22 +3081,22 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -3073,10 +3105,7 @@
         <v>0.1</v>
       </c>
       <c r="M57">
-        <v>20</v>
-      </c>
-      <c r="N57" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3084,31 +3113,31 @@
         <v>56</v>
       </c>
       <c r="B58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="G58" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -3117,10 +3146,7 @@
         <v>0.1</v>
       </c>
       <c r="M58">
-        <v>60</v>
-      </c>
-      <c r="N58" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3131,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -3149,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J59" t="s">
         <v>9</v>
@@ -3161,10 +3187,10 @@
         <v>0.1</v>
       </c>
       <c r="M59">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3190,10 +3216,10 @@
         <v>4</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J60" t="s">
         <v>9</v>
@@ -3205,10 +3231,10 @@
         <v>0.1</v>
       </c>
       <c r="M60">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3219,7 +3245,7 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3234,10 +3260,10 @@
         <v>4</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J61" t="s">
         <v>9</v>
@@ -3249,7 +3275,7 @@
         <v>0.1</v>
       </c>
       <c r="M61">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N61" t="s">
         <v>8</v>
@@ -3263,7 +3289,7 @@
         <v>1</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -3275,13 +3301,13 @@
         <v>0</v>
       </c>
       <c r="G62" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J62" t="s">
         <v>9</v>
@@ -3290,13 +3316,13 @@
         <v>0</v>
       </c>
       <c r="L62">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M62">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N62" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3319,13 +3345,13 @@
         <v>0</v>
       </c>
       <c r="G63" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J63" t="s">
         <v>9</v>
@@ -3334,13 +3360,13 @@
         <v>0</v>
       </c>
       <c r="L63">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M63">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N63" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3351,7 +3377,7 @@
         <v>1</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3363,13 +3389,13 @@
         <v>0</v>
       </c>
       <c r="G64" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H64">
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J64" t="s">
         <v>9</v>
@@ -3378,13 +3404,13 @@
         <v>0</v>
       </c>
       <c r="L64">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M64">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N64" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3395,7 +3421,7 @@
         <v>1</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -3413,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J65" t="s">
         <v>9</v>
@@ -3425,10 +3451,10 @@
         <v>1</v>
       </c>
       <c r="M65">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="N65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3439,13 +3465,13 @@
         <v>1</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -3457,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J66" t="s">
         <v>9</v>
@@ -3469,10 +3495,10 @@
         <v>1</v>
       </c>
       <c r="M66">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="N66" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -3489,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -3501,22 +3527,154 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" t="s">
+        <v>9</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <v>60</v>
+      </c>
+      <c r="N67" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="b">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" s="2">
+        <v>2</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
         <v>42</v>
       </c>
-      <c r="J67" t="s">
-        <v>9</v>
-      </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="L67">
-        <v>1</v>
-      </c>
-      <c r="M67">
+      <c r="J68" t="s">
+        <v>9</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
         <v>20</v>
       </c>
-      <c r="N67" t="s">
-        <v>48</v>
+      <c r="N68" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69" s="2">
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" t="s">
+        <v>9</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69">
+        <v>60</v>
+      </c>
+      <c r="N69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="b">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" s="2">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>42</v>
+      </c>
+      <c r="J70" t="s">
+        <v>9</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <v>20</v>
+      </c>
+      <c r="N70" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3524,19 +3682,19 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="K1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B50:M51 O50:XFD51 A68:XFD1048576 A3:XFD13 B14:XFD49 B52:XFD67 A14:A67">
+  <conditionalFormatting sqref="B53:M54 O53:XFD54 B55:XFD70 A71:XFD1048576 A3:XFD6 B7:XFD52 A7:A70">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N51">
+  <conditionalFormatting sqref="N54">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$B50</formula>
+      <formula>$B53</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N53">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$B50</formula>
+      <formula>$B53</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completing bug fix from last commit... AND Adding validation by simulating XS7 evolution using calibrated bank erosion coefficient.
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@158 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="79">
   <si>
     <t>Stencil</t>
   </si>
@@ -267,6 +267,21 @@
   </si>
   <si>
     <t>9 but 0.1m res</t>
+  </si>
+  <si>
+    <t>Validation simulation</t>
+  </si>
+  <si>
+    <t>Vgeometry</t>
+  </si>
+  <si>
+    <t>Vradius</t>
+  </si>
+  <si>
+    <t>Inputs\Selwyn_XS7_3m.csv</t>
+  </si>
+  <si>
+    <t>Inputs\Selwyn_XS7_1m.csv</t>
   </si>
 </sst>
 </file>
@@ -317,10 +332,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -337,21 +355,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -663,11 +667,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A70"/>
+      <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,18 +682,20 @@
     <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="9.5703125" customWidth="1"/>
-    <col min="14" max="14" width="61" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="C1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="6"/>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7"/>
       <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
@@ -702,15 +708,19 @@
       <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="6"/>
+      <c r="L1" s="7"/>
       <c r="M1" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -750,11 +760,17 @@
       <c r="M2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -795,10 +811,16 @@
         <v>60</v>
       </c>
       <c r="N3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3">
+        <v>-160</v>
+      </c>
+      <c r="P3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -839,10 +861,16 @@
         <v>20</v>
       </c>
       <c r="N4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4">
+        <v>-160</v>
+      </c>
+      <c r="P4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -880,13 +908,19 @@
         <v>2</v>
       </c>
       <c r="M5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5">
+        <v>-160</v>
+      </c>
+      <c r="P5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -927,10 +961,16 @@
         <v>20</v>
       </c>
       <c r="N6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6">
+        <v>-160</v>
+      </c>
+      <c r="P6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -970,11 +1010,11 @@
       <c r="M7">
         <v>5</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1012,13 +1052,13 @@
         <v>2</v>
       </c>
       <c r="M8">
-        <v>5</v>
-      </c>
-      <c r="N8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1059,10 +1099,16 @@
         <v>60</v>
       </c>
       <c r="N9" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9">
+        <v>-160</v>
+      </c>
+      <c r="P9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1103,10 +1149,16 @@
         <v>20</v>
       </c>
       <c r="N10" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10">
+        <v>-160</v>
+      </c>
+      <c r="P10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1147,10 +1199,16 @@
         <v>60</v>
       </c>
       <c r="N11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11">
+        <v>-160</v>
+      </c>
+      <c r="P11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1191,10 +1249,16 @@
         <v>20</v>
       </c>
       <c r="N12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O12">
+        <v>-160</v>
+      </c>
+      <c r="P12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1235,10 +1299,16 @@
         <v>60</v>
       </c>
       <c r="N13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13">
+        <v>-160</v>
+      </c>
+      <c r="P13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1279,10 +1349,16 @@
         <v>20</v>
       </c>
       <c r="N14" t="s">
+        <v>78</v>
+      </c>
+      <c r="O14">
+        <v>-160</v>
+      </c>
+      <c r="P14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1322,11 +1398,11 @@
       <c r="M15">
         <v>5</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1364,13 +1440,13 @@
         <v>0.1</v>
       </c>
       <c r="M16">
-        <v>5</v>
-      </c>
-      <c r="N16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1411,10 +1487,16 @@
         <v>60</v>
       </c>
       <c r="N17" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17">
+        <v>-160</v>
+      </c>
+      <c r="P17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1455,10 +1537,16 @@
         <v>20</v>
       </c>
       <c r="N18" t="s">
+        <v>78</v>
+      </c>
+      <c r="O18">
+        <v>-160</v>
+      </c>
+      <c r="P18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1499,10 +1587,16 @@
         <v>60</v>
       </c>
       <c r="N19" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19">
+        <v>-160</v>
+      </c>
+      <c r="P19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1543,10 +1637,16 @@
         <v>20</v>
       </c>
       <c r="N20" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20">
+        <v>-160</v>
+      </c>
+      <c r="P20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1587,10 +1687,16 @@
         <v>60</v>
       </c>
       <c r="N21" t="s">
+        <v>77</v>
+      </c>
+      <c r="O21">
+        <v>-160</v>
+      </c>
+      <c r="P21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1631,10 +1737,16 @@
         <v>20</v>
       </c>
       <c r="N22" t="s">
+        <v>78</v>
+      </c>
+      <c r="O22">
+        <v>-160</v>
+      </c>
+      <c r="P22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1674,8 +1786,14 @@
       <c r="M23">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>77</v>
+      </c>
+      <c r="O23">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1715,8 +1833,14 @@
       <c r="M24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>78</v>
+      </c>
+      <c r="O24">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1756,8 +1880,14 @@
       <c r="M25">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>77</v>
+      </c>
+      <c r="O25">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1797,8 +1927,14 @@
       <c r="M26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>78</v>
+      </c>
+      <c r="O26">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1839,10 +1975,16 @@
         <v>60</v>
       </c>
       <c r="N27" t="s">
+        <v>77</v>
+      </c>
+      <c r="O27">
+        <v>-160</v>
+      </c>
+      <c r="P27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1883,10 +2025,16 @@
         <v>20</v>
       </c>
       <c r="N28" t="s">
+        <v>78</v>
+      </c>
+      <c r="O28">
+        <v>-160</v>
+      </c>
+      <c r="P28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1927,10 +2075,16 @@
         <v>60</v>
       </c>
       <c r="N29" t="s">
+        <v>77</v>
+      </c>
+      <c r="O29">
+        <v>-160</v>
+      </c>
+      <c r="P29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1971,10 +2125,16 @@
         <v>20</v>
       </c>
       <c r="N30" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30">
+        <v>-160</v>
+      </c>
+      <c r="P30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2014,8 +2174,14 @@
       <c r="M31">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O31">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2055,8 +2221,14 @@
       <c r="M32">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>78</v>
+      </c>
+      <c r="O32">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2096,8 +2268,14 @@
       <c r="M33">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>77</v>
+      </c>
+      <c r="O33">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2137,8 +2315,14 @@
       <c r="M34">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>78</v>
+      </c>
+      <c r="O34">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2179,10 +2363,16 @@
         <v>60</v>
       </c>
       <c r="N35" t="s">
+        <v>77</v>
+      </c>
+      <c r="O35">
+        <v>-160</v>
+      </c>
+      <c r="P35" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2223,10 +2413,16 @@
         <v>20</v>
       </c>
       <c r="N36" t="s">
+        <v>78</v>
+      </c>
+      <c r="O36">
+        <v>-160</v>
+      </c>
+      <c r="P36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2267,10 +2463,16 @@
         <v>60</v>
       </c>
       <c r="N37" t="s">
+        <v>77</v>
+      </c>
+      <c r="O37">
+        <v>-160</v>
+      </c>
+      <c r="P37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2311,10 +2513,16 @@
         <v>20</v>
       </c>
       <c r="N38" t="s">
+        <v>78</v>
+      </c>
+      <c r="O38">
+        <v>-160</v>
+      </c>
+      <c r="P38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2354,8 +2562,14 @@
       <c r="M39">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>77</v>
+      </c>
+      <c r="O39">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2395,8 +2609,14 @@
       <c r="M40">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>78</v>
+      </c>
+      <c r="O40">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2436,8 +2656,14 @@
       <c r="M41">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>77</v>
+      </c>
+      <c r="O41">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2477,8 +2703,14 @@
       <c r="M42">
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>78</v>
+      </c>
+      <c r="O42">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2518,8 +2750,14 @@
       <c r="M43">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>77</v>
+      </c>
+      <c r="O43">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2559,8 +2797,14 @@
       <c r="M44">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>78</v>
+      </c>
+      <c r="O44">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2600,8 +2844,14 @@
       <c r="M45">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>77</v>
+      </c>
+      <c r="O45">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2641,8 +2891,14 @@
       <c r="M46">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>78</v>
+      </c>
+      <c r="O46">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2682,8 +2938,14 @@
       <c r="M47">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>77</v>
+      </c>
+      <c r="O47">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2723,8 +2985,14 @@
       <c r="M48">
         <v>20</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>78</v>
+      </c>
+      <c r="O48">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2764,8 +3032,14 @@
       <c r="M49">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>77</v>
+      </c>
+      <c r="O49">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2805,8 +3079,14 @@
       <c r="M50">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>78</v>
+      </c>
+      <c r="O50">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2847,10 +3127,16 @@
         <v>60</v>
       </c>
       <c r="N51" t="s">
+        <v>77</v>
+      </c>
+      <c r="O51">
+        <v>-160</v>
+      </c>
+      <c r="P51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2891,10 +3177,16 @@
         <v>20</v>
       </c>
       <c r="N52" t="s">
+        <v>78</v>
+      </c>
+      <c r="O52">
+        <v>-160</v>
+      </c>
+      <c r="P52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2935,10 +3227,16 @@
         <v>60</v>
       </c>
       <c r="N53" t="s">
+        <v>77</v>
+      </c>
+      <c r="O53">
+        <v>-160</v>
+      </c>
+      <c r="P53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2979,10 +3277,16 @@
         <v>20</v>
       </c>
       <c r="N54" t="s">
+        <v>78</v>
+      </c>
+      <c r="O54">
+        <v>-160</v>
+      </c>
+      <c r="P54" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3023,10 +3327,16 @@
         <v>60</v>
       </c>
       <c r="N55" t="s">
+        <v>77</v>
+      </c>
+      <c r="O55">
+        <v>-160</v>
+      </c>
+      <c r="P55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3066,8 +3376,14 @@
       <c r="M56">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N56" t="s">
+        <v>78</v>
+      </c>
+      <c r="O56">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3107,8 +3423,14 @@
       <c r="M57">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N57" t="s">
+        <v>77</v>
+      </c>
+      <c r="O57">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3148,8 +3470,14 @@
       <c r="M58">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N58" t="s">
+        <v>78</v>
+      </c>
+      <c r="O58">
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3190,10 +3518,16 @@
         <v>60</v>
       </c>
       <c r="N59" t="s">
+        <v>77</v>
+      </c>
+      <c r="O59">
+        <v>-160</v>
+      </c>
+      <c r="P59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3234,10 +3568,16 @@
         <v>20</v>
       </c>
       <c r="N60" t="s">
+        <v>78</v>
+      </c>
+      <c r="O60">
+        <v>-160</v>
+      </c>
+      <c r="P60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3278,10 +3618,16 @@
         <v>60</v>
       </c>
       <c r="N61" t="s">
+        <v>77</v>
+      </c>
+      <c r="O61">
+        <v>-160</v>
+      </c>
+      <c r="P61" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3322,10 +3668,16 @@
         <v>20</v>
       </c>
       <c r="N62" t="s">
+        <v>78</v>
+      </c>
+      <c r="O62">
+        <v>-160</v>
+      </c>
+      <c r="P62" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3366,10 +3718,16 @@
         <v>60</v>
       </c>
       <c r="N63" t="s">
+        <v>77</v>
+      </c>
+      <c r="O63">
+        <v>-160</v>
+      </c>
+      <c r="P63" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3410,10 +3768,16 @@
         <v>20</v>
       </c>
       <c r="N64" t="s">
+        <v>78</v>
+      </c>
+      <c r="O64">
+        <v>-160</v>
+      </c>
+      <c r="P64" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3454,10 +3818,16 @@
         <v>60</v>
       </c>
       <c r="N65" t="s">
+        <v>77</v>
+      </c>
+      <c r="O65">
+        <v>-160</v>
+      </c>
+      <c r="P65" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3498,10 +3868,16 @@
         <v>20</v>
       </c>
       <c r="N66" t="s">
+        <v>78</v>
+      </c>
+      <c r="O66">
+        <v>-160</v>
+      </c>
+      <c r="P66" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3542,10 +3918,16 @@
         <v>60</v>
       </c>
       <c r="N67" t="s">
+        <v>77</v>
+      </c>
+      <c r="O67">
+        <v>-160</v>
+      </c>
+      <c r="P67" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3586,10 +3968,16 @@
         <v>20</v>
       </c>
       <c r="N68" t="s">
+        <v>78</v>
+      </c>
+      <c r="O68">
+        <v>-160</v>
+      </c>
+      <c r="P68" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3630,10 +4018,16 @@
         <v>60</v>
       </c>
       <c r="N69" t="s">
+        <v>77</v>
+      </c>
+      <c r="O69">
+        <v>-160</v>
+      </c>
+      <c r="P69" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3674,27 +4068,44 @@
         <v>20</v>
       </c>
       <c r="N70" t="s">
+        <v>78</v>
+      </c>
+      <c r="O70">
+        <v>-160</v>
+      </c>
+      <c r="P70" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B53:M54 O53:XFD54 B55:XFD70 A71:XFD1048576 A3:XFD6 B7:XFD52 A7:A70">
-    <cfRule type="expression" dxfId="4" priority="2">
+  <conditionalFormatting sqref="Q53:XFD54 A71:XFD1048576 A3:M70 P55:XFD70 O3:XFD16 P17:XFD52">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N54">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="P54">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$B53</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N53">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="P53">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B53</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N70">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:O70">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B17</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fix and reduced optimisation range for 6m res slope model to ensure that it converges
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@199 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Research\BankErosionMatlab\Trunk\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BankErosion\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -446,12 +446,6 @@
     <t>2d</t>
   </si>
   <si>
-    <t>Inputs\Selwyn_XS7_7m.csv</t>
-  </si>
-  <si>
-    <t>Inputs\Selwyn_XS3_7m.csv</t>
-  </si>
-  <si>
     <t>UpwindBedload</t>
   </si>
   <si>
@@ -516,6 +510,12 @@
   </si>
   <si>
     <t>18e</t>
+  </si>
+  <si>
+    <t>Inputs\Selwyn_XS3_6m.csv</t>
+  </si>
+  <si>
+    <t>Inputs\Selwyn_XS7_6m.csv</t>
   </si>
 </sst>
 </file>
@@ -1051,6 +1051,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1063,272 +1065,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1625,7 +1366,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,10 +1390,10 @@
       <c r="C1" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="52"/>
+      <c r="D1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="54"/>
       <c r="F1" s="26" t="s">
         <v>24</v>
       </c>
@@ -1667,17 +1408,17 @@
         <v>3</v>
       </c>
       <c r="K1" s="46"/>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="53"/>
+      <c r="M1" s="55"/>
       <c r="N1" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="54" t="s">
+      <c r="O1" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="55"/>
+      <c r="P1" s="57"/>
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1706,7 +1447,7 @@
         <v>29</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J2" s="47" t="s">
         <v>31</v>
@@ -1762,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K3" s="48" t="s">
         <v>8</v>
@@ -1771,13 +1512,13 @@
         <v>0.1</v>
       </c>
       <c r="M3" s="7">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="N3" s="48">
         <v>120</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P3" s="8">
         <v>-160</v>
@@ -1839,7 +1580,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" s="48" t="b">
         <v>1</v>
@@ -2037,7 +1778,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" s="48" t="b">
         <v>1</v>
@@ -2090,7 +1831,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B10" s="50" t="b">
         <v>1</v>
@@ -2138,10 +1879,10 @@
         <v>-160</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="56" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>63</v>
       </c>
@@ -2170,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K11" s="49" t="s">
         <v>8</v>
@@ -2185,7 +1926,7 @@
         <v>60</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P11" s="17">
         <v>-160</v>
@@ -2345,7 +2086,7 @@
     </row>
     <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="50" t="b">
         <v>1</v>
@@ -2362,7 +2103,7 @@
       <c r="F15" s="38">
         <v>0</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="53">
         <v>3</v>
       </c>
       <c r="H15" s="39">
@@ -2419,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K16" s="49" t="s">
         <v>8</v>
@@ -2434,7 +2175,7 @@
         <v>60</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P16" s="17">
         <v>-160</v>
@@ -2594,7 +2335,7 @@
     </row>
     <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B20" s="50" t="b">
         <v>1</v>
@@ -2611,7 +2352,7 @@
       <c r="F20" s="38">
         <v>0</v>
       </c>
-      <c r="G20" s="57">
+      <c r="G20" s="53">
         <v>3</v>
       </c>
       <c r="H20" s="39">
@@ -2668,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K21" s="49" t="s">
         <v>8</v>
@@ -2683,7 +2424,7 @@
         <v>60</v>
       </c>
       <c r="O21" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P21" s="17">
         <v>-160</v>
@@ -2843,7 +2584,7 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B25" s="50" t="b">
         <v>1</v>
@@ -2860,7 +2601,7 @@
       <c r="F25" s="38">
         <v>0</v>
       </c>
-      <c r="G25" s="57">
+      <c r="G25" s="53">
         <v>3</v>
       </c>
       <c r="H25" s="39">
@@ -2917,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K26" s="49" t="s">
         <v>8</v>
@@ -2932,7 +2673,7 @@
         <v>60</v>
       </c>
       <c r="O26" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P26" s="17">
         <v>-160</v>
@@ -3092,7 +2833,7 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B30" s="50" t="b">
         <v>1</v>
@@ -3109,7 +2850,7 @@
       <c r="F30" s="38">
         <v>0</v>
       </c>
-      <c r="G30" s="57">
+      <c r="G30" s="53">
         <v>3</v>
       </c>
       <c r="H30" s="39">
@@ -3166,7 +2907,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K31" s="49" t="s">
         <v>8</v>
@@ -3181,7 +2922,7 @@
         <v>60</v>
       </c>
       <c r="O31" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P31" s="17">
         <v>-160</v>
@@ -3341,7 +3082,7 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35" s="50" t="b">
         <v>1</v>
@@ -3358,7 +3099,7 @@
       <c r="F35" s="38">
         <v>0</v>
       </c>
-      <c r="G35" s="57">
+      <c r="G35" s="53">
         <v>3</v>
       </c>
       <c r="H35" s="39">
@@ -3415,7 +3156,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K36" s="49" t="s">
         <v>8</v>
@@ -3430,7 +3171,7 @@
         <v>60</v>
       </c>
       <c r="O36" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P36" s="17">
         <v>-160</v>
@@ -3590,7 +3331,7 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B40" s="50" t="b">
         <v>1</v>
@@ -3607,7 +3348,7 @@
       <c r="F40" s="38">
         <v>0</v>
       </c>
-      <c r="G40" s="57">
+      <c r="G40" s="53">
         <v>3</v>
       </c>
       <c r="H40" s="39">
@@ -3664,7 +3405,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K41" s="49" t="s">
         <v>8</v>
@@ -3679,7 +3420,7 @@
         <v>60</v>
       </c>
       <c r="O41" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P41" s="17">
         <v>-160</v>
@@ -3839,7 +3580,7 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B45" s="50" t="b">
         <v>1</v>
@@ -3856,7 +3597,7 @@
       <c r="F45" s="38">
         <v>0</v>
       </c>
-      <c r="G45" s="57">
+      <c r="G45" s="53">
         <v>3</v>
       </c>
       <c r="H45" s="39">
@@ -3913,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K46" s="49" t="s">
         <v>8</v>
@@ -3928,7 +3669,7 @@
         <v>60</v>
       </c>
       <c r="O46" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P46" s="17">
         <v>-160</v>
@@ -4088,7 +3829,7 @@
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B50" s="50" t="b">
         <v>1</v>
@@ -4105,7 +3846,7 @@
       <c r="F50" s="38">
         <v>2</v>
       </c>
-      <c r="G50" s="57">
+      <c r="G50" s="53">
         <v>3</v>
       </c>
       <c r="H50" s="39">
@@ -4162,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K51" s="49" t="s">
         <v>8</v>
@@ -4177,7 +3918,7 @@
         <v>60</v>
       </c>
       <c r="O51" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P51" s="17">
         <v>-160</v>
@@ -4337,7 +4078,7 @@
     </row>
     <row r="55" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B55" s="50" t="b">
         <v>1</v>
@@ -4354,7 +4095,7 @@
       <c r="F55" s="38">
         <v>2</v>
       </c>
-      <c r="G55" s="57">
+      <c r="G55" s="53">
         <v>3</v>
       </c>
       <c r="H55" s="39">
@@ -4411,7 +4152,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K56" s="49" t="s">
         <v>8</v>
@@ -4426,7 +4167,7 @@
         <v>60</v>
       </c>
       <c r="O56" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P56" s="17">
         <v>-160</v>
@@ -4586,7 +4327,7 @@
     </row>
     <row r="60" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B60" s="50" t="b">
         <v>1</v>
@@ -4603,7 +4344,7 @@
       <c r="F60" s="38">
         <v>1</v>
       </c>
-      <c r="G60" s="57">
+      <c r="G60" s="53">
         <v>3</v>
       </c>
       <c r="H60" s="39">
@@ -4660,7 +4401,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K61" s="49" t="s">
         <v>8</v>
@@ -4675,7 +4416,7 @@
         <v>60</v>
       </c>
       <c r="O61" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P61" s="17">
         <v>-160</v>
@@ -4835,7 +4576,7 @@
     </row>
     <row r="65" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B65" s="50" t="b">
         <v>1</v>
@@ -4852,7 +4593,7 @@
       <c r="F65" s="38">
         <v>1</v>
       </c>
-      <c r="G65" s="57">
+      <c r="G65" s="53">
         <v>3</v>
       </c>
       <c r="H65" s="39">
@@ -4909,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K66" s="49" t="s">
         <v>8</v>
@@ -4924,7 +4665,7 @@
         <v>60</v>
       </c>
       <c r="O66" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P66" s="17">
         <v>-160</v>
@@ -5084,7 +4825,7 @@
     </row>
     <row r="70" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B70" s="50" t="b">
         <v>1</v>
@@ -5101,7 +4842,7 @@
       <c r="F70" s="38">
         <v>0</v>
       </c>
-      <c r="G70" s="57">
+      <c r="G70" s="53">
         <v>4</v>
       </c>
       <c r="H70" s="39">
@@ -5158,7 +4899,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K71" s="49" t="s">
         <v>8</v>
@@ -5173,7 +4914,7 @@
         <v>60</v>
       </c>
       <c r="O71" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P71" s="17">
         <v>-160</v>
@@ -5333,7 +5074,7 @@
     </row>
     <row r="75" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B75" s="50" t="b">
         <v>1</v>
@@ -5350,7 +5091,7 @@
       <c r="F75" s="38">
         <v>0</v>
       </c>
-      <c r="G75" s="57">
+      <c r="G75" s="53">
         <v>4</v>
       </c>
       <c r="H75" s="39">
@@ -5407,7 +5148,7 @@
         <v>1</v>
       </c>
       <c r="J76" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K76" s="49" t="s">
         <v>8</v>
@@ -5422,7 +5163,7 @@
         <v>60</v>
       </c>
       <c r="O76" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P76" s="17">
         <v>-160</v>
@@ -5582,7 +5323,7 @@
     </row>
     <row r="80" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B80" s="50" t="b">
         <v>1</v>
@@ -5599,7 +5340,7 @@
       <c r="F80" s="38">
         <v>0</v>
       </c>
-      <c r="G80" s="57">
+      <c r="G80" s="53">
         <v>4</v>
       </c>
       <c r="H80" s="39">
@@ -5656,7 +5397,7 @@
         <v>1</v>
       </c>
       <c r="J81" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K81" s="49" t="s">
         <v>8</v>
@@ -5671,7 +5412,7 @@
         <v>60</v>
       </c>
       <c r="O81" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P81" s="17">
         <v>-160</v>
@@ -5831,7 +5572,7 @@
     </row>
     <row r="85" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B85" s="50" t="b">
         <v>1</v>
@@ -5848,7 +5589,7 @@
       <c r="F85" s="38">
         <v>0</v>
       </c>
-      <c r="G85" s="57">
+      <c r="G85" s="53">
         <v>2</v>
       </c>
       <c r="H85" s="39">
@@ -5905,7 +5646,7 @@
         <v>1</v>
       </c>
       <c r="J86" s="49" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K86" s="49" t="s">
         <v>8</v>
@@ -5920,7 +5661,7 @@
         <v>60</v>
       </c>
       <c r="O86" s="22" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P86" s="17">
         <v>-160</v>
@@ -6080,7 +5821,7 @@
     </row>
     <row r="90" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B90" s="50" t="b">
         <v>1</v>
@@ -6097,7 +5838,7 @@
       <c r="F90" s="38">
         <v>0</v>
       </c>
-      <c r="G90" s="57">
+      <c r="G90" s="53">
         <v>2</v>
       </c>
       <c r="H90" s="39">
@@ -6154,7 +5895,7 @@
         <v>1</v>
       </c>
       <c r="J91" s="48" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="K91" s="48" t="s">
         <v>8</v>
@@ -6169,7 +5910,7 @@
         <v>60</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="P91" s="8">
         <v>-160</v>
@@ -6329,7 +6070,7 @@
     </row>
     <row r="95" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B95" s="51" t="b">
         <v>1</v>
@@ -6389,7 +6130,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:Q3">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Modifying scenario setup (including corrections to calibration coefficient ranges and adjustments to ranges to improve calibration performance)
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@203 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BankErosion\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Research\BankErosionMatlab\Trunk\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="157">
   <si>
     <t>Stencil</t>
   </si>
@@ -209,21 +209,6 @@
     <t>Inputs\Selwyn_XS7_1m.csv</t>
   </si>
   <si>
-    <t>11 + stencil</t>
-  </si>
-  <si>
-    <t>19 + degrading toe trigger</t>
-  </si>
-  <si>
-    <t>19 + stencil + trigger</t>
-  </si>
-  <si>
-    <t>19 + threshold height trigger</t>
-  </si>
-  <si>
-    <t>31 + stencil</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
@@ -359,9 +344,6 @@
     <t>18b</t>
   </si>
   <si>
-    <t>19 + stencil</t>
-  </si>
-  <si>
     <t>17c</t>
   </si>
   <si>
@@ -516,6 +498,24 @@
   </si>
   <si>
     <t>Inputs\Selwyn_XS7_6m.csv</t>
+  </si>
+  <si>
+    <t>3 + stencil</t>
+  </si>
+  <si>
+    <t>5 + stencil</t>
+  </si>
+  <si>
+    <t>7 + stencil</t>
+  </si>
+  <si>
+    <t>7 + degrading toe trigger</t>
+  </si>
+  <si>
+    <t>7 + stencil + trigger</t>
+  </si>
+  <si>
+    <t>7 + threshold height trigger</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1069,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1366,7 +1373,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1454,7 @@
         <v>29</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J2" s="47" t="s">
         <v>31</v>
@@ -1476,7 +1483,7 @@
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B3" s="48" t="b">
         <v>1</v>
@@ -1503,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K3" s="48" t="s">
         <v>8</v>
@@ -1518,7 +1525,7 @@
         <v>120</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P3" s="8">
         <v>-160</v>
@@ -1529,7 +1536,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B4" s="48" t="b">
         <v>1</v>
@@ -1580,7 +1587,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B5" s="48" t="b">
         <v>1</v>
@@ -1631,7 +1638,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B6" s="48" t="b">
         <v>1</v>
@@ -1667,7 +1674,7 @@
         <v>0.1</v>
       </c>
       <c r="M6" s="7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N6" s="48">
         <v>5</v>
@@ -1678,7 +1685,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B7" s="48" t="b">
         <v>1</v>
@@ -1714,7 +1721,7 @@
         <v>0.1</v>
       </c>
       <c r="M7" s="7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N7" s="48">
         <v>2</v>
@@ -1725,7 +1732,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B8" s="48" t="b">
         <v>1</v>
@@ -1766,9 +1773,7 @@
       <c r="N8" s="48">
         <v>20</v>
       </c>
-      <c r="O8" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="O8" s="21"/>
       <c r="P8" s="8">
         <v>-160</v>
       </c>
@@ -1778,7 +1783,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B9" s="48" t="b">
         <v>1</v>
@@ -1819,9 +1824,7 @@
       <c r="N9" s="48">
         <v>5</v>
       </c>
-      <c r="O9" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="O9" s="21"/>
       <c r="P9" s="8">
         <v>-160</v>
       </c>
@@ -1831,7 +1834,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B10" s="50" t="b">
         <v>1</v>
@@ -1857,8 +1860,8 @@
       <c r="I10" s="50">
         <v>0.5</v>
       </c>
-      <c r="J10" s="50" t="s">
-        <v>40</v>
+      <c r="J10" s="48" t="s">
+        <v>33</v>
       </c>
       <c r="K10" s="50" t="s">
         <v>8</v>
@@ -1870,21 +1873,19 @@
         <v>2</v>
       </c>
       <c r="N10" s="50">
-        <v>20</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>53</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="O10" s="23"/>
       <c r="P10" s="20">
         <v>-160</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B11" s="49" t="b">
         <v>1</v>
@@ -1911,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K11" s="49" t="s">
         <v>8</v>
@@ -1926,7 +1927,7 @@
         <v>60</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P11" s="17">
         <v>-160</v>
@@ -1937,7 +1938,7 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B12" s="48" t="b">
         <v>1</v>
@@ -1988,7 +1989,7 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B13" s="48" t="b">
         <v>1</v>
@@ -2039,7 +2040,7 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B14" s="48" t="b">
         <v>1</v>
@@ -2072,10 +2073,10 @@
         <v>8</v>
       </c>
       <c r="L14" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="7">
-        <v>2</v>
+        <v>0.01</v>
       </c>
       <c r="N14" s="48">
         <v>5</v>
@@ -2086,7 +2087,7 @@
     </row>
     <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B15" s="50" t="b">
         <v>1</v>
@@ -2118,14 +2119,14 @@
       <c r="K15" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M15" s="19">
-        <v>2</v>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0.01</v>
       </c>
       <c r="N15" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15" s="23"/>
       <c r="P15" s="20"/>
@@ -2133,7 +2134,7 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16" s="49" t="b">
         <v>1</v>
@@ -2160,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K16" s="49" t="s">
         <v>8</v>
@@ -2175,7 +2176,7 @@
         <v>60</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P16" s="17">
         <v>-160</v>
@@ -2186,7 +2187,7 @@
     </row>
     <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17" s="48" t="b">
         <v>1</v>
@@ -2237,7 +2238,7 @@
     </row>
     <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B18" s="48" t="b">
         <v>1</v>
@@ -2288,7 +2289,7 @@
     </row>
     <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B19" s="48" t="b">
         <v>1</v>
@@ -2324,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="7">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="N19" s="48">
         <v>5</v>
@@ -2335,7 +2336,7 @@
     </row>
     <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B20" s="50" t="b">
         <v>1</v>
@@ -2371,10 +2372,10 @@
         <v>0</v>
       </c>
       <c r="M20" s="19">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="N20" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O20" s="23"/>
       <c r="P20" s="20"/>
@@ -2382,7 +2383,7 @@
     </row>
     <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B21" s="49" t="b">
         <v>1</v>
@@ -2409,7 +2410,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K21" s="49" t="s">
         <v>8</v>
@@ -2424,18 +2425,18 @@
         <v>60</v>
       </c>
       <c r="O21" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P21" s="17">
         <v>-160</v>
       </c>
       <c r="Q21" s="49" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B22" s="48" t="b">
         <v>1</v>
@@ -2486,7 +2487,7 @@
     </row>
     <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B23" s="48" t="b">
         <v>1</v>
@@ -2537,7 +2538,7 @@
     </row>
     <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B24" s="48" t="b">
         <v>1</v>
@@ -2573,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="7">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="N24" s="48">
         <v>5</v>
@@ -2584,7 +2585,7 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B25" s="50" t="b">
         <v>1</v>
@@ -2620,10 +2621,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="19">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="N25" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O25" s="23"/>
       <c r="P25" s="20"/>
@@ -2631,7 +2632,7 @@
     </row>
     <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B26" s="49" t="b">
         <v>1</v>
@@ -2658,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K26" s="49" t="s">
         <v>8</v>
@@ -2673,7 +2674,7 @@
         <v>60</v>
       </c>
       <c r="O26" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P26" s="17">
         <v>-160</v>
@@ -2684,7 +2685,7 @@
     </row>
     <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B27" s="48" t="b">
         <v>1</v>
@@ -2735,7 +2736,7 @@
     </row>
     <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B28" s="48" t="b">
         <v>1</v>
@@ -2786,7 +2787,7 @@
     </row>
     <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B29" s="48" t="b">
         <v>1</v>
@@ -2819,10 +2820,10 @@
         <v>8</v>
       </c>
       <c r="L29" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N29" s="48">
         <v>5</v>
@@ -2833,7 +2834,7 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B30" s="50" t="b">
         <v>1</v>
@@ -2865,11 +2866,11 @@
       <c r="K30" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M30" s="19">
-        <v>2</v>
+      <c r="L30" s="7">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7">
+        <v>0.1</v>
       </c>
       <c r="N30" s="50">
         <v>2</v>
@@ -2880,7 +2881,7 @@
     </row>
     <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B31" s="49" t="b">
         <v>1</v>
@@ -2907,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K31" s="49" t="s">
         <v>8</v>
@@ -2922,18 +2923,18 @@
         <v>60</v>
       </c>
       <c r="O31" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P31" s="17">
         <v>-160</v>
       </c>
       <c r="Q31" s="49" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B32" s="48" t="b">
         <v>1</v>
@@ -2984,7 +2985,7 @@
     </row>
     <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B33" s="48" t="b">
         <v>1</v>
@@ -3035,7 +3036,7 @@
     </row>
     <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B34" s="48" t="b">
         <v>1</v>
@@ -3068,10 +3069,10 @@
         <v>8</v>
       </c>
       <c r="L34" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N34" s="48">
         <v>5</v>
@@ -3082,7 +3083,7 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B35" s="50" t="b">
         <v>1</v>
@@ -3114,11 +3115,11 @@
       <c r="K35" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L35" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M35" s="19">
-        <v>2</v>
+      <c r="L35" s="7">
+        <v>0</v>
+      </c>
+      <c r="M35" s="7">
+        <v>0.1</v>
       </c>
       <c r="N35" s="50">
         <v>2</v>
@@ -3129,7 +3130,7 @@
     </row>
     <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B36" s="49" t="b">
         <v>1</v>
@@ -3156,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K36" s="49" t="s">
         <v>8</v>
@@ -3171,7 +3172,7 @@
         <v>60</v>
       </c>
       <c r="O36" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P36" s="17">
         <v>-160</v>
@@ -3182,7 +3183,7 @@
     </row>
     <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B37" s="48" t="b">
         <v>1</v>
@@ -3233,7 +3234,7 @@
     </row>
     <row r="38" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B38" s="48" t="b">
         <v>1</v>
@@ -3284,7 +3285,7 @@
     </row>
     <row r="39" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B39" s="48" t="b">
         <v>1</v>
@@ -3317,10 +3318,10 @@
         <v>8</v>
       </c>
       <c r="L39" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N39" s="48">
         <v>5</v>
@@ -3331,7 +3332,7 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B40" s="50" t="b">
         <v>1</v>
@@ -3363,11 +3364,11 @@
       <c r="K40" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M40" s="19">
-        <v>2</v>
+      <c r="L40" s="7">
+        <v>0</v>
+      </c>
+      <c r="M40" s="7">
+        <v>0.1</v>
       </c>
       <c r="N40" s="50">
         <v>2</v>
@@ -3378,7 +3379,7 @@
     </row>
     <row r="41" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B41" s="49" t="b">
         <v>1</v>
@@ -3405,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K41" s="49" t="s">
         <v>8</v>
@@ -3420,18 +3421,18 @@
         <v>60</v>
       </c>
       <c r="O41" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P41" s="17">
         <v>-160</v>
       </c>
       <c r="Q41" s="49" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B42" s="48" t="b">
         <v>1</v>
@@ -3482,7 +3483,7 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B43" s="48" t="b">
         <v>1</v>
@@ -3533,7 +3534,7 @@
     </row>
     <row r="44" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B44" s="48" t="b">
         <v>1</v>
@@ -3566,10 +3567,10 @@
         <v>8</v>
       </c>
       <c r="L44" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N44" s="48">
         <v>5</v>
@@ -3580,7 +3581,7 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B45" s="50" t="b">
         <v>1</v>
@@ -3612,11 +3613,11 @@
       <c r="K45" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L45" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M45" s="19">
-        <v>2</v>
+      <c r="L45" s="7">
+        <v>0</v>
+      </c>
+      <c r="M45" s="7">
+        <v>0.1</v>
       </c>
       <c r="N45" s="50">
         <v>2</v>
@@ -3627,7 +3628,7 @@
     </row>
     <row r="46" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B46" s="49" t="b">
         <v>1</v>
@@ -3654,7 +3655,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K46" s="49" t="s">
         <v>8</v>
@@ -3669,18 +3670,18 @@
         <v>60</v>
       </c>
       <c r="O46" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P46" s="17">
         <v>-160</v>
       </c>
       <c r="Q46" s="49" t="s">
-        <v>55</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B47" s="48" t="b">
         <v>1</v>
@@ -3731,7 +3732,7 @@
     </row>
     <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B48" s="48" t="b">
         <v>1</v>
@@ -3782,7 +3783,7 @@
     </row>
     <row r="49" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B49" s="48" t="b">
         <v>1</v>
@@ -3815,10 +3816,10 @@
         <v>8</v>
       </c>
       <c r="L49" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M49" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N49" s="48">
         <v>5</v>
@@ -3829,7 +3830,7 @@
     </row>
     <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B50" s="50" t="b">
         <v>1</v>
@@ -3861,11 +3862,11 @@
       <c r="K50" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L50" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M50" s="19">
-        <v>2</v>
+      <c r="L50" s="7">
+        <v>0</v>
+      </c>
+      <c r="M50" s="7">
+        <v>0.1</v>
       </c>
       <c r="N50" s="50">
         <v>2</v>
@@ -3876,7 +3877,7 @@
     </row>
     <row r="51" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B51" s="49" t="b">
         <v>1</v>
@@ -3903,7 +3904,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K51" s="49" t="s">
         <v>8</v>
@@ -3918,18 +3919,18 @@
         <v>60</v>
       </c>
       <c r="O51" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P51" s="17">
         <v>-160</v>
       </c>
       <c r="Q51" s="49" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B52" s="48" t="b">
         <v>1</v>
@@ -3980,7 +3981,7 @@
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B53" s="48" t="b">
         <v>1</v>
@@ -4031,7 +4032,7 @@
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B54" s="48" t="b">
         <v>1</v>
@@ -4064,10 +4065,10 @@
         <v>8</v>
       </c>
       <c r="L54" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M54" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N54" s="48">
         <v>5</v>
@@ -4078,7 +4079,7 @@
     </row>
     <row r="55" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B55" s="50" t="b">
         <v>1</v>
@@ -4110,11 +4111,11 @@
       <c r="K55" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L55" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M55" s="19">
-        <v>2</v>
+      <c r="L55" s="7">
+        <v>0</v>
+      </c>
+      <c r="M55" s="7">
+        <v>0.1</v>
       </c>
       <c r="N55" s="50">
         <v>2</v>
@@ -4125,7 +4126,7 @@
     </row>
     <row r="56" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B56" s="49" t="b">
         <v>1</v>
@@ -4152,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K56" s="49" t="s">
         <v>8</v>
@@ -4167,18 +4168,18 @@
         <v>60</v>
       </c>
       <c r="O56" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P56" s="17">
         <v>-160</v>
       </c>
       <c r="Q56" s="49" t="s">
-        <v>57</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B57" s="48" t="b">
         <v>1</v>
@@ -4229,7 +4230,7 @@
     </row>
     <row r="58" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B58" s="48" t="b">
         <v>1</v>
@@ -4280,7 +4281,7 @@
     </row>
     <row r="59" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B59" s="48" t="b">
         <v>1</v>
@@ -4313,10 +4314,10 @@
         <v>8</v>
       </c>
       <c r="L59" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M59" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N59" s="48">
         <v>5</v>
@@ -4327,7 +4328,7 @@
     </row>
     <row r="60" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B60" s="50" t="b">
         <v>1</v>
@@ -4359,11 +4360,11 @@
       <c r="K60" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L60" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M60" s="19">
-        <v>2</v>
+      <c r="L60" s="7">
+        <v>0</v>
+      </c>
+      <c r="M60" s="7">
+        <v>0.1</v>
       </c>
       <c r="N60" s="50">
         <v>2</v>
@@ -4374,7 +4375,7 @@
     </row>
     <row r="61" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B61" s="49" t="b">
         <v>1</v>
@@ -4401,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K61" s="49" t="s">
         <v>8</v>
@@ -4416,18 +4417,18 @@
         <v>60</v>
       </c>
       <c r="O61" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P61" s="17">
         <v>-160</v>
       </c>
       <c r="Q61" s="49" t="s">
-        <v>56</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B62" s="48" t="b">
         <v>1</v>
@@ -4478,7 +4479,7 @@
     </row>
     <row r="63" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B63" s="48" t="b">
         <v>1</v>
@@ -4529,7 +4530,7 @@
     </row>
     <row r="64" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B64" s="48" t="b">
         <v>1</v>
@@ -4562,10 +4563,10 @@
         <v>8</v>
       </c>
       <c r="L64" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M64" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N64" s="48">
         <v>5</v>
@@ -4576,7 +4577,7 @@
     </row>
     <row r="65" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B65" s="50" t="b">
         <v>1</v>
@@ -4608,11 +4609,11 @@
       <c r="K65" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L65" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M65" s="19">
-        <v>2</v>
+      <c r="L65" s="7">
+        <v>0</v>
+      </c>
+      <c r="M65" s="7">
+        <v>0.1</v>
       </c>
       <c r="N65" s="50">
         <v>2</v>
@@ -4623,7 +4624,7 @@
     </row>
     <row r="66" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B66" s="49" t="b">
         <v>1</v>
@@ -4650,7 +4651,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K66" s="49" t="s">
         <v>8</v>
@@ -4665,7 +4666,7 @@
         <v>60</v>
       </c>
       <c r="O66" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P66" s="17">
         <v>-160</v>
@@ -4676,7 +4677,7 @@
     </row>
     <row r="67" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B67" s="48" t="b">
         <v>1</v>
@@ -4727,7 +4728,7 @@
     </row>
     <row r="68" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B68" s="48" t="b">
         <v>1</v>
@@ -4778,7 +4779,7 @@
     </row>
     <row r="69" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B69" s="48" t="b">
         <v>1</v>
@@ -4811,10 +4812,10 @@
         <v>8</v>
       </c>
       <c r="L69" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M69" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N69" s="48">
         <v>5</v>
@@ -4825,7 +4826,7 @@
     </row>
     <row r="70" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B70" s="50" t="b">
         <v>1</v>
@@ -4857,11 +4858,11 @@
       <c r="K70" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L70" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M70" s="19">
-        <v>2</v>
+      <c r="L70" s="7">
+        <v>0</v>
+      </c>
+      <c r="M70" s="7">
+        <v>0.1</v>
       </c>
       <c r="N70" s="50">
         <v>2</v>
@@ -4872,7 +4873,7 @@
     </row>
     <row r="71" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B71" s="49" t="b">
         <v>1</v>
@@ -4899,7 +4900,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K71" s="49" t="s">
         <v>8</v>
@@ -4914,7 +4915,7 @@
         <v>60</v>
       </c>
       <c r="O71" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P71" s="17">
         <v>-160</v>
@@ -4925,7 +4926,7 @@
     </row>
     <row r="72" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B72" s="48" t="b">
         <v>1</v>
@@ -4976,7 +4977,7 @@
     </row>
     <row r="73" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B73" s="48" t="b">
         <v>1</v>
@@ -5027,7 +5028,7 @@
     </row>
     <row r="74" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B74" s="48" t="b">
         <v>1</v>
@@ -5060,10 +5061,10 @@
         <v>8</v>
       </c>
       <c r="L74" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M74" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N74" s="48">
         <v>5</v>
@@ -5074,7 +5075,7 @@
     </row>
     <row r="75" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B75" s="50" t="b">
         <v>1</v>
@@ -5106,11 +5107,11 @@
       <c r="K75" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L75" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M75" s="19">
-        <v>2</v>
+      <c r="L75" s="7">
+        <v>0</v>
+      </c>
+      <c r="M75" s="7">
+        <v>0.1</v>
       </c>
       <c r="N75" s="50">
         <v>2</v>
@@ -5121,7 +5122,7 @@
     </row>
     <row r="76" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B76" s="49" t="b">
         <v>1</v>
@@ -5148,7 +5149,7 @@
         <v>1</v>
       </c>
       <c r="J76" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K76" s="49" t="s">
         <v>8</v>
@@ -5163,7 +5164,7 @@
         <v>60</v>
       </c>
       <c r="O76" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P76" s="17">
         <v>-160</v>
@@ -5174,7 +5175,7 @@
     </row>
     <row r="77" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B77" s="48" t="b">
         <v>1</v>
@@ -5225,7 +5226,7 @@
     </row>
     <row r="78" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B78" s="48" t="b">
         <v>1</v>
@@ -5276,7 +5277,7 @@
     </row>
     <row r="79" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B79" s="48" t="b">
         <v>1</v>
@@ -5309,10 +5310,10 @@
         <v>8</v>
       </c>
       <c r="L79" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M79" s="7">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="N79" s="48">
         <v>5</v>
@@ -5323,7 +5324,7 @@
     </row>
     <row r="80" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B80" s="50" t="b">
         <v>1</v>
@@ -5355,11 +5356,11 @@
       <c r="K80" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L80" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M80" s="19">
-        <v>2</v>
+      <c r="L80" s="7">
+        <v>0</v>
+      </c>
+      <c r="M80" s="7">
+        <v>0.1</v>
       </c>
       <c r="N80" s="50">
         <v>2</v>
@@ -5370,7 +5371,7 @@
     </row>
     <row r="81" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B81" s="49" t="b">
         <v>1</v>
@@ -5397,7 +5398,7 @@
         <v>1</v>
       </c>
       <c r="J81" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K81" s="49" t="s">
         <v>8</v>
@@ -5412,7 +5413,7 @@
         <v>60</v>
       </c>
       <c r="O81" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P81" s="17">
         <v>-160</v>
@@ -5423,7 +5424,7 @@
     </row>
     <row r="82" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B82" s="48" t="b">
         <v>1</v>
@@ -5474,7 +5475,7 @@
     </row>
     <row r="83" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B83" s="48" t="b">
         <v>1</v>
@@ -5525,7 +5526,7 @@
     </row>
     <row r="84" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B84" s="48" t="b">
         <v>1</v>
@@ -5558,10 +5559,10 @@
         <v>8</v>
       </c>
       <c r="L84" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M84" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N84" s="48">
         <v>5</v>
@@ -5572,7 +5573,7 @@
     </row>
     <row r="85" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B85" s="50" t="b">
         <v>1</v>
@@ -5604,11 +5605,11 @@
       <c r="K85" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L85" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M85" s="19">
-        <v>2</v>
+      <c r="L85" s="7">
+        <v>0</v>
+      </c>
+      <c r="M85" s="7">
+        <v>1</v>
       </c>
       <c r="N85" s="50">
         <v>2</v>
@@ -5619,7 +5620,7 @@
     </row>
     <row r="86" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B86" s="49" t="b">
         <v>1</v>
@@ -5646,22 +5647,22 @@
         <v>1</v>
       </c>
       <c r="J86" s="49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K86" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L86" s="16">
-        <v>0</v>
-      </c>
-      <c r="M86" s="16">
+      <c r="L86" s="22">
+        <v>0</v>
+      </c>
+      <c r="M86" s="17">
         <v>1</v>
       </c>
       <c r="N86" s="49">
         <v>60</v>
       </c>
       <c r="O86" s="22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P86" s="17">
         <v>-160</v>
@@ -5672,7 +5673,7 @@
     </row>
     <row r="87" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B87" s="48" t="b">
         <v>1</v>
@@ -5704,10 +5705,10 @@
       <c r="K87" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L87" s="7">
-        <v>0</v>
-      </c>
-      <c r="M87" s="7">
+      <c r="L87" s="21">
+        <v>0</v>
+      </c>
+      <c r="M87" s="8">
         <v>1</v>
       </c>
       <c r="N87" s="48">
@@ -5723,7 +5724,7 @@
     </row>
     <row r="88" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B88" s="48" t="b">
         <v>1</v>
@@ -5755,10 +5756,10 @@
       <c r="K88" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L88" s="7">
-        <v>0</v>
-      </c>
-      <c r="M88" s="7">
+      <c r="L88" s="21">
+        <v>0</v>
+      </c>
+      <c r="M88" s="8">
         <v>1</v>
       </c>
       <c r="N88" s="48">
@@ -5774,7 +5775,7 @@
     </row>
     <row r="89" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B89" s="48" t="b">
         <v>1</v>
@@ -5806,11 +5807,11 @@
       <c r="K89" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L89" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="M89" s="7">
-        <v>2</v>
+      <c r="L89" s="21">
+        <v>0</v>
+      </c>
+      <c r="M89" s="8">
+        <v>1</v>
       </c>
       <c r="N89" s="48">
         <v>5</v>
@@ -5821,7 +5822,7 @@
     </row>
     <row r="90" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B90" s="50" t="b">
         <v>1</v>
@@ -5853,11 +5854,11 @@
       <c r="K90" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L90" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="M90" s="19">
-        <v>2</v>
+      <c r="L90" s="23">
+        <v>0</v>
+      </c>
+      <c r="M90" s="20">
+        <v>1</v>
       </c>
       <c r="N90" s="50">
         <v>2</v>
@@ -5868,7 +5869,7 @@
     </row>
     <row r="91" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B91" s="48" t="b">
         <v>1</v>
@@ -5895,7 +5896,7 @@
         <v>1</v>
       </c>
       <c r="J91" s="48" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K91" s="48" t="s">
         <v>8</v>
@@ -5910,7 +5911,7 @@
         <v>60</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="P91" s="8">
         <v>-160</v>
@@ -5921,7 +5922,7 @@
     </row>
     <row r="92" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B92" s="48" t="b">
         <v>1</v>
@@ -5972,7 +5973,7 @@
     </row>
     <row r="93" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B93" s="48" t="b">
         <v>1</v>
@@ -6023,7 +6024,7 @@
     </row>
     <row r="94" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B94" s="48" t="b">
         <v>1</v>
@@ -6056,10 +6057,10 @@
         <v>8</v>
       </c>
       <c r="L94" s="7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M94" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N94" s="48">
         <v>5</v>
@@ -6070,7 +6071,7 @@
     </row>
     <row r="95" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B95" s="51" t="b">
         <v>1</v>
@@ -6103,10 +6104,10 @@
         <v>8</v>
       </c>
       <c r="L95" s="10">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M95" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N95" s="51">
         <v>2</v>
@@ -6125,15 +6126,20 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:Q95">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:Q3">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B95">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Using consistent WL for calculation of bank position error and making bank position error calculation work for left bank as well as right bank (i.e. outer bend for bends in either direction)
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@205 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="157">
   <si>
     <t>Stencil</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Flux</t>
   </si>
   <si>
-    <t>Flow</t>
-  </si>
-  <si>
     <t>Resolution</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
   </si>
   <si>
     <t>Nicolas derivative/test</t>
-  </si>
-  <si>
-    <t>Bankfull</t>
   </si>
   <si>
     <t>Is Bank ID sensitive to resolution</t>
@@ -516,6 +510,12 @@
   </si>
   <si>
     <t>7 + threshold height trigger</t>
+  </si>
+  <si>
+    <t>BankTestWL</t>
+  </si>
+  <si>
+    <t>VbankTestWL</t>
   </si>
 </sst>
 </file>
@@ -960,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1053,6 +1053,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1069,7 +1072,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1367,13 +1377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q95"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8:O10"/>
+      <selection pane="bottomRight" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,106 +1394,111 @@
     <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="9.5703125" customWidth="1"/>
     <col min="15" max="15" width="22.140625" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="61" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="46"/>
       <c r="C1" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="54"/>
+        <v>23</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="55"/>
       <c r="F1" s="26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I1" s="46"/>
       <c r="J1" s="46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K1" s="46"/>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="56"/>
+      <c r="N1" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="55"/>
-      <c r="N1" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" s="56" t="s">
+      <c r="O2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="Q2" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="48" t="b">
         <v>1</v>
@@ -1510,10 +1525,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="K3" s="48" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K3" s="48">
+        <v>212.5</v>
       </c>
       <c r="L3" s="7">
         <v>0.1</v>
@@ -1525,18 +1540,21 @@
         <v>120</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P3" s="8">
         <v>-160</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="48" t="b">
         <v>1</v>
@@ -1563,10 +1581,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K4" s="48">
+        <v>212.5</v>
       </c>
       <c r="L4" s="7">
         <v>0.1</v>
@@ -1578,16 +1596,19 @@
         <v>60</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P4" s="8">
         <v>-160</v>
       </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="48" t="b">
         <v>1</v>
@@ -1614,10 +1635,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K5" s="48">
+        <v>212.5</v>
       </c>
       <c r="L5" s="7">
         <v>0.1</v>
@@ -1629,16 +1650,19 @@
         <v>20</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P5" s="8">
         <v>-160</v>
       </c>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q5" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R5" s="8"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="48" t="b">
         <v>1</v>
@@ -1665,16 +1689,16 @@
         <v>1</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K6" s="48">
+        <v>212.5</v>
       </c>
       <c r="L6" s="7">
         <v>0.1</v>
       </c>
       <c r="M6" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N6" s="48">
         <v>5</v>
@@ -1682,10 +1706,11 @@
       <c r="O6" s="21"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="8"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="48" t="b">
         <v>1</v>
@@ -1712,16 +1737,16 @@
         <v>1</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="48" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K7" s="48">
+        <v>212.5</v>
       </c>
       <c r="L7" s="7">
         <v>0.1</v>
       </c>
       <c r="M7" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N7" s="48">
         <v>2</v>
@@ -1729,10 +1754,11 @@
       <c r="O7" s="21"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="48" t="b">
         <v>1</v>
@@ -1759,10 +1785,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K8" s="48">
+        <v>212.5</v>
       </c>
       <c r="L8" s="7">
         <v>0.1</v>
@@ -1774,16 +1800,15 @@
         <v>20</v>
       </c>
       <c r="O8" s="21"/>
-      <c r="P8" s="8">
-        <v>-160</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" s="48" t="b">
         <v>1</v>
@@ -1810,10 +1835,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K9" s="48">
+        <v>212.5</v>
       </c>
       <c r="L9" s="7">
         <v>0.1</v>
@@ -1825,16 +1850,15 @@
         <v>5</v>
       </c>
       <c r="O9" s="21"/>
-      <c r="P9" s="8">
-        <v>-160</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B10" s="50" t="b">
         <v>1</v>
@@ -1861,10 +1885,10 @@
         <v>0.5</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="50" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K10" s="50">
+        <v>212.5</v>
       </c>
       <c r="L10" s="19">
         <v>0.1</v>
@@ -1876,16 +1900,15 @@
         <v>60</v>
       </c>
       <c r="O10" s="23"/>
-      <c r="P10" s="20">
-        <v>-160</v>
-      </c>
-      <c r="Q10" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="49" t="b">
         <v>1</v>
@@ -1912,10 +1935,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K11" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K11" s="49">
+        <v>212.5</v>
       </c>
       <c r="L11" s="16">
         <v>0</v>
@@ -1927,18 +1950,21 @@
         <v>60</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P11" s="17">
         <v>-160</v>
       </c>
-      <c r="Q11" s="49" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q11" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R11" s="49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="48" t="b">
         <v>1</v>
@@ -1965,10 +1991,10 @@
         <v>1</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K12" s="48">
+        <v>212.5</v>
       </c>
       <c r="L12" s="7">
         <v>0</v>
@@ -1980,16 +2006,19 @@
         <v>60</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P12" s="8">
         <v>-160</v>
       </c>
-      <c r="Q12" s="48"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q12" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R12" s="48"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" s="48" t="b">
         <v>1</v>
@@ -2016,10 +2045,10 @@
         <v>1</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K13" s="48">
+        <v>212.5</v>
       </c>
       <c r="L13" s="7">
         <v>0</v>
@@ -2031,16 +2060,19 @@
         <v>20</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P13" s="8">
         <v>-160</v>
       </c>
-      <c r="Q13" s="48"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q13" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R13" s="48"/>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="48" t="b">
         <v>1</v>
@@ -2067,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K14" s="48">
+        <v>212.5</v>
       </c>
       <c r="L14" s="7">
         <v>0</v>
@@ -2083,11 +2115,12 @@
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="48"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q14" s="8"/>
+      <c r="R14" s="48"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B15" s="50" t="b">
         <v>1</v>
@@ -2114,10 +2147,10 @@
         <v>1</v>
       </c>
       <c r="J15" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K15" s="50">
+        <v>212.5</v>
       </c>
       <c r="L15" s="7">
         <v>0</v>
@@ -2130,11 +2163,12 @@
       </c>
       <c r="O15" s="23"/>
       <c r="P15" s="20"/>
-      <c r="Q15" s="50"/>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q15" s="20"/>
+      <c r="R15" s="50"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="49" t="b">
         <v>1</v>
@@ -2161,10 +2195,10 @@
         <v>1</v>
       </c>
       <c r="J16" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K16" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K16" s="49">
+        <v>212.5</v>
       </c>
       <c r="L16" s="16">
         <v>0</v>
@@ -2176,18 +2210,21 @@
         <v>60</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P16" s="17">
         <v>-160</v>
       </c>
-      <c r="Q16" s="49" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q16" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R16" s="49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="48" t="b">
         <v>1</v>
@@ -2214,10 +2251,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K17" s="48">
+        <v>212.5</v>
       </c>
       <c r="L17" s="7">
         <v>0</v>
@@ -2229,16 +2266,19 @@
         <v>60</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P17" s="8">
         <v>-160</v>
       </c>
-      <c r="Q17" s="48"/>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q17" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R17" s="48"/>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="48" t="b">
         <v>1</v>
@@ -2265,10 +2305,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K18" s="48">
+        <v>212.5</v>
       </c>
       <c r="L18" s="7">
         <v>0</v>
@@ -2280,16 +2320,19 @@
         <v>20</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P18" s="8">
         <v>-160</v>
       </c>
-      <c r="Q18" s="48"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q18" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R18" s="48"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="48" t="b">
         <v>1</v>
@@ -2316,10 +2359,10 @@
         <v>1</v>
       </c>
       <c r="J19" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K19" s="48">
+        <v>212.5</v>
       </c>
       <c r="L19" s="7">
         <v>0</v>
@@ -2332,11 +2375,12 @@
       </c>
       <c r="O19" s="21"/>
       <c r="P19" s="8"/>
-      <c r="Q19" s="48"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q19" s="8"/>
+      <c r="R19" s="48"/>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" s="50" t="b">
         <v>1</v>
@@ -2363,10 +2407,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K20" s="50">
+        <v>212.5</v>
       </c>
       <c r="L20" s="19">
         <v>0</v>
@@ -2379,11 +2423,12 @@
       </c>
       <c r="O20" s="23"/>
       <c r="P20" s="20"/>
-      <c r="Q20" s="50"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q20" s="20"/>
+      <c r="R20" s="50"/>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="49" t="b">
         <v>1</v>
@@ -2410,10 +2455,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K21" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K21" s="49">
+        <v>212.5</v>
       </c>
       <c r="L21" s="16">
         <v>0</v>
@@ -2425,18 +2470,21 @@
         <v>60</v>
       </c>
       <c r="O21" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P21" s="17">
         <v>-160</v>
       </c>
-      <c r="Q21" s="49" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q21" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R21" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B22" s="48" t="b">
         <v>1</v>
@@ -2463,10 +2511,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K22" s="48">
+        <v>212.5</v>
       </c>
       <c r="L22" s="7">
         <v>0</v>
@@ -2478,16 +2526,19 @@
         <v>60</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P22" s="8">
         <v>-160</v>
       </c>
-      <c r="Q22" s="48"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q22" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R22" s="48"/>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="48" t="b">
         <v>1</v>
@@ -2514,10 +2565,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K23" s="48">
+        <v>212.5</v>
       </c>
       <c r="L23" s="7">
         <v>0</v>
@@ -2529,16 +2580,19 @@
         <v>20</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P23" s="8">
         <v>-160</v>
       </c>
-      <c r="Q23" s="48"/>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q23" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R23" s="48"/>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" s="48" t="b">
         <v>1</v>
@@ -2565,10 +2619,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K24" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K24" s="48">
+        <v>212.5</v>
       </c>
       <c r="L24" s="7">
         <v>0</v>
@@ -2581,11 +2635,12 @@
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="8"/>
-      <c r="Q24" s="48"/>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q24" s="8"/>
+      <c r="R24" s="48"/>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" s="50" t="b">
         <v>1</v>
@@ -2612,10 +2667,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K25" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K25" s="50">
+        <v>212.5</v>
       </c>
       <c r="L25" s="19">
         <v>0</v>
@@ -2628,11 +2683,12 @@
       </c>
       <c r="O25" s="23"/>
       <c r="P25" s="20"/>
-      <c r="Q25" s="50"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q25" s="20"/>
+      <c r="R25" s="50"/>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="49" t="b">
         <v>1</v>
@@ -2659,10 +2715,10 @@
         <v>1</v>
       </c>
       <c r="J26" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K26" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K26" s="49">
+        <v>212.5</v>
       </c>
       <c r="L26" s="16">
         <v>0</v>
@@ -2674,18 +2730,21 @@
         <v>60</v>
       </c>
       <c r="O26" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P26" s="17">
         <v>-160</v>
       </c>
-      <c r="Q26" s="49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q26" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R26" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="48" t="b">
         <v>1</v>
@@ -2712,10 +2771,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K27" s="48">
+        <v>212.5</v>
       </c>
       <c r="L27" s="7">
         <v>0</v>
@@ -2727,16 +2786,19 @@
         <v>60</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P27" s="8">
         <v>-160</v>
       </c>
-      <c r="Q27" s="48"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q27" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R27" s="48"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="48" t="b">
         <v>1</v>
@@ -2763,10 +2825,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K28" s="48">
+        <v>212.5</v>
       </c>
       <c r="L28" s="7">
         <v>0</v>
@@ -2778,16 +2840,19 @@
         <v>20</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P28" s="8">
         <v>-160</v>
       </c>
-      <c r="Q28" s="48"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q28" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R28" s="48"/>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="48" t="b">
         <v>1</v>
@@ -2814,10 +2879,10 @@
         <v>1</v>
       </c>
       <c r="J29" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K29" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K29" s="48">
+        <v>212.5</v>
       </c>
       <c r="L29" s="7">
         <v>0</v>
@@ -2830,11 +2895,12 @@
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="8"/>
-      <c r="Q29" s="48"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q29" s="8"/>
+      <c r="R29" s="48"/>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B30" s="50" t="b">
         <v>1</v>
@@ -2861,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K30" s="50">
+        <v>212.5</v>
       </c>
       <c r="L30" s="7">
         <v>0</v>
@@ -2877,11 +2943,12 @@
       </c>
       <c r="O30" s="23"/>
       <c r="P30" s="20"/>
-      <c r="Q30" s="50"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q30" s="20"/>
+      <c r="R30" s="50"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="49" t="b">
         <v>1</v>
@@ -2908,10 +2975,10 @@
         <v>1</v>
       </c>
       <c r="J31" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K31" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K31" s="49">
+        <v>212.5</v>
       </c>
       <c r="L31" s="16">
         <v>0</v>
@@ -2923,18 +2990,21 @@
         <v>60</v>
       </c>
       <c r="O31" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P31" s="17">
         <v>-160</v>
       </c>
-      <c r="Q31" s="49" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q31" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R31" s="49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="48" t="b">
         <v>1</v>
@@ -2961,10 +3031,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K32" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K32" s="48">
+        <v>212.5</v>
       </c>
       <c r="L32" s="7">
         <v>0</v>
@@ -2976,16 +3046,19 @@
         <v>60</v>
       </c>
       <c r="O32" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P32" s="8">
         <v>-160</v>
       </c>
-      <c r="Q32" s="48"/>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q32" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R32" s="48"/>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B33" s="48" t="b">
         <v>1</v>
@@ -3012,10 +3085,10 @@
         <v>1</v>
       </c>
       <c r="J33" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K33" s="48">
+        <v>212.5</v>
       </c>
       <c r="L33" s="7">
         <v>0</v>
@@ -3027,16 +3100,19 @@
         <v>20</v>
       </c>
       <c r="O33" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P33" s="8">
         <v>-160</v>
       </c>
-      <c r="Q33" s="48"/>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q33" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R33" s="48"/>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" s="48" t="b">
         <v>1</v>
@@ -3063,10 +3139,10 @@
         <v>1</v>
       </c>
       <c r="J34" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K34" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K34" s="48">
+        <v>212.5</v>
       </c>
       <c r="L34" s="7">
         <v>0</v>
@@ -3079,11 +3155,12 @@
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="8"/>
-      <c r="Q34" s="48"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q34" s="8"/>
+      <c r="R34" s="48"/>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B35" s="50" t="b">
         <v>1</v>
@@ -3110,10 +3187,10 @@
         <v>1</v>
       </c>
       <c r="J35" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K35" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K35" s="50">
+        <v>212.5</v>
       </c>
       <c r="L35" s="7">
         <v>0</v>
@@ -3126,11 +3203,12 @@
       </c>
       <c r="O35" s="23"/>
       <c r="P35" s="20"/>
-      <c r="Q35" s="50"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q35" s="20"/>
+      <c r="R35" s="50"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36" s="49" t="b">
         <v>1</v>
@@ -3157,10 +3235,10 @@
         <v>1</v>
       </c>
       <c r="J36" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K36" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K36" s="49">
+        <v>212.5</v>
       </c>
       <c r="L36" s="16">
         <v>0</v>
@@ -3172,18 +3250,21 @@
         <v>60</v>
       </c>
       <c r="O36" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P36" s="17">
         <v>-160</v>
       </c>
-      <c r="Q36" s="49" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q36" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R36" s="49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37" s="48" t="b">
         <v>1</v>
@@ -3210,10 +3291,10 @@
         <v>1</v>
       </c>
       <c r="J37" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K37" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K37" s="48">
+        <v>212.5</v>
       </c>
       <c r="L37" s="7">
         <v>0</v>
@@ -3225,16 +3306,19 @@
         <v>60</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P37" s="8">
         <v>-160</v>
       </c>
-      <c r="Q37" s="48"/>
-    </row>
-    <row r="38" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q37" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R37" s="48"/>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B38" s="48" t="b">
         <v>1</v>
@@ -3261,10 +3345,10 @@
         <v>1</v>
       </c>
       <c r="J38" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K38" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K38" s="48">
+        <v>212.5</v>
       </c>
       <c r="L38" s="7">
         <v>0</v>
@@ -3276,16 +3360,19 @@
         <v>20</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P38" s="8">
         <v>-160</v>
       </c>
-      <c r="Q38" s="48"/>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q38" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R38" s="48"/>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B39" s="48" t="b">
         <v>1</v>
@@ -3312,10 +3399,10 @@
         <v>1</v>
       </c>
       <c r="J39" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K39" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K39" s="48">
+        <v>212.5</v>
       </c>
       <c r="L39" s="7">
         <v>0</v>
@@ -3328,11 +3415,12 @@
       </c>
       <c r="O39" s="21"/>
       <c r="P39" s="8"/>
-      <c r="Q39" s="48"/>
-    </row>
-    <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q39" s="8"/>
+      <c r="R39" s="48"/>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B40" s="50" t="b">
         <v>1</v>
@@ -3359,10 +3447,10 @@
         <v>1</v>
       </c>
       <c r="J40" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K40" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K40" s="50">
+        <v>212.5</v>
       </c>
       <c r="L40" s="7">
         <v>0</v>
@@ -3375,11 +3463,12 @@
       </c>
       <c r="O40" s="23"/>
       <c r="P40" s="20"/>
-      <c r="Q40" s="50"/>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q40" s="20"/>
+      <c r="R40" s="50"/>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B41" s="49" t="b">
         <v>1</v>
@@ -3406,10 +3495,10 @@
         <v>1</v>
       </c>
       <c r="J41" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K41" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K41" s="49">
+        <v>212.5</v>
       </c>
       <c r="L41" s="16">
         <v>0</v>
@@ -3421,18 +3510,21 @@
         <v>60</v>
       </c>
       <c r="O41" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P41" s="17">
         <v>-160</v>
       </c>
-      <c r="Q41" s="49" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q41" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R41" s="49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B42" s="48" t="b">
         <v>1</v>
@@ -3459,10 +3551,10 @@
         <v>1</v>
       </c>
       <c r="J42" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K42" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K42" s="48">
+        <v>212.5</v>
       </c>
       <c r="L42" s="7">
         <v>0</v>
@@ -3474,16 +3566,19 @@
         <v>60</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P42" s="8">
         <v>-160</v>
       </c>
-      <c r="Q42" s="48"/>
-    </row>
-    <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q42" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R42" s="48"/>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B43" s="48" t="b">
         <v>1</v>
@@ -3510,10 +3605,10 @@
         <v>1</v>
       </c>
       <c r="J43" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K43" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K43" s="48">
+        <v>212.5</v>
       </c>
       <c r="L43" s="7">
         <v>0</v>
@@ -3525,16 +3620,19 @@
         <v>20</v>
       </c>
       <c r="O43" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P43" s="8">
         <v>-160</v>
       </c>
-      <c r="Q43" s="48"/>
-    </row>
-    <row r="44" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q43" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R43" s="48"/>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B44" s="48" t="b">
         <v>1</v>
@@ -3561,10 +3659,10 @@
         <v>1</v>
       </c>
       <c r="J44" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K44" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K44" s="48">
+        <v>212.5</v>
       </c>
       <c r="L44" s="7">
         <v>0</v>
@@ -3577,11 +3675,12 @@
       </c>
       <c r="O44" s="21"/>
       <c r="P44" s="8"/>
-      <c r="Q44" s="48"/>
-    </row>
-    <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q44" s="8"/>
+      <c r="R44" s="48"/>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B45" s="50" t="b">
         <v>1</v>
@@ -3608,10 +3707,10 @@
         <v>1</v>
       </c>
       <c r="J45" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K45" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K45" s="50">
+        <v>212.5</v>
       </c>
       <c r="L45" s="7">
         <v>0</v>
@@ -3624,11 +3723,12 @@
       </c>
       <c r="O45" s="23"/>
       <c r="P45" s="20"/>
-      <c r="Q45" s="50"/>
-    </row>
-    <row r="46" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q45" s="20"/>
+      <c r="R45" s="50"/>
+    </row>
+    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" s="49" t="b">
         <v>1</v>
@@ -3655,10 +3755,10 @@
         <v>1</v>
       </c>
       <c r="J46" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K46" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K46" s="49">
+        <v>212.5</v>
       </c>
       <c r="L46" s="16">
         <v>0</v>
@@ -3670,18 +3770,21 @@
         <v>60</v>
       </c>
       <c r="O46" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P46" s="17">
         <v>-160</v>
       </c>
-      <c r="Q46" s="49" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q46" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R46" s="49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B47" s="48" t="b">
         <v>1</v>
@@ -3708,10 +3811,10 @@
         <v>1</v>
       </c>
       <c r="J47" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K47" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K47" s="48">
+        <v>212.5</v>
       </c>
       <c r="L47" s="7">
         <v>0</v>
@@ -3723,16 +3826,19 @@
         <v>60</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P47" s="8">
         <v>-160</v>
       </c>
-      <c r="Q47" s="48"/>
-    </row>
-    <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q47" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R47" s="48"/>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B48" s="48" t="b">
         <v>1</v>
@@ -3759,10 +3865,10 @@
         <v>1</v>
       </c>
       <c r="J48" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K48" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K48" s="48">
+        <v>212.5</v>
       </c>
       <c r="L48" s="7">
         <v>0</v>
@@ -3774,16 +3880,19 @@
         <v>20</v>
       </c>
       <c r="O48" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P48" s="8">
         <v>-160</v>
       </c>
-      <c r="Q48" s="48"/>
-    </row>
-    <row r="49" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q48" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R48" s="48"/>
+    </row>
+    <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B49" s="48" t="b">
         <v>1</v>
@@ -3810,10 +3919,10 @@
         <v>1</v>
       </c>
       <c r="J49" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K49" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K49" s="48">
+        <v>212.5</v>
       </c>
       <c r="L49" s="7">
         <v>0</v>
@@ -3826,11 +3935,12 @@
       </c>
       <c r="O49" s="21"/>
       <c r="P49" s="8"/>
-      <c r="Q49" s="48"/>
-    </row>
-    <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q49" s="8"/>
+      <c r="R49" s="48"/>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B50" s="50" t="b">
         <v>1</v>
@@ -3857,10 +3967,10 @@
         <v>1</v>
       </c>
       <c r="J50" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K50" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K50" s="50">
+        <v>212.5</v>
       </c>
       <c r="L50" s="7">
         <v>0</v>
@@ -3873,11 +3983,12 @@
       </c>
       <c r="O50" s="23"/>
       <c r="P50" s="20"/>
-      <c r="Q50" s="50"/>
-    </row>
-    <row r="51" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q50" s="20"/>
+      <c r="R50" s="50"/>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B51" s="49" t="b">
         <v>1</v>
@@ -3904,10 +4015,10 @@
         <v>1</v>
       </c>
       <c r="J51" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K51" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K51" s="49">
+        <v>212.5</v>
       </c>
       <c r="L51" s="16">
         <v>0</v>
@@ -3919,18 +4030,21 @@
         <v>60</v>
       </c>
       <c r="O51" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P51" s="17">
         <v>-160</v>
       </c>
-      <c r="Q51" s="49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q51" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R51" s="49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" s="48" t="b">
         <v>1</v>
@@ -3957,10 +4071,10 @@
         <v>1</v>
       </c>
       <c r="J52" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K52" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K52" s="48">
+        <v>212.5</v>
       </c>
       <c r="L52" s="7">
         <v>0</v>
@@ -3972,16 +4086,19 @@
         <v>60</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P52" s="8">
         <v>-160</v>
       </c>
-      <c r="Q52" s="48"/>
-    </row>
-    <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q52" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R52" s="48"/>
+    </row>
+    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B53" s="48" t="b">
         <v>1</v>
@@ -4008,10 +4125,10 @@
         <v>1</v>
       </c>
       <c r="J53" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K53" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K53" s="48">
+        <v>212.5</v>
       </c>
       <c r="L53" s="7">
         <v>0</v>
@@ -4023,16 +4140,19 @@
         <v>20</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P53" s="8">
         <v>-160</v>
       </c>
-      <c r="Q53" s="48"/>
-    </row>
-    <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q53" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R53" s="48"/>
+    </row>
+    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B54" s="48" t="b">
         <v>1</v>
@@ -4059,10 +4179,10 @@
         <v>1</v>
       </c>
       <c r="J54" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K54" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K54" s="48">
+        <v>212.5</v>
       </c>
       <c r="L54" s="7">
         <v>0</v>
@@ -4075,11 +4195,12 @@
       </c>
       <c r="O54" s="21"/>
       <c r="P54" s="8"/>
-      <c r="Q54" s="48"/>
-    </row>
-    <row r="55" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q54" s="8"/>
+      <c r="R54" s="48"/>
+    </row>
+    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B55" s="50" t="b">
         <v>1</v>
@@ -4106,10 +4227,10 @@
         <v>1</v>
       </c>
       <c r="J55" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K55" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K55" s="50">
+        <v>212.5</v>
       </c>
       <c r="L55" s="7">
         <v>0</v>
@@ -4122,11 +4243,12 @@
       </c>
       <c r="O55" s="23"/>
       <c r="P55" s="20"/>
-      <c r="Q55" s="50"/>
-    </row>
-    <row r="56" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q55" s="20"/>
+      <c r="R55" s="50"/>
+    </row>
+    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B56" s="49" t="b">
         <v>1</v>
@@ -4153,10 +4275,10 @@
         <v>1</v>
       </c>
       <c r="J56" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K56" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K56" s="49">
+        <v>212.5</v>
       </c>
       <c r="L56" s="16">
         <v>0</v>
@@ -4168,18 +4290,21 @@
         <v>60</v>
       </c>
       <c r="O56" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P56" s="17">
         <v>-160</v>
       </c>
-      <c r="Q56" s="49" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q56" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R56" s="49" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B57" s="48" t="b">
         <v>1</v>
@@ -4206,10 +4331,10 @@
         <v>1</v>
       </c>
       <c r="J57" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K57" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K57" s="48">
+        <v>212.5</v>
       </c>
       <c r="L57" s="7">
         <v>0</v>
@@ -4221,16 +4346,19 @@
         <v>60</v>
       </c>
       <c r="O57" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P57" s="8">
         <v>-160</v>
       </c>
-      <c r="Q57" s="48"/>
-    </row>
-    <row r="58" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q57" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R57" s="48"/>
+    </row>
+    <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B58" s="48" t="b">
         <v>1</v>
@@ -4257,10 +4385,10 @@
         <v>1</v>
       </c>
       <c r="J58" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K58" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K58" s="48">
+        <v>212.5</v>
       </c>
       <c r="L58" s="7">
         <v>0</v>
@@ -4272,16 +4400,19 @@
         <v>20</v>
       </c>
       <c r="O58" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P58" s="8">
         <v>-160</v>
       </c>
-      <c r="Q58" s="48"/>
-    </row>
-    <row r="59" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q58" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R58" s="48"/>
+    </row>
+    <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B59" s="48" t="b">
         <v>1</v>
@@ -4308,10 +4439,10 @@
         <v>1</v>
       </c>
       <c r="J59" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K59" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K59" s="48">
+        <v>212.5</v>
       </c>
       <c r="L59" s="7">
         <v>0</v>
@@ -4324,11 +4455,12 @@
       </c>
       <c r="O59" s="21"/>
       <c r="P59" s="8"/>
-      <c r="Q59" s="48"/>
-    </row>
-    <row r="60" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q59" s="8"/>
+      <c r="R59" s="48"/>
+    </row>
+    <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B60" s="50" t="b">
         <v>1</v>
@@ -4355,10 +4487,10 @@
         <v>1</v>
       </c>
       <c r="J60" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K60" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K60" s="50">
+        <v>212.5</v>
       </c>
       <c r="L60" s="7">
         <v>0</v>
@@ -4371,11 +4503,12 @@
       </c>
       <c r="O60" s="23"/>
       <c r="P60" s="20"/>
-      <c r="Q60" s="50"/>
-    </row>
-    <row r="61" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q60" s="20"/>
+      <c r="R60" s="50"/>
+    </row>
+    <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B61" s="49" t="b">
         <v>1</v>
@@ -4402,10 +4535,10 @@
         <v>1</v>
       </c>
       <c r="J61" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K61" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K61" s="49">
+        <v>212.5</v>
       </c>
       <c r="L61" s="16">
         <v>0</v>
@@ -4417,18 +4550,21 @@
         <v>60</v>
       </c>
       <c r="O61" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P61" s="17">
         <v>-160</v>
       </c>
-      <c r="Q61" s="49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q61" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R61" s="49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B62" s="48" t="b">
         <v>1</v>
@@ -4455,10 +4591,10 @@
         <v>1</v>
       </c>
       <c r="J62" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K62" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K62" s="48">
+        <v>212.5</v>
       </c>
       <c r="L62" s="7">
         <v>0</v>
@@ -4470,16 +4606,19 @@
         <v>60</v>
       </c>
       <c r="O62" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P62" s="8">
         <v>-160</v>
       </c>
-      <c r="Q62" s="48"/>
-    </row>
-    <row r="63" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q62" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R62" s="48"/>
+    </row>
+    <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B63" s="48" t="b">
         <v>1</v>
@@ -4506,10 +4645,10 @@
         <v>1</v>
       </c>
       <c r="J63" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K63" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K63" s="48">
+        <v>212.5</v>
       </c>
       <c r="L63" s="7">
         <v>0</v>
@@ -4521,16 +4660,19 @@
         <v>20</v>
       </c>
       <c r="O63" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P63" s="8">
         <v>-160</v>
       </c>
-      <c r="Q63" s="48"/>
-    </row>
-    <row r="64" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q63" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R63" s="48"/>
+    </row>
+    <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B64" s="48" t="b">
         <v>1</v>
@@ -4557,10 +4699,10 @@
         <v>1</v>
       </c>
       <c r="J64" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K64" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K64" s="48">
+        <v>212.5</v>
       </c>
       <c r="L64" s="7">
         <v>0</v>
@@ -4573,11 +4715,12 @@
       </c>
       <c r="O64" s="21"/>
       <c r="P64" s="8"/>
-      <c r="Q64" s="48"/>
-    </row>
-    <row r="65" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q64" s="8"/>
+      <c r="R64" s="48"/>
+    </row>
+    <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B65" s="50" t="b">
         <v>1</v>
@@ -4604,10 +4747,10 @@
         <v>1</v>
       </c>
       <c r="J65" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K65" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K65" s="50">
+        <v>212.5</v>
       </c>
       <c r="L65" s="7">
         <v>0</v>
@@ -4620,11 +4763,12 @@
       </c>
       <c r="O65" s="23"/>
       <c r="P65" s="20"/>
-      <c r="Q65" s="50"/>
-    </row>
-    <row r="66" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q65" s="20"/>
+      <c r="R65" s="50"/>
+    </row>
+    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B66" s="49" t="b">
         <v>1</v>
@@ -4651,10 +4795,10 @@
         <v>1</v>
       </c>
       <c r="J66" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K66" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K66" s="49">
+        <v>212.5</v>
       </c>
       <c r="L66" s="16">
         <v>0</v>
@@ -4666,18 +4810,21 @@
         <v>60</v>
       </c>
       <c r="O66" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P66" s="17">
         <v>-160</v>
       </c>
-      <c r="Q66" s="49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q66" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R66" s="49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B67" s="48" t="b">
         <v>1</v>
@@ -4704,10 +4851,10 @@
         <v>1</v>
       </c>
       <c r="J67" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K67" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K67" s="48">
+        <v>212.5</v>
       </c>
       <c r="L67" s="7">
         <v>0</v>
@@ -4719,16 +4866,19 @@
         <v>60</v>
       </c>
       <c r="O67" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P67" s="8">
         <v>-160</v>
       </c>
-      <c r="Q67" s="48"/>
-    </row>
-    <row r="68" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q67" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R67" s="48"/>
+    </row>
+    <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B68" s="48" t="b">
         <v>1</v>
@@ -4755,10 +4905,10 @@
         <v>1</v>
       </c>
       <c r="J68" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K68" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K68" s="48">
+        <v>212.5</v>
       </c>
       <c r="L68" s="7">
         <v>0</v>
@@ -4770,16 +4920,19 @@
         <v>20</v>
       </c>
       <c r="O68" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P68" s="8">
         <v>-160</v>
       </c>
-      <c r="Q68" s="48"/>
-    </row>
-    <row r="69" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q68" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R68" s="48"/>
+    </row>
+    <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B69" s="48" t="b">
         <v>1</v>
@@ -4806,10 +4959,10 @@
         <v>1</v>
       </c>
       <c r="J69" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K69" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K69" s="48">
+        <v>212.5</v>
       </c>
       <c r="L69" s="7">
         <v>0</v>
@@ -4822,11 +4975,12 @@
       </c>
       <c r="O69" s="21"/>
       <c r="P69" s="8"/>
-      <c r="Q69" s="48"/>
-    </row>
-    <row r="70" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q69" s="8"/>
+      <c r="R69" s="48"/>
+    </row>
+    <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B70" s="50" t="b">
         <v>1</v>
@@ -4853,10 +5007,10 @@
         <v>1</v>
       </c>
       <c r="J70" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K70" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K70" s="50">
+        <v>212.5</v>
       </c>
       <c r="L70" s="7">
         <v>0</v>
@@ -4869,11 +5023,12 @@
       </c>
       <c r="O70" s="23"/>
       <c r="P70" s="20"/>
-      <c r="Q70" s="50"/>
-    </row>
-    <row r="71" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q70" s="20"/>
+      <c r="R70" s="50"/>
+    </row>
+    <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B71" s="49" t="b">
         <v>1</v>
@@ -4900,10 +5055,10 @@
         <v>1</v>
       </c>
       <c r="J71" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K71" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K71" s="49">
+        <v>212.5</v>
       </c>
       <c r="L71" s="16">
         <v>0</v>
@@ -4915,18 +5070,21 @@
         <v>60</v>
       </c>
       <c r="O71" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P71" s="17">
         <v>-160</v>
       </c>
-      <c r="Q71" s="49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q71" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R71" s="49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B72" s="48" t="b">
         <v>1</v>
@@ -4953,10 +5111,10 @@
         <v>1</v>
       </c>
       <c r="J72" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K72" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K72" s="48">
+        <v>212.5</v>
       </c>
       <c r="L72" s="7">
         <v>0</v>
@@ -4968,16 +5126,19 @@
         <v>60</v>
       </c>
       <c r="O72" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P72" s="8">
         <v>-160</v>
       </c>
-      <c r="Q72" s="48"/>
-    </row>
-    <row r="73" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q72" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R72" s="48"/>
+    </row>
+    <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B73" s="48" t="b">
         <v>1</v>
@@ -5004,10 +5165,10 @@
         <v>1</v>
       </c>
       <c r="J73" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K73" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K73" s="48">
+        <v>212.5</v>
       </c>
       <c r="L73" s="7">
         <v>0</v>
@@ -5019,16 +5180,19 @@
         <v>20</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P73" s="8">
         <v>-160</v>
       </c>
-      <c r="Q73" s="48"/>
-    </row>
-    <row r="74" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q73" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R73" s="48"/>
+    </row>
+    <row r="74" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B74" s="48" t="b">
         <v>1</v>
@@ -5055,10 +5219,10 @@
         <v>1</v>
       </c>
       <c r="J74" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K74" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K74" s="48">
+        <v>212.5</v>
       </c>
       <c r="L74" s="7">
         <v>0</v>
@@ -5071,11 +5235,12 @@
       </c>
       <c r="O74" s="21"/>
       <c r="P74" s="8"/>
-      <c r="Q74" s="48"/>
-    </row>
-    <row r="75" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q74" s="8"/>
+      <c r="R74" s="48"/>
+    </row>
+    <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B75" s="50" t="b">
         <v>1</v>
@@ -5102,10 +5267,10 @@
         <v>1</v>
       </c>
       <c r="J75" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K75" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K75" s="50">
+        <v>212.5</v>
       </c>
       <c r="L75" s="7">
         <v>0</v>
@@ -5118,11 +5283,12 @@
       </c>
       <c r="O75" s="23"/>
       <c r="P75" s="20"/>
-      <c r="Q75" s="50"/>
-    </row>
-    <row r="76" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q75" s="20"/>
+      <c r="R75" s="50"/>
+    </row>
+    <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B76" s="49" t="b">
         <v>1</v>
@@ -5149,10 +5315,10 @@
         <v>1</v>
       </c>
       <c r="J76" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K76" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K76" s="49">
+        <v>212.5</v>
       </c>
       <c r="L76" s="16">
         <v>0</v>
@@ -5164,18 +5330,21 @@
         <v>60</v>
       </c>
       <c r="O76" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P76" s="17">
         <v>-160</v>
       </c>
-      <c r="Q76" s="49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q76" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R76" s="49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B77" s="48" t="b">
         <v>1</v>
@@ -5202,10 +5371,10 @@
         <v>1</v>
       </c>
       <c r="J77" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K77" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K77" s="48">
+        <v>212.5</v>
       </c>
       <c r="L77" s="7">
         <v>0</v>
@@ -5217,16 +5386,19 @@
         <v>60</v>
       </c>
       <c r="O77" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P77" s="8">
         <v>-160</v>
       </c>
-      <c r="Q77" s="48"/>
-    </row>
-    <row r="78" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q77" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R77" s="48"/>
+    </row>
+    <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B78" s="48" t="b">
         <v>1</v>
@@ -5253,10 +5425,10 @@
         <v>1</v>
       </c>
       <c r="J78" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K78" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K78" s="48">
+        <v>212.5</v>
       </c>
       <c r="L78" s="7">
         <v>0</v>
@@ -5268,16 +5440,19 @@
         <v>20</v>
       </c>
       <c r="O78" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P78" s="8">
         <v>-160</v>
       </c>
-      <c r="Q78" s="48"/>
-    </row>
-    <row r="79" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q78" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R78" s="48"/>
+    </row>
+    <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B79" s="48" t="b">
         <v>1</v>
@@ -5304,10 +5479,10 @@
         <v>1</v>
       </c>
       <c r="J79" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K79" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K79" s="48">
+        <v>212.5</v>
       </c>
       <c r="L79" s="7">
         <v>0</v>
@@ -5320,11 +5495,12 @@
       </c>
       <c r="O79" s="21"/>
       <c r="P79" s="8"/>
-      <c r="Q79" s="48"/>
-    </row>
-    <row r="80" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q79" s="8"/>
+      <c r="R79" s="48"/>
+    </row>
+    <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B80" s="50" t="b">
         <v>1</v>
@@ -5351,10 +5527,10 @@
         <v>1</v>
       </c>
       <c r="J80" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K80" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K80" s="50">
+        <v>212.5</v>
       </c>
       <c r="L80" s="7">
         <v>0</v>
@@ -5367,11 +5543,12 @@
       </c>
       <c r="O80" s="23"/>
       <c r="P80" s="20"/>
-      <c r="Q80" s="50"/>
-    </row>
-    <row r="81" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q80" s="20"/>
+      <c r="R80" s="50"/>
+    </row>
+    <row r="81" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B81" s="49" t="b">
         <v>1</v>
@@ -5398,10 +5575,10 @@
         <v>1</v>
       </c>
       <c r="J81" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K81" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K81" s="49">
+        <v>212.5</v>
       </c>
       <c r="L81" s="16">
         <v>0</v>
@@ -5413,18 +5590,21 @@
         <v>60</v>
       </c>
       <c r="O81" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P81" s="17">
         <v>-160</v>
       </c>
-      <c r="Q81" s="49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q81" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R81" s="49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B82" s="48" t="b">
         <v>1</v>
@@ -5451,10 +5631,10 @@
         <v>1</v>
       </c>
       <c r="J82" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K82" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K82" s="48">
+        <v>212.5</v>
       </c>
       <c r="L82" s="7">
         <v>0</v>
@@ -5466,16 +5646,19 @@
         <v>60</v>
       </c>
       <c r="O82" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P82" s="8">
         <v>-160</v>
       </c>
-      <c r="Q82" s="48"/>
-    </row>
-    <row r="83" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q82" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R82" s="48"/>
+    </row>
+    <row r="83" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B83" s="48" t="b">
         <v>1</v>
@@ -5502,10 +5685,10 @@
         <v>1</v>
       </c>
       <c r="J83" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K83" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K83" s="48">
+        <v>212.5</v>
       </c>
       <c r="L83" s="7">
         <v>0</v>
@@ -5517,16 +5700,19 @@
         <v>20</v>
       </c>
       <c r="O83" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P83" s="8">
         <v>-160</v>
       </c>
-      <c r="Q83" s="48"/>
-    </row>
-    <row r="84" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q83" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R83" s="48"/>
+    </row>
+    <row r="84" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B84" s="48" t="b">
         <v>1</v>
@@ -5553,10 +5739,10 @@
         <v>1</v>
       </c>
       <c r="J84" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K84" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K84" s="48">
+        <v>212.5</v>
       </c>
       <c r="L84" s="7">
         <v>0</v>
@@ -5569,11 +5755,12 @@
       </c>
       <c r="O84" s="21"/>
       <c r="P84" s="8"/>
-      <c r="Q84" s="48"/>
-    </row>
-    <row r="85" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q84" s="8"/>
+      <c r="R84" s="48"/>
+    </row>
+    <row r="85" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B85" s="50" t="b">
         <v>1</v>
@@ -5600,10 +5787,10 @@
         <v>1</v>
       </c>
       <c r="J85" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K85" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K85" s="50">
+        <v>212.5</v>
       </c>
       <c r="L85" s="7">
         <v>0</v>
@@ -5616,11 +5803,12 @@
       </c>
       <c r="O85" s="23"/>
       <c r="P85" s="20"/>
-      <c r="Q85" s="50"/>
-    </row>
-    <row r="86" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q85" s="20"/>
+      <c r="R85" s="50"/>
+    </row>
+    <row r="86" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B86" s="49" t="b">
         <v>1</v>
@@ -5647,10 +5835,10 @@
         <v>1</v>
       </c>
       <c r="J86" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="K86" s="49" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K86" s="49">
+        <v>212.5</v>
       </c>
       <c r="L86" s="22">
         <v>0</v>
@@ -5662,18 +5850,21 @@
         <v>60</v>
       </c>
       <c r="O86" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P86" s="17">
         <v>-160</v>
       </c>
-      <c r="Q86" s="49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q86" s="17">
+        <v>210.5</v>
+      </c>
+      <c r="R86" s="49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B87" s="48" t="b">
         <v>1</v>
@@ -5700,10 +5891,10 @@
         <v>1</v>
       </c>
       <c r="J87" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K87" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K87" s="48">
+        <v>212.5</v>
       </c>
       <c r="L87" s="21">
         <v>0</v>
@@ -5715,16 +5906,19 @@
         <v>60</v>
       </c>
       <c r="O87" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P87" s="8">
         <v>-160</v>
       </c>
-      <c r="Q87" s="48"/>
-    </row>
-    <row r="88" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q87" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R87" s="48"/>
+    </row>
+    <row r="88" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B88" s="48" t="b">
         <v>1</v>
@@ -5751,10 +5945,10 @@
         <v>1</v>
       </c>
       <c r="J88" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K88" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K88" s="48">
+        <v>212.5</v>
       </c>
       <c r="L88" s="21">
         <v>0</v>
@@ -5766,16 +5960,19 @@
         <v>20</v>
       </c>
       <c r="O88" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P88" s="8">
         <v>-160</v>
       </c>
-      <c r="Q88" s="48"/>
-    </row>
-    <row r="89" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q88" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R88" s="48"/>
+    </row>
+    <row r="89" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B89" s="48" t="b">
         <v>1</v>
@@ -5802,10 +5999,10 @@
         <v>1</v>
       </c>
       <c r="J89" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K89" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K89" s="48">
+        <v>212.5</v>
       </c>
       <c r="L89" s="21">
         <v>0</v>
@@ -5818,11 +6015,12 @@
       </c>
       <c r="O89" s="21"/>
       <c r="P89" s="8"/>
-      <c r="Q89" s="48"/>
-    </row>
-    <row r="90" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q89" s="8"/>
+      <c r="R89" s="48"/>
+    </row>
+    <row r="90" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B90" s="50" t="b">
         <v>1</v>
@@ -5849,10 +6047,10 @@
         <v>1</v>
       </c>
       <c r="J90" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K90" s="50" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K90" s="50">
+        <v>212.5</v>
       </c>
       <c r="L90" s="23">
         <v>0</v>
@@ -5865,11 +6063,12 @@
       </c>
       <c r="O90" s="23"/>
       <c r="P90" s="20"/>
-      <c r="Q90" s="50"/>
-    </row>
-    <row r="91" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q90" s="20"/>
+      <c r="R90" s="50"/>
+    </row>
+    <row r="91" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B91" s="48" t="b">
         <v>1</v>
@@ -5896,10 +6095,10 @@
         <v>1</v>
       </c>
       <c r="J91" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="K91" s="48" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="K91" s="48">
+        <v>212.5</v>
       </c>
       <c r="L91" s="7">
         <v>0</v>
@@ -5911,18 +6110,21 @@
         <v>60</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P91" s="8">
         <v>-160</v>
       </c>
-      <c r="Q91" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q91" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R91" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B92" s="48" t="b">
         <v>1</v>
@@ -5949,10 +6151,10 @@
         <v>1</v>
       </c>
       <c r="J92" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="K92" s="48" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="K92" s="48">
+        <v>212.5</v>
       </c>
       <c r="L92" s="7">
         <v>0</v>
@@ -5964,16 +6166,19 @@
         <v>60</v>
       </c>
       <c r="O92" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P92" s="8">
         <v>-160</v>
       </c>
-      <c r="Q92" s="8"/>
-    </row>
-    <row r="93" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q92" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R92" s="8"/>
+    </row>
+    <row r="93" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B93" s="48" t="b">
         <v>1</v>
@@ -6000,10 +6205,10 @@
         <v>1</v>
       </c>
       <c r="J93" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K93" s="48" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="K93" s="48">
+        <v>212.5</v>
       </c>
       <c r="L93" s="7">
         <v>0</v>
@@ -6015,16 +6220,19 @@
         <v>20</v>
       </c>
       <c r="O93" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P93" s="8">
         <v>-160</v>
       </c>
-      <c r="Q93" s="8"/>
-    </row>
-    <row r="94" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q93" s="8">
+        <v>210.5</v>
+      </c>
+      <c r="R93" s="8"/>
+    </row>
+    <row r="94" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B94" s="48" t="b">
         <v>1</v>
@@ -6051,10 +6259,10 @@
         <v>1</v>
       </c>
       <c r="J94" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="K94" s="48" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="K94" s="48">
+        <v>212.5</v>
       </c>
       <c r="L94" s="7">
         <v>0</v>
@@ -6068,10 +6276,11 @@
       <c r="O94" s="21"/>
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
-    </row>
-    <row r="95" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R94" s="8"/>
+    </row>
+    <row r="95" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B95" s="51" t="b">
         <v>1</v>
@@ -6098,10 +6307,10 @@
         <v>1</v>
       </c>
       <c r="J95" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="K95" s="51" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="K95" s="51">
+        <v>212.5</v>
       </c>
       <c r="L95" s="10">
         <v>0</v>
@@ -6115,6 +6324,7 @@
       <c r="O95" s="24"/>
       <c r="P95" s="11"/>
       <c r="Q95" s="11"/>
+      <c r="R95" s="11"/>
     </row>
   </sheetData>
   <sortState ref="A3:P76">
@@ -6125,14 +6335,24 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="O1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:Q95">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="A6:R95 A4:P5 R4:R5">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:Q3">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A3:R3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B3&lt;&gt;TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B4&lt;&gt;TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B5&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6160,57 +6380,57 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slight change to optimisation bounds for scenarios 1d and 1e
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@207 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1325,10 +1325,10 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1643,7 @@
         <v>0.1</v>
       </c>
       <c r="M6" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N6" s="47">
         <v>5</v>
@@ -1691,7 +1691,7 @@
         <v>0.1</v>
       </c>
       <c r="M7" s="6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N7" s="47">
         <v>2</v>

</xml_diff>

<commit_message>
Switching to central option for bedload at edges as this increases stability of high res models
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@208 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1325,10 +1325,10 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="47" t="s">
         <v>136</v>
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J4" s="47" t="s">
         <v>20</v>
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J5" s="47" t="s">
         <v>27</v>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J6" s="47" t="s">
         <v>34</v>
@@ -1640,10 +1640,10 @@
         <v>212.5</v>
       </c>
       <c r="L6" s="6">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N6" s="47">
         <v>5</v>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="47" t="s">
         <v>35</v>
@@ -1688,7 +1688,7 @@
         <v>212.5</v>
       </c>
       <c r="L7" s="6">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="M7" s="6">
         <v>10</v>
@@ -1727,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J8" s="47" t="s">
         <v>20</v>
@@ -1742,7 +1742,7 @@
         <v>2</v>
       </c>
       <c r="N8" s="47">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="7"/>
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J9" s="47" t="s">
         <v>20</v>
@@ -1792,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="N9" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O9" s="20"/>
       <c r="P9" s="7"/>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
         <v>20</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J11" s="48" t="s">
         <v>136</v>
@@ -1933,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J12" s="47" t="s">
         <v>20</v>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J13" s="47" t="s">
         <v>27</v>
@@ -2041,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J14" s="47" t="s">
         <v>34</v>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J15" s="49" t="s">
         <v>35</v>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="48" t="s">
         <v>136</v>
@@ -2193,7 +2193,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J17" s="47" t="s">
         <v>20</v>
@@ -2247,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J18" s="47" t="s">
         <v>27</v>
@@ -2301,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J19" s="47" t="s">
         <v>34</v>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="6">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="N19" s="47">
         <v>5</v>
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J20" s="49" t="s">
         <v>35</v>
@@ -2361,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="18">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="N20" s="49">
         <v>1</v>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J21" s="48" t="s">
         <v>136</v>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J22" s="47" t="s">
         <v>20</v>
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J23" s="47" t="s">
         <v>27</v>
@@ -2561,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J24" s="47" t="s">
         <v>34</v>
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="6">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="N24" s="47">
         <v>5</v>
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J25" s="49" t="s">
         <v>35</v>
@@ -2621,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="18">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="N25" s="49">
         <v>1</v>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J26" s="48" t="s">
         <v>136</v>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J27" s="47" t="s">
         <v>20</v>
@@ -2767,7 +2767,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J28" s="47" t="s">
         <v>27</v>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J29" s="47" t="s">
         <v>34</v>
@@ -2869,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J30" s="49" t="s">
         <v>35</v>
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J31" s="48" t="s">
         <v>136</v>
@@ -2973,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J32" s="47" t="s">
         <v>20</v>
@@ -3027,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J33" s="47" t="s">
         <v>27</v>
@@ -3081,7 +3081,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J34" s="47" t="s">
         <v>34</v>
@@ -3129,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J35" s="49" t="s">
         <v>35</v>
@@ -3177,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J36" s="48" t="s">
         <v>136</v>
@@ -3233,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J37" s="47" t="s">
         <v>20</v>
@@ -3287,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J38" s="47" t="s">
         <v>27</v>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J39" s="47" t="s">
         <v>34</v>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J40" s="49" t="s">
         <v>35</v>
@@ -3437,7 +3437,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J41" s="48" t="s">
         <v>136</v>
@@ -3493,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J42" s="47" t="s">
         <v>20</v>
@@ -3547,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J43" s="47" t="s">
         <v>27</v>
@@ -3601,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J44" s="47" t="s">
         <v>34</v>
@@ -3649,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J45" s="49" t="s">
         <v>35</v>
@@ -3697,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J46" s="48" t="s">
         <v>136</v>
@@ -3753,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J47" s="47" t="s">
         <v>20</v>
@@ -3807,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J48" s="47" t="s">
         <v>27</v>
@@ -3861,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J49" s="47" t="s">
         <v>34</v>
@@ -3909,7 +3909,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J50" s="49" t="s">
         <v>35</v>
@@ -3957,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J51" s="48" t="s">
         <v>136</v>
@@ -4013,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J52" s="47" t="s">
         <v>20</v>
@@ -4067,7 +4067,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J53" s="47" t="s">
         <v>27</v>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J54" s="47" t="s">
         <v>34</v>
@@ -4169,7 +4169,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J55" s="49" t="s">
         <v>35</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J56" s="48" t="s">
         <v>136</v>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J57" s="47" t="s">
         <v>20</v>
@@ -4327,7 +4327,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J58" s="47" t="s">
         <v>27</v>
@@ -4381,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J59" s="47" t="s">
         <v>34</v>
@@ -4429,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J60" s="49" t="s">
         <v>35</v>
@@ -4477,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J61" s="48" t="s">
         <v>136</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J62" s="47" t="s">
         <v>20</v>
@@ -4587,7 +4587,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J63" s="47" t="s">
         <v>27</v>
@@ -4641,7 +4641,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J64" s="47" t="s">
         <v>34</v>
@@ -4689,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J65" s="49" t="s">
         <v>35</v>
@@ -4737,7 +4737,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J66" s="48" t="s">
         <v>136</v>
@@ -4793,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J67" s="47" t="s">
         <v>20</v>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J68" s="47" t="s">
         <v>27</v>
@@ -4901,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J69" s="47" t="s">
         <v>34</v>
@@ -4949,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J70" s="49" t="s">
         <v>35</v>
@@ -4997,7 +4997,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J71" s="48" t="s">
         <v>136</v>
@@ -5053,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J72" s="47" t="s">
         <v>20</v>
@@ -5107,7 +5107,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J73" s="47" t="s">
         <v>27</v>
@@ -5161,7 +5161,7 @@
         <v>1</v>
       </c>
       <c r="I74" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J74" s="47" t="s">
         <v>34</v>
@@ -5209,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="I75" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J75" s="49" t="s">
         <v>35</v>
@@ -5257,7 +5257,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J76" s="48" t="s">
         <v>136</v>
@@ -5313,7 +5313,7 @@
         <v>1</v>
       </c>
       <c r="I77" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J77" s="47" t="s">
         <v>20</v>
@@ -5367,7 +5367,7 @@
         <v>1</v>
       </c>
       <c r="I78" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J78" s="47" t="s">
         <v>27</v>
@@ -5421,7 +5421,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J79" s="47" t="s">
         <v>34</v>
@@ -5469,7 +5469,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J80" s="49" t="s">
         <v>35</v>
@@ -5517,7 +5517,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J81" s="48" t="s">
         <v>136</v>
@@ -5573,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J82" s="47" t="s">
         <v>20</v>
@@ -5627,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J83" s="47" t="s">
         <v>27</v>
@@ -5681,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J84" s="47" t="s">
         <v>34</v>
@@ -5729,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J85" s="49" t="s">
         <v>35</v>
@@ -5777,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J86" s="48" t="s">
         <v>136</v>
@@ -5833,7 +5833,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J87" s="47" t="s">
         <v>20</v>
@@ -5887,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J88" s="47" t="s">
         <v>27</v>
@@ -5941,7 +5941,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J89" s="47" t="s">
         <v>34</v>
@@ -5989,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J90" s="49" t="s">
         <v>35</v>
@@ -6037,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="I91" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J91" s="47" t="s">
         <v>136</v>
@@ -6093,7 +6093,7 @@
         <v>0</v>
       </c>
       <c r="I92" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J92" s="47" t="s">
         <v>20</v>
@@ -6147,7 +6147,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J93" s="47" t="s">
         <v>27</v>
@@ -6201,7 +6201,7 @@
         <v>0</v>
       </c>
       <c r="I94" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J94" s="47" t="s">
         <v>34</v>
@@ -6249,7 +6249,7 @@
         <v>0</v>
       </c>
       <c r="I95" s="50">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J95" s="50" t="s">
         <v>35</v>
@@ -6280,12 +6280,12 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="O1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:R95 A4:P5 R4:R5">
+  <conditionalFormatting sqref="A10:R95 R4:R5 J4:P5 A4:H9 J6:R9">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:R3">
+  <conditionalFormatting sqref="A3:R3 I4:I9">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Setting inactive edges in Centre2Edge.m to make sure zero fluvial transport at edges between active and inactive cells (i.e. cells with depth > and < than SedThr).
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@210 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1017,7 +1017,126 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1325,10 +1444,10 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomRight" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1777,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="30">
         <v>0</v>
@@ -1691,7 +1810,7 @@
         <v>3</v>
       </c>
       <c r="M7" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N7" s="47">
         <v>2</v>
@@ -2068,7 +2187,7 @@
         <v>119</v>
       </c>
       <c r="B15" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="36">
         <v>4</v>
@@ -2328,7 +2447,7 @@
         <v>120</v>
       </c>
       <c r="B20" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="36">
         <v>3</v>
@@ -2588,7 +2707,7 @@
         <v>121</v>
       </c>
       <c r="B25" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="36">
         <v>3</v>
@@ -2836,7 +2955,7 @@
         <v>0.1</v>
       </c>
       <c r="N29" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O29" s="20"/>
       <c r="P29" s="7"/>
@@ -2844,37 +2963,37 @@
       <c r="R29" s="47"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B30" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" s="36">
-        <v>1</v>
-      </c>
-      <c r="D30" s="37">
-        <v>0</v>
-      </c>
-      <c r="E30" s="37">
-        <v>0</v>
-      </c>
-      <c r="F30" s="37">
-        <v>0</v>
-      </c>
-      <c r="G30" s="52">
-        <v>3</v>
-      </c>
-      <c r="H30" s="38">
-        <v>0</v>
-      </c>
-      <c r="I30" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="J30" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="31">
+        <v>0</v>
+      </c>
+      <c r="E30" s="31">
+        <v>0</v>
+      </c>
+      <c r="F30" s="31">
+        <v>0</v>
+      </c>
+      <c r="G30" s="40">
+        <v>3</v>
+      </c>
+      <c r="H30" s="32">
+        <v>0</v>
+      </c>
+      <c r="I30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="J30" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="K30" s="49">
+      <c r="K30" s="47">
         <v>212.5</v>
       </c>
       <c r="L30" s="6">
@@ -2883,13 +3002,13 @@
       <c r="M30" s="6">
         <v>0.1</v>
       </c>
-      <c r="N30" s="49">
-        <v>2</v>
-      </c>
-      <c r="O30" s="22"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="49"/>
+      <c r="N30" s="47">
+        <v>2</v>
+      </c>
+      <c r="O30" s="20"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="47"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
@@ -3108,7 +3227,7 @@
         <v>123</v>
       </c>
       <c r="B35" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="36">
         <v>1</v>
@@ -3368,7 +3487,7 @@
         <v>124</v>
       </c>
       <c r="B40" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="36">
         <v>2</v>
@@ -3628,7 +3747,7 @@
         <v>125</v>
       </c>
       <c r="B45" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="36">
         <v>2</v>
@@ -3888,7 +4007,7 @@
         <v>126</v>
       </c>
       <c r="B50" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="36">
         <v>2</v>
@@ -4148,7 +4267,7 @@
         <v>127</v>
       </c>
       <c r="B55" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" s="36">
         <v>2</v>
@@ -4408,7 +4527,7 @@
         <v>128</v>
       </c>
       <c r="B60" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="36">
         <v>2</v>
@@ -4668,7 +4787,7 @@
         <v>129</v>
       </c>
       <c r="B65" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="36">
         <v>2</v>
@@ -4924,37 +5043,37 @@
       <c r="R69" s="47"/>
     </row>
     <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B70" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="C70" s="36">
-        <v>1</v>
-      </c>
-      <c r="D70" s="37">
-        <v>0</v>
-      </c>
-      <c r="E70" s="37">
-        <v>0</v>
-      </c>
-      <c r="F70" s="37">
-        <v>0</v>
-      </c>
-      <c r="G70" s="52">
+        <v>0</v>
+      </c>
+      <c r="C70" s="30">
+        <v>1</v>
+      </c>
+      <c r="D70" s="31">
+        <v>0</v>
+      </c>
+      <c r="E70" s="31">
+        <v>0</v>
+      </c>
+      <c r="F70" s="31">
+        <v>0</v>
+      </c>
+      <c r="G70" s="40">
         <v>4</v>
       </c>
-      <c r="H70" s="38">
-        <v>0</v>
-      </c>
-      <c r="I70" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="J70" s="49" t="s">
+      <c r="H70" s="32">
+        <v>0</v>
+      </c>
+      <c r="I70" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="J70" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="K70" s="49">
+      <c r="K70" s="47">
         <v>212.5</v>
       </c>
       <c r="L70" s="6">
@@ -4963,13 +5082,13 @@
       <c r="M70" s="6">
         <v>0.1</v>
       </c>
-      <c r="N70" s="49">
-        <v>2</v>
-      </c>
-      <c r="O70" s="22"/>
-      <c r="P70" s="19"/>
-      <c r="Q70" s="19"/>
-      <c r="R70" s="49"/>
+      <c r="N70" s="47">
+        <v>2</v>
+      </c>
+      <c r="O70" s="20"/>
+      <c r="P70" s="7"/>
+      <c r="Q70" s="7"/>
+      <c r="R70" s="47"/>
     </row>
     <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
@@ -5184,37 +5303,37 @@
       <c r="R74" s="47"/>
     </row>
     <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="5" t="s">
         <v>131</v>
       </c>
       <c r="B75" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="C75" s="36">
-        <v>1</v>
-      </c>
-      <c r="D75" s="37">
-        <v>0</v>
-      </c>
-      <c r="E75" s="37">
-        <v>0</v>
-      </c>
-      <c r="F75" s="37">
-        <v>0</v>
-      </c>
-      <c r="G75" s="52">
+        <v>0</v>
+      </c>
+      <c r="C75" s="30">
+        <v>1</v>
+      </c>
+      <c r="D75" s="31">
+        <v>0</v>
+      </c>
+      <c r="E75" s="31">
+        <v>0</v>
+      </c>
+      <c r="F75" s="31">
+        <v>0</v>
+      </c>
+      <c r="G75" s="40">
         <v>4</v>
       </c>
-      <c r="H75" s="38">
-        <v>1</v>
-      </c>
-      <c r="I75" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="J75" s="49" t="s">
+      <c r="H75" s="32">
+        <v>1</v>
+      </c>
+      <c r="I75" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="J75" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="K75" s="49">
+      <c r="K75" s="47">
         <v>212.5</v>
       </c>
       <c r="L75" s="6">
@@ -5223,13 +5342,13 @@
       <c r="M75" s="6">
         <v>0.1</v>
       </c>
-      <c r="N75" s="49">
-        <v>2</v>
-      </c>
-      <c r="O75" s="22"/>
-      <c r="P75" s="19"/>
-      <c r="Q75" s="19"/>
-      <c r="R75" s="49"/>
+      <c r="N75" s="47">
+        <v>2</v>
+      </c>
+      <c r="O75" s="20"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="47"/>
     </row>
     <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
@@ -5448,7 +5567,7 @@
         <v>132</v>
       </c>
       <c r="B80" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" s="36">
         <v>2</v>
@@ -5708,7 +5827,7 @@
         <v>133</v>
       </c>
       <c r="B85" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" s="36">
         <v>1</v>
@@ -5968,7 +6087,7 @@
         <v>134</v>
       </c>
       <c r="B90" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" s="36">
         <v>2</v>
@@ -6228,7 +6347,7 @@
         <v>135</v>
       </c>
       <c r="B95" s="50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" s="41">
         <v>2</v>
@@ -6280,24 +6399,29 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="O1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A10:R95 R4:R5 J4:P5 A4:H9 J6:R9">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="R4:R5 J4:P5 A8:H9 J6:R9 A4:A7 C4:H7 A10:R95">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:R3 I4:I9">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$B5&lt;&gt;TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B7">
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6306,6 +6430,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reverting to upwind bedload for sensitivity analysis as it results in better representation of overbank flow conditions (bank gets eroded using central)
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@211 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1017,119 +1017,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1447,7 +1335,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F97" sqref="F97"/>
+      <selection pane="bottomRight" activeCell="N87" sqref="N87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J3" s="47" t="s">
         <v>136</v>
@@ -1642,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J4" s="47" t="s">
         <v>20</v>
@@ -1696,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J5" s="47" t="s">
         <v>27</v>
@@ -1750,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J6" s="47" t="s">
         <v>34</v>
@@ -1765,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="N6" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O6" s="20"/>
       <c r="P6" s="7"/>
@@ -1798,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J7" s="47" t="s">
         <v>35</v>
@@ -1813,7 +1701,7 @@
         <v>15</v>
       </c>
       <c r="N7" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="7"/>
@@ -1846,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J8" s="47" t="s">
         <v>20</v>
@@ -1896,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="47" t="s">
         <v>20</v>
@@ -1946,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="49">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="47" t="s">
         <v>20</v>
@@ -1996,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J11" s="48" t="s">
         <v>136</v>
@@ -2011,7 +1899,7 @@
         <v>0.1</v>
       </c>
       <c r="N11" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O11" s="21" t="s">
         <v>137</v>
@@ -2052,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J12" s="47" t="s">
         <v>20</v>
@@ -2106,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J13" s="47" t="s">
         <v>27</v>
@@ -2160,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J14" s="47" t="s">
         <v>34</v>
@@ -2175,7 +2063,7 @@
         <v>0.01</v>
       </c>
       <c r="N14" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O14" s="20"/>
       <c r="P14" s="7"/>
@@ -2208,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J15" s="49" t="s">
         <v>35</v>
@@ -2256,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="48" t="s">
         <v>136</v>
@@ -2271,7 +2159,7 @@
         <v>0.1</v>
       </c>
       <c r="N16" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O16" s="21" t="s">
         <v>137</v>
@@ -2312,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J17" s="47" t="s">
         <v>20</v>
@@ -2366,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J18" s="47" t="s">
         <v>27</v>
@@ -2420,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J19" s="47" t="s">
         <v>34</v>
@@ -2435,7 +2323,7 @@
         <v>0.02</v>
       </c>
       <c r="N19" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O19" s="20"/>
       <c r="P19" s="7"/>
@@ -2468,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J20" s="49" t="s">
         <v>35</v>
@@ -2516,7 +2404,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J21" s="48" t="s">
         <v>136</v>
@@ -2531,7 +2419,7 @@
         <v>0.1</v>
       </c>
       <c r="N21" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O21" s="21" t="s">
         <v>137</v>
@@ -2572,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J22" s="47" t="s">
         <v>20</v>
@@ -2626,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J23" s="47" t="s">
         <v>27</v>
@@ -2680,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J24" s="47" t="s">
         <v>34</v>
@@ -2695,7 +2583,7 @@
         <v>0.02</v>
       </c>
       <c r="N24" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O24" s="20"/>
       <c r="P24" s="7"/>
@@ -2728,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J25" s="49" t="s">
         <v>35</v>
@@ -2776,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J26" s="48" t="s">
         <v>136</v>
@@ -2791,7 +2679,7 @@
         <v>0.1</v>
       </c>
       <c r="N26" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O26" s="21" t="s">
         <v>137</v>
@@ -2832,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J27" s="47" t="s">
         <v>20</v>
@@ -2886,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J28" s="47" t="s">
         <v>27</v>
@@ -2940,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J29" s="47" t="s">
         <v>34</v>
@@ -2988,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
         <v>35</v>
@@ -3003,7 +2891,7 @@
         <v>0.1</v>
       </c>
       <c r="N30" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O30" s="20"/>
       <c r="P30" s="7"/>
@@ -3036,7 +2924,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J31" s="48" t="s">
         <v>136</v>
@@ -3051,7 +2939,7 @@
         <v>0.1</v>
       </c>
       <c r="N31" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O31" s="21" t="s">
         <v>137</v>
@@ -3092,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J32" s="47" t="s">
         <v>20</v>
@@ -3146,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J33" s="47" t="s">
         <v>27</v>
@@ -3200,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J34" s="47" t="s">
         <v>34</v>
@@ -3215,7 +3103,7 @@
         <v>0.1</v>
       </c>
       <c r="N34" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O34" s="20"/>
       <c r="P34" s="7"/>
@@ -3248,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J35" s="49" t="s">
         <v>35</v>
@@ -3263,7 +3151,7 @@
         <v>0.1</v>
       </c>
       <c r="N35" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O35" s="22"/>
       <c r="P35" s="19"/>
@@ -3296,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J36" s="48" t="s">
         <v>136</v>
@@ -3311,7 +3199,7 @@
         <v>0.1</v>
       </c>
       <c r="N36" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O36" s="21" t="s">
         <v>137</v>
@@ -3352,7 +3240,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J37" s="47" t="s">
         <v>20</v>
@@ -3406,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J38" s="47" t="s">
         <v>27</v>
@@ -3460,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J39" s="47" t="s">
         <v>34</v>
@@ -3475,7 +3363,7 @@
         <v>0.1</v>
       </c>
       <c r="N39" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O39" s="20"/>
       <c r="P39" s="7"/>
@@ -3508,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J40" s="49" t="s">
         <v>35</v>
@@ -3523,7 +3411,7 @@
         <v>0.1</v>
       </c>
       <c r="N40" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O40" s="22"/>
       <c r="P40" s="19"/>
@@ -3556,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J41" s="48" t="s">
         <v>136</v>
@@ -3571,7 +3459,7 @@
         <v>0.1</v>
       </c>
       <c r="N41" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O41" s="21" t="s">
         <v>137</v>
@@ -3612,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J42" s="47" t="s">
         <v>20</v>
@@ -3666,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J43" s="47" t="s">
         <v>27</v>
@@ -3720,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J44" s="47" t="s">
         <v>34</v>
@@ -3735,7 +3623,7 @@
         <v>0.1</v>
       </c>
       <c r="N44" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O44" s="20"/>
       <c r="P44" s="7"/>
@@ -3768,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J45" s="49" t="s">
         <v>35</v>
@@ -3783,7 +3671,7 @@
         <v>0.1</v>
       </c>
       <c r="N45" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O45" s="22"/>
       <c r="P45" s="19"/>
@@ -3816,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J46" s="48" t="s">
         <v>136</v>
@@ -3831,7 +3719,7 @@
         <v>0.1</v>
       </c>
       <c r="N46" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O46" s="21" t="s">
         <v>137</v>
@@ -3872,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J47" s="47" t="s">
         <v>20</v>
@@ -3926,7 +3814,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J48" s="47" t="s">
         <v>27</v>
@@ -3980,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J49" s="47" t="s">
         <v>34</v>
@@ -3995,7 +3883,7 @@
         <v>0.1</v>
       </c>
       <c r="N49" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O49" s="20"/>
       <c r="P49" s="7"/>
@@ -4028,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J50" s="49" t="s">
         <v>35</v>
@@ -4043,7 +3931,7 @@
         <v>0.1</v>
       </c>
       <c r="N50" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O50" s="22"/>
       <c r="P50" s="19"/>
@@ -4076,7 +3964,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J51" s="48" t="s">
         <v>136</v>
@@ -4091,7 +3979,7 @@
         <v>0.1</v>
       </c>
       <c r="N51" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O51" s="21" t="s">
         <v>137</v>
@@ -4132,7 +4020,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J52" s="47" t="s">
         <v>20</v>
@@ -4186,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J53" s="47" t="s">
         <v>27</v>
@@ -4240,7 +4128,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J54" s="47" t="s">
         <v>34</v>
@@ -4255,7 +4143,7 @@
         <v>0.1</v>
       </c>
       <c r="N54" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O54" s="20"/>
       <c r="P54" s="7"/>
@@ -4288,7 +4176,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J55" s="49" t="s">
         <v>35</v>
@@ -4303,7 +4191,7 @@
         <v>0.1</v>
       </c>
       <c r="N55" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O55" s="22"/>
       <c r="P55" s="19"/>
@@ -4336,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J56" s="48" t="s">
         <v>136</v>
@@ -4351,7 +4239,7 @@
         <v>0.1</v>
       </c>
       <c r="N56" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O56" s="21" t="s">
         <v>137</v>
@@ -4392,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J57" s="47" t="s">
         <v>20</v>
@@ -4446,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J58" s="47" t="s">
         <v>27</v>
@@ -4500,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J59" s="47" t="s">
         <v>34</v>
@@ -4515,7 +4403,7 @@
         <v>0.1</v>
       </c>
       <c r="N59" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O59" s="20"/>
       <c r="P59" s="7"/>
@@ -4548,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J60" s="49" t="s">
         <v>35</v>
@@ -4563,7 +4451,7 @@
         <v>0.1</v>
       </c>
       <c r="N60" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O60" s="22"/>
       <c r="P60" s="19"/>
@@ -4596,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J61" s="48" t="s">
         <v>136</v>
@@ -4611,7 +4499,7 @@
         <v>0.1</v>
       </c>
       <c r="N61" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O61" s="21" t="s">
         <v>137</v>
@@ -4652,7 +4540,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J62" s="47" t="s">
         <v>20</v>
@@ -4706,7 +4594,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J63" s="47" t="s">
         <v>27</v>
@@ -4760,7 +4648,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J64" s="47" t="s">
         <v>34</v>
@@ -4775,7 +4663,7 @@
         <v>0.1</v>
       </c>
       <c r="N64" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O64" s="20"/>
       <c r="P64" s="7"/>
@@ -4808,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J65" s="49" t="s">
         <v>35</v>
@@ -4823,7 +4711,7 @@
         <v>0.1</v>
       </c>
       <c r="N65" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O65" s="22"/>
       <c r="P65" s="19"/>
@@ -4856,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J66" s="48" t="s">
         <v>136</v>
@@ -4871,7 +4759,7 @@
         <v>0.1</v>
       </c>
       <c r="N66" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O66" s="21" t="s">
         <v>137</v>
@@ -4912,7 +4800,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J67" s="47" t="s">
         <v>20</v>
@@ -4966,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J68" s="47" t="s">
         <v>27</v>
@@ -5020,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J69" s="47" t="s">
         <v>34</v>
@@ -5035,7 +4923,7 @@
         <v>0.1</v>
       </c>
       <c r="N69" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O69" s="20"/>
       <c r="P69" s="7"/>
@@ -5068,7 +4956,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J70" s="47" t="s">
         <v>35</v>
@@ -5083,7 +4971,7 @@
         <v>0.1</v>
       </c>
       <c r="N70" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O70" s="20"/>
       <c r="P70" s="7"/>
@@ -5116,7 +5004,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J71" s="48" t="s">
         <v>136</v>
@@ -5131,7 +5019,7 @@
         <v>0.1</v>
       </c>
       <c r="N71" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O71" s="21" t="s">
         <v>137</v>
@@ -5172,7 +5060,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J72" s="47" t="s">
         <v>20</v>
@@ -5226,7 +5114,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J73" s="47" t="s">
         <v>27</v>
@@ -5280,7 +5168,7 @@
         <v>1</v>
       </c>
       <c r="I74" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J74" s="47" t="s">
         <v>34</v>
@@ -5295,7 +5183,7 @@
         <v>0.1</v>
       </c>
       <c r="N74" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O74" s="20"/>
       <c r="P74" s="7"/>
@@ -5328,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="I75" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J75" s="47" t="s">
         <v>35</v>
@@ -5343,7 +5231,7 @@
         <v>0.1</v>
       </c>
       <c r="N75" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O75" s="20"/>
       <c r="P75" s="7"/>
@@ -5376,7 +5264,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J76" s="48" t="s">
         <v>136</v>
@@ -5391,7 +5279,7 @@
         <v>0.1</v>
       </c>
       <c r="N76" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O76" s="21" t="s">
         <v>137</v>
@@ -5432,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="I77" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J77" s="47" t="s">
         <v>20</v>
@@ -5486,7 +5374,7 @@
         <v>1</v>
       </c>
       <c r="I78" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J78" s="47" t="s">
         <v>27</v>
@@ -5540,7 +5428,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J79" s="47" t="s">
         <v>34</v>
@@ -5555,7 +5443,7 @@
         <v>0.1</v>
       </c>
       <c r="N79" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O79" s="20"/>
       <c r="P79" s="7"/>
@@ -5588,7 +5476,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J80" s="49" t="s">
         <v>35</v>
@@ -5603,7 +5491,7 @@
         <v>0.1</v>
       </c>
       <c r="N80" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O80" s="22"/>
       <c r="P80" s="19"/>
@@ -5636,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J81" s="48" t="s">
         <v>136</v>
@@ -5651,7 +5539,7 @@
         <v>1</v>
       </c>
       <c r="N81" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O81" s="21" t="s">
         <v>137</v>
@@ -5692,7 +5580,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J82" s="47" t="s">
         <v>20</v>
@@ -5746,7 +5634,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J83" s="47" t="s">
         <v>27</v>
@@ -5800,7 +5688,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J84" s="47" t="s">
         <v>34</v>
@@ -5815,7 +5703,7 @@
         <v>1</v>
       </c>
       <c r="N84" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O84" s="20"/>
       <c r="P84" s="7"/>
@@ -5848,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J85" s="49" t="s">
         <v>35</v>
@@ -5863,7 +5751,7 @@
         <v>1</v>
       </c>
       <c r="N85" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O85" s="22"/>
       <c r="P85" s="19"/>
@@ -5896,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J86" s="48" t="s">
         <v>136</v>
@@ -5911,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="N86" s="48">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O86" s="21" t="s">
         <v>137</v>
@@ -5952,7 +5840,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J87" s="47" t="s">
         <v>20</v>
@@ -6006,7 +5894,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J88" s="47" t="s">
         <v>27</v>
@@ -6060,7 +5948,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J89" s="47" t="s">
         <v>34</v>
@@ -6075,7 +5963,7 @@
         <v>1</v>
       </c>
       <c r="N89" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O89" s="20"/>
       <c r="P89" s="7"/>
@@ -6108,7 +5996,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J90" s="49" t="s">
         <v>35</v>
@@ -6123,7 +6011,7 @@
         <v>1</v>
       </c>
       <c r="N90" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O90" s="22"/>
       <c r="P90" s="19"/>
@@ -6156,7 +6044,7 @@
         <v>0</v>
       </c>
       <c r="I91" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J91" s="47" t="s">
         <v>136</v>
@@ -6171,7 +6059,7 @@
         <v>1</v>
       </c>
       <c r="N91" s="47">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="O91" s="20" t="s">
         <v>137</v>
@@ -6212,7 +6100,7 @@
         <v>0</v>
       </c>
       <c r="I92" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J92" s="47" t="s">
         <v>20</v>
@@ -6266,7 +6154,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J93" s="47" t="s">
         <v>27</v>
@@ -6320,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="I94" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J94" s="47" t="s">
         <v>34</v>
@@ -6335,7 +6223,7 @@
         <v>1</v>
       </c>
       <c r="N94" s="47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O94" s="20"/>
       <c r="P94" s="7"/>
@@ -6368,7 +6256,7 @@
         <v>0</v>
       </c>
       <c r="I95" s="50">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J95" s="50" t="s">
         <v>35</v>
@@ -6383,7 +6271,7 @@
         <v>1</v>
       </c>
       <c r="N95" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O95" s="23"/>
       <c r="P95" s="10"/>
@@ -6400,27 +6288,27 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="R4:R5 J4:P5 A8:H9 J6:R9 A4:A7 C4:H7 A10:R95">
-    <cfRule type="expression" dxfId="20" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:R3 I4:I9">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B5&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B7">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Radius of calibration and validation scenarios adjusted based on accurate measurement from GIS
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@213 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1350,10 +1350,10 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1513,7 @@
         <v>118</v>
       </c>
       <c r="P3" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q3" s="5">
         <v>210.5</v>
@@ -1569,7 +1569,7 @@
         <v>38</v>
       </c>
       <c r="P4" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q4" s="5">
         <v>210.5</v>
@@ -1623,7 +1623,7 @@
         <v>39</v>
       </c>
       <c r="P5" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q5" s="5">
         <v>210.5</v>
@@ -1875,7 +1875,7 @@
         <v>118</v>
       </c>
       <c r="P10" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q10" s="14">
         <v>210.5</v>
@@ -1931,7 +1931,7 @@
         <v>38</v>
       </c>
       <c r="P11" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q11" s="5">
         <v>210.5</v>
@@ -1985,7 +1985,7 @@
         <v>39</v>
       </c>
       <c r="P12" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q12" s="5">
         <v>210.5</v>
@@ -2087,7 +2087,7 @@
         <v>118</v>
       </c>
       <c r="P14" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q14" s="14">
         <v>210.5</v>
@@ -2143,7 +2143,7 @@
         <v>38</v>
       </c>
       <c r="P15" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q15" s="5">
         <v>210.5</v>
@@ -2197,7 +2197,7 @@
         <v>39</v>
       </c>
       <c r="P16" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q16" s="5">
         <v>210.5</v>
@@ -2299,7 +2299,7 @@
         <v>118</v>
       </c>
       <c r="P18" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q18" s="14">
         <v>210.5</v>
@@ -2355,7 +2355,7 @@
         <v>38</v>
       </c>
       <c r="P19" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q19" s="5">
         <v>210.5</v>
@@ -2409,7 +2409,7 @@
         <v>39</v>
       </c>
       <c r="P20" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q20" s="5">
         <v>210.5</v>
@@ -2511,7 +2511,7 @@
         <v>118</v>
       </c>
       <c r="P22" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q22" s="14">
         <v>210.5</v>
@@ -2567,7 +2567,7 @@
         <v>38</v>
       </c>
       <c r="P23" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q23" s="5">
         <v>210.5</v>
@@ -2621,7 +2621,7 @@
         <v>39</v>
       </c>
       <c r="P24" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q24" s="5">
         <v>210.5</v>
@@ -2723,7 +2723,7 @@
         <v>118</v>
       </c>
       <c r="P26" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q26" s="14">
         <v>210.5</v>
@@ -2779,7 +2779,7 @@
         <v>38</v>
       </c>
       <c r="P27" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q27" s="5">
         <v>210.5</v>
@@ -2833,7 +2833,7 @@
         <v>39</v>
       </c>
       <c r="P28" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q28" s="5">
         <v>210.5</v>
@@ -2935,7 +2935,7 @@
         <v>118</v>
       </c>
       <c r="P30" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q30" s="14">
         <v>210.5</v>
@@ -2991,7 +2991,7 @@
         <v>38</v>
       </c>
       <c r="P31" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q31" s="5">
         <v>210.5</v>
@@ -3045,7 +3045,7 @@
         <v>39</v>
       </c>
       <c r="P32" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q32" s="5">
         <v>210.5</v>
@@ -3147,7 +3147,7 @@
         <v>118</v>
       </c>
       <c r="P34" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q34" s="14">
         <v>210.5</v>
@@ -3203,7 +3203,7 @@
         <v>38</v>
       </c>
       <c r="P35" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q35" s="5">
         <v>210.5</v>
@@ -3248,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="4">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N36" s="44">
         <v>20</v>
@@ -3257,7 +3257,7 @@
         <v>39</v>
       </c>
       <c r="P36" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q36" s="5">
         <v>210.5</v>
@@ -3359,7 +3359,7 @@
         <v>118</v>
       </c>
       <c r="P38" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q38" s="14">
         <v>210.5</v>
@@ -3415,7 +3415,7 @@
         <v>38</v>
       </c>
       <c r="P39" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q39" s="5">
         <v>210.5</v>
@@ -3469,7 +3469,7 @@
         <v>39</v>
       </c>
       <c r="P40" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q40" s="5">
         <v>210.5</v>
@@ -3571,7 +3571,7 @@
         <v>118</v>
       </c>
       <c r="P42" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q42" s="14">
         <v>210.5</v>
@@ -3627,7 +3627,7 @@
         <v>38</v>
       </c>
       <c r="P43" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q43" s="5">
         <v>210.5</v>
@@ -3672,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="4">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N44" s="44">
         <v>20</v>
@@ -3681,7 +3681,7 @@
         <v>39</v>
       </c>
       <c r="P44" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q44" s="5">
         <v>210.5</v>
@@ -3783,7 +3783,7 @@
         <v>118</v>
       </c>
       <c r="P46" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q46" s="14">
         <v>210.5</v>
@@ -3839,7 +3839,7 @@
         <v>38</v>
       </c>
       <c r="P47" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q47" s="5">
         <v>210.5</v>
@@ -3893,7 +3893,7 @@
         <v>39</v>
       </c>
       <c r="P48" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q48" s="5">
         <v>210.5</v>
@@ -3995,7 +3995,7 @@
         <v>118</v>
       </c>
       <c r="P50" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q50" s="14">
         <v>210.5</v>
@@ -4051,7 +4051,7 @@
         <v>38</v>
       </c>
       <c r="P51" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q51" s="5">
         <v>210.5</v>
@@ -4105,7 +4105,7 @@
         <v>39</v>
       </c>
       <c r="P52" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q52" s="5">
         <v>210.5</v>
@@ -4207,7 +4207,7 @@
         <v>118</v>
       </c>
       <c r="P54" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q54" s="14">
         <v>210.5</v>
@@ -4263,7 +4263,7 @@
         <v>38</v>
       </c>
       <c r="P55" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q55" s="5">
         <v>210.5</v>
@@ -4317,7 +4317,7 @@
         <v>39</v>
       </c>
       <c r="P56" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q56" s="5">
         <v>210.5</v>
@@ -4419,7 +4419,7 @@
         <v>118</v>
       </c>
       <c r="P58" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q58" s="14">
         <v>210.5</v>
@@ -4475,7 +4475,7 @@
         <v>38</v>
       </c>
       <c r="P59" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q59" s="5">
         <v>210.5</v>
@@ -4529,7 +4529,7 @@
         <v>39</v>
       </c>
       <c r="P60" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q60" s="5">
         <v>210.5</v>
@@ -4631,7 +4631,7 @@
         <v>118</v>
       </c>
       <c r="P62" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q62" s="14">
         <v>210.5</v>
@@ -4687,7 +4687,7 @@
         <v>38</v>
       </c>
       <c r="P63" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q63" s="5">
         <v>210.5</v>
@@ -4741,7 +4741,7 @@
         <v>39</v>
       </c>
       <c r="P64" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q64" s="5">
         <v>210.5</v>
@@ -4843,7 +4843,7 @@
         <v>118</v>
       </c>
       <c r="P66" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q66" s="14">
         <v>210.5</v>
@@ -4899,7 +4899,7 @@
         <v>38</v>
       </c>
       <c r="P67" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q67" s="5">
         <v>210.5</v>
@@ -4953,7 +4953,7 @@
         <v>39</v>
       </c>
       <c r="P68" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q68" s="5">
         <v>210.5</v>
@@ -5055,7 +5055,7 @@
         <v>118</v>
       </c>
       <c r="P70" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q70" s="14">
         <v>210.5</v>
@@ -5111,7 +5111,7 @@
         <v>38</v>
       </c>
       <c r="P71" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q71" s="5">
         <v>210.5</v>
@@ -5165,7 +5165,7 @@
         <v>39</v>
       </c>
       <c r="P72" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q72" s="5">
         <v>210.5</v>
@@ -5267,7 +5267,7 @@
         <v>118</v>
       </c>
       <c r="P74" s="14">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q74" s="14">
         <v>210.5</v>
@@ -5323,7 +5323,7 @@
         <v>38</v>
       </c>
       <c r="P75" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q75" s="5">
         <v>210.5</v>
@@ -5377,7 +5377,7 @@
         <v>39</v>
       </c>
       <c r="P76" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q76" s="5">
         <v>210.5</v>
@@ -5479,7 +5479,7 @@
         <v>118</v>
       </c>
       <c r="P78" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q78" s="5">
         <v>210.5</v>
@@ -5535,7 +5535,7 @@
         <v>38</v>
       </c>
       <c r="P79" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q79" s="5">
         <v>210.5</v>
@@ -5589,7 +5589,7 @@
         <v>39</v>
       </c>
       <c r="P80" s="5">
-        <v>-160</v>
+        <v>-240</v>
       </c>
       <c r="Q80" s="5">
         <v>210.5</v>

</xml_diff>

<commit_message>
Added direction of bank position error to output (+ve = too much Bank Erosion, -ve = too little)
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@216 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BankErosion\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Research\BankErosionMatlab\Trunk\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Richard Measures: </t>
         </r>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>In some cases bounds have been adjusted for specific scenarios to improve calibration.</t>
         </r>
@@ -60,7 +60,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Richard Measures:</t>
         </r>
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Timestep reduced to try and improve stability</t>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="131">
   <si>
     <t>Stencil</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>Inputs\Selwyn_XS7_3m.csv</t>
-  </si>
-  <si>
-    <t>Inputs\Selwyn_XS7_1m.csv</t>
   </si>
   <si>
     <t>1a</t>
@@ -510,14 +507,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1350,10 +1347,10 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O42" sqref="O42"/>
+      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,13 +1433,13 @@
         <v>16</v>
       </c>
       <c r="I2" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J2" s="43" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>21</v>
@@ -1460,7 +1457,7 @@
         <v>37</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>4</v>
@@ -1468,10 +1465,10 @@
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="27">
         <v>0</v>
@@ -1495,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K3" s="44">
         <v>212.5</v>
@@ -1510,7 +1507,7 @@
         <v>120</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P3" s="5">
         <v>-240</v>
@@ -1524,10 +1521,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="27">
         <v>0</v>
@@ -1578,10 +1575,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1619,23 +1616,17 @@
       <c r="N5" s="44">
         <v>20</v>
       </c>
-      <c r="O5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O5" s="18"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -1680,10 +1671,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="27">
         <v>0</v>
@@ -1730,10 +1721,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="27">
         <v>0</v>
@@ -1780,10 +1771,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="33">
         <v>0</v>
@@ -1825,15 +1816,15 @@
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="30">
         <v>4</v>
@@ -1857,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K10" s="45">
         <v>212.5</v>
@@ -1872,7 +1863,7 @@
         <v>120</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P10" s="14">
         <v>-240</v>
@@ -1886,10 +1877,10 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="27">
         <v>4</v>
@@ -1940,10 +1931,10 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="27">
         <v>4</v>
@@ -1981,23 +1972,17 @@
       <c r="N12" s="44">
         <v>20</v>
       </c>
-      <c r="O12" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O12" s="18"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
       <c r="R12" s="44"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="27">
         <v>4</v>
@@ -2042,10 +2027,10 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="30">
         <v>3</v>
@@ -2069,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K14" s="45">
         <v>212.5</v>
@@ -2084,7 +2069,7 @@
         <v>120</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P14" s="14">
         <v>-240</v>
@@ -2098,10 +2083,10 @@
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="27">
         <v>3</v>
@@ -2152,10 +2137,10 @@
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="27">
         <v>3</v>
@@ -2193,23 +2178,17 @@
       <c r="N16" s="44">
         <v>20</v>
       </c>
-      <c r="O16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O16" s="18"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="44"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="27">
         <v>3</v>
@@ -2254,10 +2233,10 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="30">
         <v>3</v>
@@ -2281,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K18" s="45">
         <v>212.5</v>
@@ -2296,7 +2275,7 @@
         <v>120</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P18" s="14">
         <v>-240</v>
@@ -2305,15 +2284,15 @@
         <v>210.5</v>
       </c>
       <c r="R18" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="27">
         <v>3</v>
@@ -2364,10 +2343,10 @@
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="27">
         <v>3</v>
@@ -2405,23 +2384,17 @@
       <c r="N20" s="44">
         <v>20</v>
       </c>
-      <c r="O20" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P20" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O20" s="18"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
       <c r="R20" s="44"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="27">
         <v>3</v>
@@ -2466,10 +2439,10 @@
     </row>
     <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="30">
         <v>1</v>
@@ -2493,7 +2466,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K22" s="45">
         <v>212.5</v>
@@ -2508,7 +2481,7 @@
         <v>120</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P22" s="14">
         <v>-240</v>
@@ -2522,10 +2495,10 @@
     </row>
     <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="27">
         <v>1</v>
@@ -2576,10 +2549,10 @@
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="27">
         <v>1</v>
@@ -2617,23 +2590,17 @@
       <c r="N24" s="44">
         <v>20</v>
       </c>
-      <c r="O24" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P24" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q24" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O24" s="18"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
       <c r="R24" s="44"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="27">
         <v>1</v>
@@ -2678,10 +2645,10 @@
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="30">
         <v>1</v>
@@ -2705,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K26" s="45">
         <v>212.5</v>
@@ -2720,7 +2687,7 @@
         <v>120</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P26" s="14">
         <v>-240</v>
@@ -2729,15 +2696,15 @@
         <v>210.5</v>
       </c>
       <c r="R26" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="27">
         <v>1</v>
@@ -2788,10 +2755,10 @@
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="27">
         <v>1</v>
@@ -2829,23 +2796,17 @@
       <c r="N28" s="44">
         <v>20</v>
       </c>
-      <c r="O28" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P28" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q28" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O28" s="18"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
       <c r="R28" s="44"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="27">
         <v>1</v>
@@ -2890,10 +2851,10 @@
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="30">
         <v>2</v>
@@ -2917,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K30" s="45">
         <v>212.5</v>
@@ -2932,7 +2893,7 @@
         <v>120</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P30" s="14">
         <v>-240</v>
@@ -2946,10 +2907,10 @@
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="27">
         <v>2</v>
@@ -3000,10 +2961,10 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="27">
         <v>2</v>
@@ -3041,23 +3002,17 @@
       <c r="N32" s="44">
         <v>20</v>
       </c>
-      <c r="O32" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P32" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q32" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O32" s="18"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
       <c r="R32" s="44"/>
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="27">
         <v>2</v>
@@ -3102,10 +3057,10 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="30">
         <v>2</v>
@@ -3129,7 +3084,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K34" s="45">
         <v>212.5</v>
@@ -3144,7 +3099,7 @@
         <v>120</v>
       </c>
       <c r="O34" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P34" s="14">
         <v>-240</v>
@@ -3153,15 +3108,15 @@
         <v>210.5</v>
       </c>
       <c r="R34" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="27">
         <v>2</v>
@@ -3212,10 +3167,10 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B36" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="27">
         <v>2</v>
@@ -3253,23 +3208,17 @@
       <c r="N36" s="44">
         <v>20</v>
       </c>
-      <c r="O36" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P36" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q36" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O36" s="18"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
       <c r="R36" s="44"/>
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" s="27">
         <v>2</v>
@@ -3314,10 +3263,10 @@
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="30">
         <v>2</v>
@@ -3341,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K38" s="45">
         <v>212.5</v>
@@ -3356,7 +3305,7 @@
         <v>120</v>
       </c>
       <c r="O38" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P38" s="14">
         <v>-240</v>
@@ -3365,15 +3314,15 @@
         <v>210.5</v>
       </c>
       <c r="R38" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="27">
         <v>2</v>
@@ -3424,10 +3373,10 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="27">
         <v>2</v>
@@ -3465,23 +3414,17 @@
       <c r="N40" s="44">
         <v>20</v>
       </c>
-      <c r="O40" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P40" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q40" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O40" s="18"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
       <c r="R40" s="44"/>
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="27">
         <v>2</v>
@@ -3526,10 +3469,10 @@
     </row>
     <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="30">
         <v>2</v>
@@ -3553,7 +3496,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K42" s="45">
         <v>212.5</v>
@@ -3568,7 +3511,7 @@
         <v>120</v>
       </c>
       <c r="O42" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P42" s="14">
         <v>-240</v>
@@ -3577,15 +3520,15 @@
         <v>210.5</v>
       </c>
       <c r="R42" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="27">
         <v>2</v>
@@ -3636,10 +3579,10 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="27">
         <v>2</v>
@@ -3677,23 +3620,17 @@
       <c r="N44" s="44">
         <v>20</v>
       </c>
-      <c r="O44" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P44" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q44" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O44" s="18"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
       <c r="R44" s="44"/>
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="27">
         <v>2</v>
@@ -3738,7 +3675,7 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" s="45" t="b">
         <v>1</v>
@@ -3765,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K46" s="45">
         <v>212.5</v>
@@ -3780,7 +3717,7 @@
         <v>120</v>
       </c>
       <c r="O46" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P46" s="14">
         <v>-240</v>
@@ -3789,15 +3726,15 @@
         <v>210.5</v>
       </c>
       <c r="R46" s="45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="27">
         <v>2</v>
@@ -3848,10 +3785,10 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="27">
         <v>2</v>
@@ -3889,23 +3826,17 @@
       <c r="N48" s="44">
         <v>20</v>
       </c>
-      <c r="O48" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P48" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q48" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O48" s="18"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
       <c r="R48" s="44"/>
     </row>
     <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B49" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" s="27">
         <v>2</v>
@@ -3950,10 +3881,10 @@
     </row>
     <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="30">
         <v>2</v>
@@ -3977,7 +3908,7 @@
         <v>1</v>
       </c>
       <c r="J50" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K50" s="45">
         <v>212.5</v>
@@ -3992,7 +3923,7 @@
         <v>120</v>
       </c>
       <c r="O50" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P50" s="14">
         <v>-240</v>
@@ -4001,15 +3932,15 @@
         <v>210.5</v>
       </c>
       <c r="R50" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="27">
         <v>2</v>
@@ -4060,10 +3991,10 @@
     </row>
     <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" s="27">
         <v>2</v>
@@ -4101,23 +4032,17 @@
       <c r="N52" s="44">
         <v>20</v>
       </c>
-      <c r="O52" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P52" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q52" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O52" s="18"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
       <c r="R52" s="44"/>
     </row>
     <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" s="27">
         <v>2</v>
@@ -4162,10 +4087,10 @@
     </row>
     <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B54" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="30">
         <v>1</v>
@@ -4189,7 +4114,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K54" s="45">
         <v>212.5</v>
@@ -4204,7 +4129,7 @@
         <v>120</v>
       </c>
       <c r="O54" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P54" s="14">
         <v>-240</v>
@@ -4218,10 +4143,10 @@
     </row>
     <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B55" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" s="27">
         <v>1</v>
@@ -4272,10 +4197,10 @@
     </row>
     <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="27">
         <v>1</v>
@@ -4313,23 +4238,17 @@
       <c r="N56" s="44">
         <v>20</v>
       </c>
-      <c r="O56" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P56" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q56" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O56" s="18"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
       <c r="R56" s="44"/>
     </row>
     <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B57" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" s="27">
         <v>1</v>
@@ -4374,10 +4293,10 @@
     </row>
     <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="30">
         <v>1</v>
@@ -4401,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K58" s="45">
         <v>212.5</v>
@@ -4416,7 +4335,7 @@
         <v>120</v>
       </c>
       <c r="O58" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P58" s="14">
         <v>-240</v>
@@ -4430,10 +4349,10 @@
     </row>
     <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" s="27">
         <v>1</v>
@@ -4484,10 +4403,10 @@
     </row>
     <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="27">
         <v>1</v>
@@ -4520,28 +4439,22 @@
         <v>0</v>
       </c>
       <c r="M60" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N60" s="44">
         <v>20</v>
       </c>
-      <c r="O60" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P60" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q60" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O60" s="18"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
       <c r="R60" s="44"/>
     </row>
     <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B61" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" s="27">
         <v>1</v>
@@ -4586,10 +4499,10 @@
     </row>
     <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B62" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" s="30">
         <v>2</v>
@@ -4613,7 +4526,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K62" s="45">
         <v>212.5</v>
@@ -4628,7 +4541,7 @@
         <v>120</v>
       </c>
       <c r="O62" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P62" s="14">
         <v>-240</v>
@@ -4642,10 +4555,10 @@
     </row>
     <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B63" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" s="27">
         <v>2</v>
@@ -4696,10 +4609,10 @@
     </row>
     <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B64" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" s="27">
         <v>2</v>
@@ -4732,28 +4645,22 @@
         <v>0</v>
       </c>
       <c r="M64" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N64" s="44">
         <v>20</v>
       </c>
-      <c r="O64" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P64" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q64" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O64" s="18"/>
+      <c r="P64" s="5"/>
+      <c r="Q64" s="5"/>
       <c r="R64" s="44"/>
     </row>
     <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B65" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="27">
         <v>2</v>
@@ -4798,10 +4705,10 @@
     </row>
     <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="30">
         <v>1</v>
@@ -4825,7 +4732,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K66" s="45">
         <v>212.5</v>
@@ -4840,7 +4747,7 @@
         <v>120</v>
       </c>
       <c r="O66" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P66" s="14">
         <v>-240</v>
@@ -4854,10 +4761,10 @@
     </row>
     <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B67" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" s="27">
         <v>1</v>
@@ -4908,10 +4815,10 @@
     </row>
     <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B68" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68" s="27">
         <v>1</v>
@@ -4949,23 +4856,17 @@
       <c r="N68" s="44">
         <v>20</v>
       </c>
-      <c r="O68" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P68" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q68" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O68" s="18"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
       <c r="R68" s="44"/>
     </row>
     <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B69" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" s="27">
         <v>1</v>
@@ -5010,10 +4911,10 @@
     </row>
     <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" s="30">
         <v>2</v>
@@ -5037,7 +4938,7 @@
         <v>1</v>
       </c>
       <c r="J70" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K70" s="45">
         <v>212.5</v>
@@ -5052,7 +4953,7 @@
         <v>120</v>
       </c>
       <c r="O70" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P70" s="14">
         <v>-240</v>
@@ -5066,10 +4967,10 @@
     </row>
     <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" s="27">
         <v>2</v>
@@ -5120,10 +5021,10 @@
     </row>
     <row r="72" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" s="27">
         <v>2</v>
@@ -5161,23 +5062,17 @@
       <c r="N72" s="44">
         <v>20</v>
       </c>
-      <c r="O72" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P72" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q72" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O72" s="18"/>
+      <c r="P72" s="5"/>
+      <c r="Q72" s="5"/>
       <c r="R72" s="44"/>
     </row>
     <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B73" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" s="27">
         <v>2</v>
@@ -5222,10 +5117,10 @@
     </row>
     <row r="74" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B74" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74" s="30">
         <v>2</v>
@@ -5249,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K74" s="45">
         <v>212.5</v>
@@ -5264,7 +5159,7 @@
         <v>120</v>
       </c>
       <c r="O74" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P74" s="14">
         <v>-240</v>
@@ -5278,10 +5173,10 @@
     </row>
     <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B75" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" s="27">
         <v>2</v>
@@ -5332,10 +5227,10 @@
     </row>
     <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B76" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" s="27">
         <v>2</v>
@@ -5373,23 +5268,17 @@
       <c r="N76" s="44">
         <v>20</v>
       </c>
-      <c r="O76" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P76" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q76" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O76" s="18"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
       <c r="R76" s="44"/>
     </row>
     <row r="77" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B77" s="46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="33">
         <v>2</v>
@@ -5434,10 +5323,10 @@
     </row>
     <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B78" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" s="27">
         <v>3</v>
@@ -5461,7 +5350,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K78" s="44">
         <v>212.5</v>
@@ -5476,7 +5365,7 @@
         <v>120</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P78" s="5">
         <v>-240</v>
@@ -5485,15 +5374,15 @@
         <v>210.5</v>
       </c>
       <c r="R78" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" s="27">
         <v>3</v>
@@ -5544,10 +5433,10 @@
     </row>
     <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B80" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" s="27">
         <v>3</v>
@@ -5585,23 +5474,17 @@
       <c r="N80" s="44">
         <v>20</v>
       </c>
-      <c r="O80" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P80" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q80" s="5">
-        <v>210.5</v>
-      </c>
+      <c r="O80" s="18"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
       <c r="R80" s="5"/>
     </row>
     <row r="81" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B81" s="47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" s="38">
         <v>3</v>

</xml_diff>

<commit_message>
Improving optimisation plot to show +/- or error.
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@217 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1347,10 +1347,10 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1468,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="27">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="27">
         <v>0</v>
@@ -1578,7 +1578,7 @@
         <v>113</v>
       </c>
       <c r="B5" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1626,7 +1626,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -1674,7 +1674,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="27">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>48</v>
       </c>
       <c r="B8" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="27">
         <v>0</v>
@@ -1774,7 +1774,7 @@
         <v>114</v>
       </c>
       <c r="B9" s="46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="33">
         <v>0</v>
@@ -1824,7 +1824,7 @@
         <v>43</v>
       </c>
       <c r="B10" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="30">
         <v>4</v>
@@ -1880,7 +1880,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="27">
         <v>4</v>
@@ -1934,7 +1934,7 @@
         <v>110</v>
       </c>
       <c r="B12" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="27">
         <v>4</v>
@@ -1982,7 +1982,7 @@
         <v>111</v>
       </c>
       <c r="B13" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="27">
         <v>4</v>
@@ -2030,7 +2030,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="30">
         <v>3</v>
@@ -2086,7 +2086,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="27">
         <v>3</v>
@@ -2140,7 +2140,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="27">
         <v>3</v>
@@ -2188,7 +2188,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="27">
         <v>3</v>
@@ -2236,7 +2236,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="30">
         <v>3</v>
@@ -2292,7 +2292,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="27">
         <v>3</v>
@@ -2346,7 +2346,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="27">
         <v>3</v>
@@ -2394,7 +2394,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="27">
         <v>3</v>
@@ -2442,7 +2442,7 @@
         <v>54</v>
       </c>
       <c r="B22" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="30">
         <v>1</v>
@@ -2498,7 +2498,7 @@
         <v>55</v>
       </c>
       <c r="B23" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="27">
         <v>1</v>
@@ -2552,7 +2552,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="27">
         <v>1</v>
@@ -2600,7 +2600,7 @@
         <v>57</v>
       </c>
       <c r="B25" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="27">
         <v>1</v>
@@ -2648,7 +2648,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="30">
         <v>1</v>
@@ -2704,7 +2704,7 @@
         <v>59</v>
       </c>
       <c r="B27" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="27">
         <v>1</v>
@@ -2758,7 +2758,7 @@
         <v>96</v>
       </c>
       <c r="B28" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="27">
         <v>1</v>
@@ -2806,7 +2806,7 @@
         <v>97</v>
       </c>
       <c r="B29" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="27">
         <v>1</v>
@@ -2854,7 +2854,7 @@
         <v>60</v>
       </c>
       <c r="B30" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="30">
         <v>2</v>
@@ -2910,7 +2910,7 @@
         <v>61</v>
       </c>
       <c r="B31" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="27">
         <v>2</v>
@@ -2964,7 +2964,7 @@
         <v>108</v>
       </c>
       <c r="B32" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="27">
         <v>2</v>
@@ -3012,7 +3012,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="27">
         <v>2</v>
@@ -3060,7 +3060,7 @@
         <v>62</v>
       </c>
       <c r="B34" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="30">
         <v>2</v>
@@ -3116,7 +3116,7 @@
         <v>63</v>
       </c>
       <c r="B35" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="27">
         <v>2</v>
@@ -3170,7 +3170,7 @@
         <v>106</v>
       </c>
       <c r="B36" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="27">
         <v>2</v>
@@ -3218,7 +3218,7 @@
         <v>107</v>
       </c>
       <c r="B37" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="27">
         <v>2</v>
@@ -3266,7 +3266,7 @@
         <v>64</v>
       </c>
       <c r="B38" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="30">
         <v>2</v>
@@ -3322,7 +3322,7 @@
         <v>65</v>
       </c>
       <c r="B39" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="27">
         <v>2</v>
@@ -3376,7 +3376,7 @@
         <v>104</v>
       </c>
       <c r="B40" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="27">
         <v>2</v>
@@ -3424,7 +3424,7 @@
         <v>105</v>
       </c>
       <c r="B41" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="27">
         <v>2</v>
@@ -3472,7 +3472,7 @@
         <v>66</v>
       </c>
       <c r="B42" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="30">
         <v>2</v>
@@ -3528,7 +3528,7 @@
         <v>67</v>
       </c>
       <c r="B43" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" s="27">
         <v>2</v>
@@ -3582,7 +3582,7 @@
         <v>102</v>
       </c>
       <c r="B44" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="27">
         <v>2</v>
@@ -3630,7 +3630,7 @@
         <v>103</v>
       </c>
       <c r="B45" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="27">
         <v>2</v>
@@ -3734,7 +3734,7 @@
         <v>69</v>
       </c>
       <c r="B47" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="27">
         <v>2</v>
@@ -3788,7 +3788,7 @@
         <v>100</v>
       </c>
       <c r="B48" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="27">
         <v>2</v>
@@ -3836,7 +3836,7 @@
         <v>101</v>
       </c>
       <c r="B49" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="27">
         <v>2</v>
@@ -3884,7 +3884,7 @@
         <v>70</v>
       </c>
       <c r="B50" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" s="30">
         <v>2</v>
@@ -3940,7 +3940,7 @@
         <v>71</v>
       </c>
       <c r="B51" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="27">
         <v>2</v>
@@ -3994,7 +3994,7 @@
         <v>98</v>
       </c>
       <c r="B52" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" s="27">
         <v>2</v>
@@ -4042,7 +4042,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="27">
         <v>2</v>
@@ -4090,7 +4090,7 @@
         <v>72</v>
       </c>
       <c r="B54" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="30">
         <v>1</v>
@@ -4146,7 +4146,7 @@
         <v>73</v>
       </c>
       <c r="B55" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" s="27">
         <v>1</v>
@@ -4200,7 +4200,7 @@
         <v>90</v>
       </c>
       <c r="B56" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56" s="27">
         <v>1</v>
@@ -4248,7 +4248,7 @@
         <v>91</v>
       </c>
       <c r="B57" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" s="27">
         <v>1</v>
@@ -4296,7 +4296,7 @@
         <v>74</v>
       </c>
       <c r="B58" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" s="30">
         <v>1</v>
@@ -4352,7 +4352,7 @@
         <v>75</v>
       </c>
       <c r="B59" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" s="27">
         <v>1</v>
@@ -4406,7 +4406,7 @@
         <v>94</v>
       </c>
       <c r="B60" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="27">
         <v>1</v>
@@ -4454,7 +4454,7 @@
         <v>95</v>
       </c>
       <c r="B61" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61" s="27">
         <v>1</v>
@@ -4502,7 +4502,7 @@
         <v>76</v>
       </c>
       <c r="B62" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62" s="30">
         <v>2</v>
@@ -4558,7 +4558,7 @@
         <v>77</v>
       </c>
       <c r="B63" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" s="27">
         <v>2</v>
@@ -4612,7 +4612,7 @@
         <v>92</v>
       </c>
       <c r="B64" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" s="27">
         <v>2</v>
@@ -4660,7 +4660,7 @@
         <v>93</v>
       </c>
       <c r="B65" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" s="27">
         <v>2</v>
@@ -4708,7 +4708,7 @@
         <v>78</v>
       </c>
       <c r="B66" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" s="30">
         <v>1</v>
@@ -4764,7 +4764,7 @@
         <v>79</v>
       </c>
       <c r="B67" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" s="27">
         <v>1</v>
@@ -4818,7 +4818,7 @@
         <v>88</v>
       </c>
       <c r="B68" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" s="27">
         <v>1</v>
@@ -4866,7 +4866,7 @@
         <v>89</v>
       </c>
       <c r="B69" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69" s="27">
         <v>1</v>
@@ -4914,7 +4914,7 @@
         <v>80</v>
       </c>
       <c r="B70" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70" s="30">
         <v>2</v>
@@ -4970,7 +4970,7 @@
         <v>81</v>
       </c>
       <c r="B71" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71" s="27">
         <v>2</v>
@@ -5024,7 +5024,7 @@
         <v>84</v>
       </c>
       <c r="B72" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" s="27">
         <v>2</v>
@@ -5072,7 +5072,7 @@
         <v>85</v>
       </c>
       <c r="B73" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73" s="27">
         <v>2</v>
@@ -5120,7 +5120,7 @@
         <v>82</v>
       </c>
       <c r="B74" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" s="30">
         <v>2</v>
@@ -5176,7 +5176,7 @@
         <v>83</v>
       </c>
       <c r="B75" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75" s="27">
         <v>2</v>
@@ -5230,7 +5230,7 @@
         <v>86</v>
       </c>
       <c r="B76" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76" s="27">
         <v>2</v>
@@ -5278,7 +5278,7 @@
         <v>87</v>
       </c>
       <c r="B77" s="46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77" s="33">
         <v>2</v>
@@ -5326,7 +5326,7 @@
         <v>126</v>
       </c>
       <c r="B78" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78" s="27">
         <v>3</v>
@@ -5382,7 +5382,7 @@
         <v>127</v>
       </c>
       <c r="B79" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79" s="27">
         <v>3</v>
@@ -5436,7 +5436,7 @@
         <v>128</v>
       </c>
       <c r="B80" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80" s="27">
         <v>3</v>
@@ -5484,7 +5484,7 @@
         <v>129</v>
       </c>
       <c r="B81" s="47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" s="38">
         <v>3</v>

</xml_diff>

<commit_message>
Bug fix relating to getting trailing spaces into file name.
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@219 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Research\BankErosionMatlab\Trunk\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BankErosion\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -422,9 +422,6 @@
     <t>UpwindBedload</t>
   </si>
   <si>
-    <t xml:space="preserve">1c </t>
-  </si>
-  <si>
     <t>1g</t>
   </si>
   <si>
@@ -474,6 +471,9 @@
   </si>
   <si>
     <t>Delft3D but bank height ID</t>
+  </si>
+  <si>
+    <t>1c</t>
   </si>
 </sst>
 </file>
@@ -1347,10 +1347,10 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1439,7 @@
         <v>18</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>21</v>
@@ -1457,7 +1457,7 @@
         <v>37</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>4</v>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K3" s="44">
         <v>212.5</v>
@@ -1507,7 +1507,7 @@
         <v>120</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P3" s="5">
         <v>-240</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B5" s="44" t="b">
         <v>1</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="46" t="b">
         <v>1</v>
@@ -1816,7 +1816,7 @@
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K10" s="45">
         <v>212.5</v>
@@ -1863,7 +1863,7 @@
         <v>120</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P10" s="14">
         <v>-240</v>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K14" s="45">
         <v>212.5</v>
@@ -2069,7 +2069,7 @@
         <v>120</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P14" s="14">
         <v>-240</v>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K18" s="45">
         <v>212.5</v>
@@ -2275,7 +2275,7 @@
         <v>120</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P18" s="14">
         <v>-240</v>
@@ -2284,7 +2284,7 @@
         <v>210.5</v>
       </c>
       <c r="R18" s="45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K22" s="45">
         <v>212.5</v>
@@ -2481,7 +2481,7 @@
         <v>120</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P22" s="14">
         <v>-240</v>
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K26" s="45">
         <v>212.5</v>
@@ -2687,7 +2687,7 @@
         <v>120</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P26" s="14">
         <v>-240</v>
@@ -2696,7 +2696,7 @@
         <v>210.5</v>
       </c>
       <c r="R26" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K30" s="45">
         <v>212.5</v>
@@ -2893,7 +2893,7 @@
         <v>120</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P30" s="14">
         <v>-240</v>
@@ -3084,7 +3084,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K34" s="45">
         <v>212.5</v>
@@ -3099,7 +3099,7 @@
         <v>120</v>
       </c>
       <c r="O34" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P34" s="14">
         <v>-240</v>
@@ -3108,7 +3108,7 @@
         <v>210.5</v>
       </c>
       <c r="R34" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3290,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K38" s="45">
         <v>212.5</v>
@@ -3305,7 +3305,7 @@
         <v>120</v>
       </c>
       <c r="O38" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P38" s="14">
         <v>-240</v>
@@ -3314,7 +3314,7 @@
         <v>210.5</v>
       </c>
       <c r="R38" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3496,7 +3496,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K42" s="45">
         <v>212.5</v>
@@ -3511,7 +3511,7 @@
         <v>120</v>
       </c>
       <c r="O42" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P42" s="14">
         <v>-240</v>
@@ -3520,7 +3520,7 @@
         <v>210.5</v>
       </c>
       <c r="R42" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K46" s="45">
         <v>212.5</v>
@@ -3717,7 +3717,7 @@
         <v>120</v>
       </c>
       <c r="O46" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P46" s="14">
         <v>-240</v>
@@ -3726,7 +3726,7 @@
         <v>210.5</v>
       </c>
       <c r="R46" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
         <v>1</v>
       </c>
       <c r="J50" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K50" s="45">
         <v>212.5</v>
@@ -3923,7 +3923,7 @@
         <v>120</v>
       </c>
       <c r="O50" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P50" s="14">
         <v>-240</v>
@@ -3932,7 +3932,7 @@
         <v>210.5</v>
       </c>
       <c r="R50" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -4114,7 +4114,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K54" s="45">
         <v>212.5</v>
@@ -4129,7 +4129,7 @@
         <v>120</v>
       </c>
       <c r="O54" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P54" s="14">
         <v>-240</v>
@@ -4320,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K58" s="45">
         <v>212.5</v>
@@ -4335,7 +4335,7 @@
         <v>120</v>
       </c>
       <c r="O58" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P58" s="14">
         <v>-240</v>
@@ -4526,7 +4526,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K62" s="45">
         <v>212.5</v>
@@ -4541,7 +4541,7 @@
         <v>120</v>
       </c>
       <c r="O62" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P62" s="14">
         <v>-240</v>
@@ -4732,7 +4732,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K66" s="45">
         <v>212.5</v>
@@ -4747,7 +4747,7 @@
         <v>120</v>
       </c>
       <c r="O66" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P66" s="14">
         <v>-240</v>
@@ -4938,7 +4938,7 @@
         <v>1</v>
       </c>
       <c r="J70" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K70" s="45">
         <v>212.5</v>
@@ -4953,7 +4953,7 @@
         <v>120</v>
       </c>
       <c r="O70" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P70" s="14">
         <v>-240</v>
@@ -5144,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K74" s="45">
         <v>212.5</v>
@@ -5159,7 +5159,7 @@
         <v>120</v>
       </c>
       <c r="O74" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P74" s="14">
         <v>-240</v>
@@ -5323,7 +5323,7 @@
     </row>
     <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" s="44" t="b">
         <v>1</v>
@@ -5350,7 +5350,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K78" s="44">
         <v>212.5</v>
@@ -5365,7 +5365,7 @@
         <v>120</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P78" s="5">
         <v>-240</v>
@@ -5374,12 +5374,12 @@
         <v>210.5</v>
       </c>
       <c r="R78" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B79" s="44" t="b">
         <v>1</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B80" s="44" t="b">
         <v>1</v>
@@ -5481,7 +5481,7 @@
     </row>
     <row r="81" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B81" s="47" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Changed slope for bank identification so that it is consistent with bank height (at a resolution of 3m).
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@222 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BankErosion\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Research\BankErosionMatlab\Trunk\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1347,10 +1347,10 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="P79" sqref="P79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3502,7 +3502,7 @@
         <v>212.5</v>
       </c>
       <c r="L42" s="13">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="M42" s="13">
         <v>0.1</v>
@@ -3561,7 +3561,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N43" s="44">
         <v>60</v>
@@ -5000,7 +5000,7 @@
         <v>212.5</v>
       </c>
       <c r="L71" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M71" s="5">
         <v>1</v>
@@ -5206,7 +5206,7 @@
         <v>212.5</v>
       </c>
       <c r="L75" s="18">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M75" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Changing scenarios to simplify in line with changes made to paper. Analysis of triggers and stencils has been removed.
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@230 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Research\BankErosionMatlab\Trunk\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Sediment_processes\MarieCurie\BankErosionPaper\model\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N61" authorId="0" shapeId="0">
+    <comment ref="N33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
   <si>
     <t>Stencil</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Transport/no-transport ID - bank flux proportional to toe transport</t>
   </si>
   <si>
-    <t>Delft3D but transport/non-transport ID and stencil</t>
-  </si>
-  <si>
     <t>Slope ID - flux proportional to toe transport</t>
   </si>
   <si>
@@ -293,96 +290,12 @@
     <t>11b</t>
   </si>
   <si>
-    <t>12a</t>
-  </si>
-  <si>
-    <t>12b</t>
-  </si>
-  <si>
-    <t>13a</t>
-  </si>
-  <si>
-    <t>13b</t>
-  </si>
-  <si>
-    <t>14a</t>
-  </si>
-  <si>
-    <t>14b</t>
-  </si>
-  <si>
-    <t>15a</t>
-  </si>
-  <si>
-    <t>15b</t>
-  </si>
-  <si>
-    <t>16a</t>
-  </si>
-  <si>
-    <t>16b</t>
-  </si>
-  <si>
-    <t>17a</t>
-  </si>
-  <si>
-    <t>17b</t>
-  </si>
-  <si>
-    <t>18a</t>
-  </si>
-  <si>
-    <t>18b</t>
-  </si>
-  <si>
-    <t>17c</t>
-  </si>
-  <si>
-    <t>17d</t>
-  </si>
-  <si>
-    <t>18c</t>
-  </si>
-  <si>
-    <t>18d</t>
-  </si>
-  <si>
-    <t>16c</t>
-  </si>
-  <si>
-    <t>16d</t>
-  </si>
-  <si>
-    <t>13c</t>
-  </si>
-  <si>
-    <t>13d</t>
-  </si>
-  <si>
-    <t>15c</t>
-  </si>
-  <si>
-    <t>15d</t>
-  </si>
-  <si>
-    <t>14c</t>
-  </si>
-  <si>
-    <t>14d</t>
-  </si>
-  <si>
     <t>6c</t>
   </si>
   <si>
     <t>6d</t>
   </si>
   <si>
-    <t>12c</t>
-  </si>
-  <si>
-    <t>12d</t>
-  </si>
-  <si>
     <t>11c</t>
   </si>
   <si>
@@ -395,9 +308,6 @@
     <t>10d</t>
   </si>
   <si>
-    <t>9c</t>
-  </si>
-  <si>
     <t>9d</t>
   </si>
   <si>
@@ -434,46 +344,19 @@
     <t>Inputs\Selwyn_XS7_6m.csv</t>
   </si>
   <si>
-    <t>3 + stencil</t>
-  </si>
-  <si>
-    <t>5 + stencil</t>
-  </si>
-  <si>
-    <t>7 + stencil</t>
-  </si>
-  <si>
-    <t>7 + degrading toe trigger</t>
-  </si>
-  <si>
-    <t>7 + stencil + trigger</t>
-  </si>
-  <si>
-    <t>7 + threshold height trigger</t>
-  </si>
-  <si>
     <t>BankTestWL</t>
   </si>
   <si>
     <t>VbankTestWL</t>
   </si>
   <si>
-    <t>19a</t>
-  </si>
-  <si>
-    <t>19b</t>
-  </si>
-  <si>
-    <t>19c</t>
-  </si>
-  <si>
-    <t>19d</t>
-  </si>
-  <si>
     <t>Delft3D but bank height ID</t>
   </si>
   <si>
     <t>1c</t>
+  </si>
+  <si>
+    <t>96c</t>
   </si>
 </sst>
 </file>
@@ -931,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,7 +896,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1344,13 +1226,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P79" sqref="P79"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,19 +1252,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51"/>
+      <c r="A1" s="50"/>
       <c r="B1" s="42"/>
       <c r="C1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="50" t="s">
+      <c r="D1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="52"/>
+      <c r="F1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="49" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="23" t="s">
@@ -1393,19 +1275,19 @@
         <v>2</v>
       </c>
       <c r="K1" s="42"/>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="54"/>
+      <c r="M1" s="53"/>
       <c r="N1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
+      <c r="O1" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1433,13 +1315,13 @@
         <v>16</v>
       </c>
       <c r="I2" s="43" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="J2" s="43" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>21</v>
@@ -1451,13 +1333,13 @@
         <v>25</v>
       </c>
       <c r="O2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>37</v>
-      </c>
       <c r="Q2" s="11" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>4</v>
@@ -1465,7 +1347,7 @@
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="44" t="b">
         <v>1</v>
@@ -1492,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K3" s="44">
         <v>212.5</v>
@@ -1507,7 +1389,7 @@
         <v>120</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P3" s="5">
         <v>-240</v>
@@ -1521,7 +1403,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="44" t="b">
         <v>1</v>
@@ -1563,7 +1445,7 @@
         <v>60</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P4" s="5">
         <v>-240</v>
@@ -1575,7 +1457,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="B5" s="44" t="b">
         <v>1</v>
@@ -1623,7 +1505,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="44" t="b">
         <v>1</v>
@@ -1650,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K6" s="44">
         <v>212.5</v>
@@ -1671,7 +1553,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="44" t="b">
         <v>1</v>
@@ -1721,7 +1603,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="44" t="b">
         <v>1</v>
@@ -1771,7 +1653,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B9" s="46" t="b">
         <v>1</v>
@@ -1816,12 +1698,12 @@
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="45" t="b">
         <v>1</v>
@@ -1848,7 +1730,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K10" s="45">
         <v>212.5</v>
@@ -1863,7 +1745,7 @@
         <v>120</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P10" s="14">
         <v>-240</v>
@@ -1872,12 +1754,12 @@
         <v>210.5</v>
       </c>
       <c r="R10" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="44" t="b">
         <v>1</v>
@@ -1919,7 +1801,7 @@
         <v>60</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P11" s="5">
         <v>-240</v>
@@ -1931,7 +1813,7 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B12" s="44" t="b">
         <v>1</v>
@@ -1979,7 +1861,7 @@
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B13" s="44" t="b">
         <v>1</v>
@@ -2006,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="44">
         <v>212.5</v>
@@ -2027,7 +1909,7 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="45" t="b">
         <v>1</v>
@@ -2054,7 +1936,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K14" s="45">
         <v>212.5</v>
@@ -2069,7 +1951,7 @@
         <v>120</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P14" s="14">
         <v>-240</v>
@@ -2083,7 +1965,7 @@
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="44" t="b">
         <v>1</v>
@@ -2125,7 +2007,7 @@
         <v>60</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P15" s="5">
         <v>-240</v>
@@ -2137,7 +2019,7 @@
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="44" t="b">
         <v>1</v>
@@ -2185,7 +2067,7 @@
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="44" t="b">
         <v>1</v>
@@ -2212,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K17" s="44">
         <v>212.5</v>
@@ -2233,19 +2115,19 @@
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="45" t="b">
         <v>1</v>
       </c>
       <c r="C18" s="30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="31">
         <v>0</v>
       </c>
       <c r="E18" s="31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="31">
         <v>0</v>
@@ -2260,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K18" s="45">
         <v>212.5</v>
@@ -2275,7 +2157,7 @@
         <v>120</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P18" s="14">
         <v>-240</v>
@@ -2284,24 +2166,24 @@
         <v>210.5</v>
       </c>
       <c r="R18" s="45" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C19" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="28">
         <v>0</v>
       </c>
       <c r="E19" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="28">
         <v>0</v>
@@ -2331,7 +2213,7 @@
         <v>60</v>
       </c>
       <c r="O19" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P19" s="5">
         <v>-240</v>
@@ -2343,19 +2225,19 @@
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C20" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" s="28">
         <v>0</v>
       </c>
       <c r="E20" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20" s="28">
         <v>0</v>
@@ -2391,19 +2273,19 @@
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C21" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" s="28">
         <v>0</v>
       </c>
       <c r="E21" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" s="28">
         <v>0</v>
@@ -2418,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" s="44">
         <v>212.5</v>
@@ -2427,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="4">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="N21" s="44">
         <v>2</v>
@@ -2439,13 +2321,13 @@
     </row>
     <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="45" t="b">
         <v>1</v>
       </c>
       <c r="C22" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="31">
         <v>0</v>
@@ -2466,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K22" s="45">
         <v>212.5</v>
@@ -2481,7 +2363,7 @@
         <v>120</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P22" s="14">
         <v>-240</v>
@@ -2490,18 +2372,18 @@
         <v>210.5</v>
       </c>
       <c r="R22" s="45" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C23" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="28">
         <v>0</v>
@@ -2537,7 +2419,7 @@
         <v>60</v>
       </c>
       <c r="O23" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P23" s="5">
         <v>-240</v>
@@ -2549,13 +2431,13 @@
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C24" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="28">
         <v>0</v>
@@ -2597,13 +2479,13 @@
     </row>
     <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C25" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="28">
         <v>0</v>
@@ -2624,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K25" s="44">
         <v>212.5</v>
@@ -2645,7 +2527,7 @@
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="45" t="b">
         <v>1</v>
@@ -2657,13 +2539,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F26" s="31">
         <v>0</v>
       </c>
       <c r="G26" s="36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H26" s="32">
         <v>0</v>
@@ -2672,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K26" s="45">
         <v>212.5</v>
@@ -2687,7 +2569,7 @@
         <v>120</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P26" s="14">
         <v>-240</v>
@@ -2696,12 +2578,12 @@
         <v>210.5</v>
       </c>
       <c r="R26" s="45" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="44" t="b">
         <v>1</v>
@@ -2713,13 +2595,13 @@
         <v>0</v>
       </c>
       <c r="E27" s="28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F27" s="28">
         <v>0</v>
       </c>
       <c r="G27" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H27" s="29">
         <v>0</v>
@@ -2743,7 +2625,7 @@
         <v>60</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P27" s="5">
         <v>-240</v>
@@ -2755,7 +2637,7 @@
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B28" s="44" t="b">
         <v>1</v>
@@ -2767,13 +2649,13 @@
         <v>0</v>
       </c>
       <c r="E28" s="28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F28" s="28">
         <v>0</v>
       </c>
       <c r="G28" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H28" s="29">
         <v>0</v>
@@ -2803,7 +2685,7 @@
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B29" s="44" t="b">
         <v>1</v>
@@ -2815,13 +2697,13 @@
         <v>0</v>
       </c>
       <c r="E29" s="28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F29" s="28">
         <v>0</v>
       </c>
       <c r="G29" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H29" s="29">
         <v>0</v>
@@ -2830,7 +2712,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K29" s="44">
         <v>212.5</v>
@@ -2851,13 +2733,13 @@
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="45" t="b">
         <v>1</v>
       </c>
       <c r="C30" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" s="31">
         <v>0</v>
@@ -2869,16 +2751,16 @@
         <v>0</v>
       </c>
       <c r="G30" s="36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H30" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="45">
         <v>1</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K30" s="45">
         <v>212.5</v>
@@ -2893,7 +2775,7 @@
         <v>120</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P30" s="14">
         <v>-240</v>
@@ -2902,18 +2784,18 @@
         <v>210.5</v>
       </c>
       <c r="R30" s="45" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C31" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="28">
         <v>0</v>
@@ -2925,10 +2807,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H31" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="44">
         <v>1</v>
@@ -2949,7 +2831,7 @@
         <v>60</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P31" s="5">
         <v>-240</v>
@@ -2961,13 +2843,13 @@
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="B32" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C32" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="28">
         <v>0</v>
@@ -2979,10 +2861,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="44">
         <v>1</v>
@@ -2997,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N32" s="44">
         <v>20</v>
@@ -3009,13 +2891,13 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="B33" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C33" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="28">
         <v>0</v>
@@ -3027,16 +2909,16 @@
         <v>0</v>
       </c>
       <c r="G33" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H33" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="44">
         <v>1</v>
       </c>
       <c r="J33" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K33" s="44">
         <v>212.5</v>
@@ -3048,7 +2930,7 @@
         <v>0.1</v>
       </c>
       <c r="N33" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O33" s="18"/>
       <c r="P33" s="5"/>
@@ -3057,7 +2939,7 @@
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="45" t="b">
         <v>1</v>
@@ -3069,22 +2951,22 @@
         <v>0</v>
       </c>
       <c r="E34" s="31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="31">
         <v>0</v>
       </c>
       <c r="G34" s="36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H34" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="45">
         <v>1</v>
       </c>
       <c r="J34" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K34" s="45">
         <v>212.5</v>
@@ -3099,7 +2981,7 @@
         <v>120</v>
       </c>
       <c r="O34" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P34" s="14">
         <v>-240</v>
@@ -3108,12 +2990,12 @@
         <v>210.5</v>
       </c>
       <c r="R34" s="45" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="44" t="b">
         <v>1</v>
@@ -3125,16 +3007,16 @@
         <v>0</v>
       </c>
       <c r="E35" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35" s="28">
         <v>0</v>
       </c>
       <c r="G35" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H35" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="44">
         <v>1</v>
@@ -3155,7 +3037,7 @@
         <v>60</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P35" s="5">
         <v>-240</v>
@@ -3167,7 +3049,7 @@
     </row>
     <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="B36" s="44" t="b">
         <v>1</v>
@@ -3179,16 +3061,16 @@
         <v>0</v>
       </c>
       <c r="E36" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36" s="28">
         <v>0</v>
       </c>
       <c r="G36" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H36" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="44">
         <v>1</v>
@@ -3203,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N36" s="44">
         <v>20</v>
@@ -3215,7 +3097,7 @@
     </row>
     <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="B37" s="44" t="b">
         <v>1</v>
@@ -3227,22 +3109,22 @@
         <v>0</v>
       </c>
       <c r="E37" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37" s="28">
         <v>0</v>
       </c>
       <c r="G37" s="37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H37" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="44">
         <v>1</v>
       </c>
       <c r="J37" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K37" s="44">
         <v>212.5</v>
@@ -3263,13 +3145,13 @@
     </row>
     <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="45" t="b">
         <v>1</v>
       </c>
       <c r="C38" s="30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="31">
         <v>0</v>
@@ -3278,10 +3160,10 @@
         <v>0</v>
       </c>
       <c r="F38" s="31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G38" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H38" s="32">
         <v>0</v>
@@ -3290,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K38" s="45">
         <v>212.5</v>
@@ -3299,13 +3181,13 @@
         <v>0</v>
       </c>
       <c r="M38" s="13">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N38" s="45">
         <v>120</v>
       </c>
       <c r="O38" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P38" s="14">
         <v>-240</v>
@@ -3314,18 +3196,18 @@
         <v>210.5</v>
       </c>
       <c r="R38" s="45" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C39" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="28">
         <v>0</v>
@@ -3334,10 +3216,10 @@
         <v>0</v>
       </c>
       <c r="F39" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G39" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H39" s="29">
         <v>0</v>
@@ -3355,13 +3237,13 @@
         <v>0</v>
       </c>
       <c r="M39" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N39" s="44">
         <v>60</v>
       </c>
       <c r="O39" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P39" s="5">
         <v>-240</v>
@@ -3373,13 +3255,13 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B40" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C40" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="28">
         <v>0</v>
@@ -3388,10 +3270,10 @@
         <v>0</v>
       </c>
       <c r="F40" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G40" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40" s="29">
         <v>0</v>
@@ -3409,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N40" s="44">
         <v>20</v>
@@ -3421,13 +3303,13 @@
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="B41" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C41" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" s="28">
         <v>0</v>
@@ -3436,10 +3318,10 @@
         <v>0</v>
       </c>
       <c r="F41" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G41" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H41" s="29">
         <v>0</v>
@@ -3448,7 +3330,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K41" s="44">
         <v>212.5</v>
@@ -3457,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N41" s="44">
         <v>2</v>
@@ -3469,7 +3351,7 @@
     </row>
     <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" s="45" t="b">
         <v>1</v>
@@ -3481,13 +3363,13 @@
         <v>0</v>
       </c>
       <c r="E42" s="31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F42" s="31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G42" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H42" s="32">
         <v>0</v>
@@ -3496,22 +3378,22 @@
         <v>1</v>
       </c>
       <c r="J42" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K42" s="45">
         <v>212.5</v>
       </c>
-      <c r="L42" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="M42" s="13">
-        <v>0.1</v>
+      <c r="L42" s="19">
+        <v>0</v>
+      </c>
+      <c r="M42" s="14">
+        <v>1</v>
       </c>
       <c r="N42" s="45">
         <v>120</v>
       </c>
       <c r="O42" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P42" s="14">
         <v>-240</v>
@@ -3520,12 +3402,12 @@
         <v>210.5</v>
       </c>
       <c r="R42" s="45" t="s">
-        <v>121</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" s="44" t="b">
         <v>1</v>
@@ -3537,13 +3419,13 @@
         <v>0</v>
       </c>
       <c r="E43" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G43" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H43" s="29">
         <v>0</v>
@@ -3557,17 +3439,17 @@
       <c r="K43" s="44">
         <v>212.5</v>
       </c>
-      <c r="L43" s="4">
-        <v>0</v>
-      </c>
-      <c r="M43" s="4">
-        <v>0.05</v>
+      <c r="L43" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="M43" s="5">
+        <v>1</v>
       </c>
       <c r="N43" s="44">
         <v>60</v>
       </c>
       <c r="O43" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P43" s="5">
         <v>-240</v>
@@ -3579,7 +3461,7 @@
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B44" s="44" t="b">
         <v>1</v>
@@ -3591,13 +3473,13 @@
         <v>0</v>
       </c>
       <c r="E44" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G44" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H44" s="29">
         <v>0</v>
@@ -3611,11 +3493,11 @@
       <c r="K44" s="44">
         <v>212.5</v>
       </c>
-      <c r="L44" s="4">
-        <v>0</v>
-      </c>
-      <c r="M44" s="4">
-        <v>7.0000000000000007E-2</v>
+      <c r="L44" s="18">
+        <v>0</v>
+      </c>
+      <c r="M44" s="5">
+        <v>1</v>
       </c>
       <c r="N44" s="44">
         <v>20</v>
@@ -3627,7 +3509,7 @@
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B45" s="44" t="b">
         <v>1</v>
@@ -3639,13 +3521,13 @@
         <v>0</v>
       </c>
       <c r="E45" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F45" s="28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G45" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H45" s="29">
         <v>0</v>
@@ -3654,16 +3536,16 @@
         <v>1</v>
       </c>
       <c r="J45" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K45" s="44">
         <v>212.5</v>
       </c>
-      <c r="L45" s="4">
-        <v>0</v>
-      </c>
-      <c r="M45" s="4">
-        <v>0.1</v>
+      <c r="L45" s="18">
+        <v>0</v>
+      </c>
+      <c r="M45" s="5">
+        <v>1</v>
       </c>
       <c r="N45" s="44">
         <v>2</v>
@@ -3675,13 +3557,13 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="45" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" s="31">
         <v>0</v>
@@ -3690,10 +3572,10 @@
         <v>0</v>
       </c>
       <c r="F46" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H46" s="32">
         <v>0</v>
@@ -3702,7 +3584,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="45" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="K46" s="45">
         <v>212.5</v>
@@ -3711,13 +3593,13 @@
         <v>0</v>
       </c>
       <c r="M46" s="13">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N46" s="45">
         <v>120</v>
       </c>
       <c r="O46" s="19" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="P46" s="14">
         <v>-240</v>
@@ -3725,19 +3607,19 @@
       <c r="Q46" s="14">
         <v>210.5</v>
       </c>
-      <c r="R46" s="45" t="s">
-        <v>122</v>
+      <c r="R46" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C47" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" s="28">
         <v>0</v>
@@ -3746,10 +3628,10 @@
         <v>0</v>
       </c>
       <c r="F47" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H47" s="29">
         <v>0</v>
@@ -3767,13 +3649,13 @@
         <v>0</v>
       </c>
       <c r="M47" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N47" s="44">
         <v>60</v>
       </c>
       <c r="O47" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P47" s="5">
         <v>-240</v>
@@ -3781,17 +3663,17 @@
       <c r="Q47" s="5">
         <v>210.5</v>
       </c>
-      <c r="R47" s="44"/>
+      <c r="R47" s="5"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B48" s="44" t="b">
         <v>1</v>
       </c>
       <c r="C48" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48" s="28">
         <v>0</v>
@@ -3800,10 +3682,10 @@
         <v>0</v>
       </c>
       <c r="F48" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H48" s="29">
         <v>0</v>
@@ -3821,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N48" s="44">
         <v>20</v>
@@ -3829,1703 +3711,55 @@
       <c r="O48" s="18"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
-      <c r="R48" s="44"/>
-    </row>
-    <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" s="27">
-        <v>2</v>
-      </c>
-      <c r="D49" s="28">
-        <v>0</v>
-      </c>
-      <c r="E49" s="28">
-        <v>0</v>
-      </c>
-      <c r="F49" s="28">
-        <v>1</v>
-      </c>
-      <c r="G49" s="37">
+      <c r="R48" s="5"/>
+    </row>
+    <row r="49" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" s="38">
         <v>3</v>
       </c>
-      <c r="H49" s="29">
-        <v>0</v>
-      </c>
-      <c r="I49" s="44">
-        <v>1</v>
-      </c>
-      <c r="J49" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K49" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L49" s="4">
-        <v>0</v>
-      </c>
-      <c r="M49" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N49" s="44">
-        <v>2</v>
-      </c>
-      <c r="O49" s="18"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="44"/>
-    </row>
-    <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C50" s="30">
-        <v>2</v>
-      </c>
-      <c r="D50" s="31">
-        <v>0</v>
-      </c>
-      <c r="E50" s="31">
-        <v>2</v>
-      </c>
-      <c r="F50" s="31">
-        <v>1</v>
-      </c>
-      <c r="G50" s="36">
-        <v>3</v>
-      </c>
-      <c r="H50" s="32">
-        <v>0</v>
-      </c>
-      <c r="I50" s="45">
-        <v>1</v>
-      </c>
-      <c r="J50" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K50" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L50" s="13">
-        <v>0</v>
-      </c>
-      <c r="M50" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="N50" s="45">
-        <v>120</v>
-      </c>
-      <c r="O50" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P50" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q50" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R50" s="45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C51" s="27">
-        <v>2</v>
-      </c>
-      <c r="D51" s="28">
-        <v>0</v>
-      </c>
-      <c r="E51" s="28">
-        <v>2</v>
-      </c>
-      <c r="F51" s="28">
-        <v>1</v>
-      </c>
-      <c r="G51" s="37">
-        <v>3</v>
-      </c>
-      <c r="H51" s="29">
-        <v>0</v>
-      </c>
-      <c r="I51" s="44">
-        <v>1</v>
-      </c>
-      <c r="J51" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K51" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L51" s="4">
-        <v>0</v>
-      </c>
-      <c r="M51" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N51" s="44">
-        <v>60</v>
-      </c>
-      <c r="O51" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P51" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q51" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R51" s="44"/>
-    </row>
-    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C52" s="27">
-        <v>2</v>
-      </c>
-      <c r="D52" s="28">
-        <v>0</v>
-      </c>
-      <c r="E52" s="28">
-        <v>2</v>
-      </c>
-      <c r="F52" s="28">
-        <v>1</v>
-      </c>
-      <c r="G52" s="37">
-        <v>3</v>
-      </c>
-      <c r="H52" s="29">
-        <v>0</v>
-      </c>
-      <c r="I52" s="44">
-        <v>1</v>
-      </c>
-      <c r="J52" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K52" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L52" s="4">
-        <v>0</v>
-      </c>
-      <c r="M52" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N52" s="44">
-        <v>20</v>
-      </c>
-      <c r="O52" s="18"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="44"/>
-    </row>
-    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C53" s="27">
-        <v>2</v>
-      </c>
-      <c r="D53" s="28">
-        <v>0</v>
-      </c>
-      <c r="E53" s="28">
-        <v>2</v>
-      </c>
-      <c r="F53" s="28">
-        <v>1</v>
-      </c>
-      <c r="G53" s="37">
-        <v>3</v>
-      </c>
-      <c r="H53" s="29">
-        <v>0</v>
-      </c>
-      <c r="I53" s="44">
-        <v>1</v>
-      </c>
-      <c r="J53" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K53" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L53" s="4">
-        <v>0</v>
-      </c>
-      <c r="M53" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N53" s="44">
-        <v>2</v>
-      </c>
-      <c r="O53" s="18"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="44"/>
-    </row>
-    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C54" s="30">
-        <v>1</v>
-      </c>
-      <c r="D54" s="31">
-        <v>0</v>
-      </c>
-      <c r="E54" s="31">
-        <v>0</v>
-      </c>
-      <c r="F54" s="31">
-        <v>0</v>
-      </c>
-      <c r="G54" s="36">
-        <v>4</v>
-      </c>
-      <c r="H54" s="32">
-        <v>0</v>
-      </c>
-      <c r="I54" s="45">
-        <v>1</v>
-      </c>
-      <c r="J54" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K54" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L54" s="13">
-        <v>0</v>
-      </c>
-      <c r="M54" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="N54" s="45">
-        <v>120</v>
-      </c>
-      <c r="O54" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P54" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q54" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R54" s="45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C55" s="27">
-        <v>1</v>
-      </c>
-      <c r="D55" s="28">
-        <v>0</v>
-      </c>
-      <c r="E55" s="28">
-        <v>0</v>
-      </c>
-      <c r="F55" s="28">
-        <v>0</v>
-      </c>
-      <c r="G55" s="37">
-        <v>4</v>
-      </c>
-      <c r="H55" s="29">
-        <v>0</v>
-      </c>
-      <c r="I55" s="44">
-        <v>1</v>
-      </c>
-      <c r="J55" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K55" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L55" s="4">
-        <v>0</v>
-      </c>
-      <c r="M55" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N55" s="44">
-        <v>60</v>
-      </c>
-      <c r="O55" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P55" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q55" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R55" s="44"/>
-    </row>
-    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C56" s="27">
-        <v>1</v>
-      </c>
-      <c r="D56" s="28">
-        <v>0</v>
-      </c>
-      <c r="E56" s="28">
-        <v>0</v>
-      </c>
-      <c r="F56" s="28">
-        <v>0</v>
-      </c>
-      <c r="G56" s="37">
-        <v>4</v>
-      </c>
-      <c r="H56" s="29">
-        <v>0</v>
-      </c>
-      <c r="I56" s="44">
-        <v>1</v>
-      </c>
-      <c r="J56" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K56" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L56" s="4">
-        <v>0</v>
-      </c>
-      <c r="M56" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N56" s="44">
-        <v>20</v>
-      </c>
-      <c r="O56" s="18"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="44"/>
-    </row>
-    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C57" s="27">
-        <v>1</v>
-      </c>
-      <c r="D57" s="28">
-        <v>0</v>
-      </c>
-      <c r="E57" s="28">
-        <v>0</v>
-      </c>
-      <c r="F57" s="28">
-        <v>0</v>
-      </c>
-      <c r="G57" s="37">
-        <v>4</v>
-      </c>
-      <c r="H57" s="29">
-        <v>0</v>
-      </c>
-      <c r="I57" s="44">
-        <v>1</v>
-      </c>
-      <c r="J57" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K57" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L57" s="4">
-        <v>0</v>
-      </c>
-      <c r="M57" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N57" s="44">
-        <v>2</v>
-      </c>
-      <c r="O57" s="18"/>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="44"/>
-    </row>
-    <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C58" s="30">
-        <v>1</v>
-      </c>
-      <c r="D58" s="31">
-        <v>0</v>
-      </c>
-      <c r="E58" s="31">
-        <v>0</v>
-      </c>
-      <c r="F58" s="31">
-        <v>0</v>
-      </c>
-      <c r="G58" s="36">
-        <v>4</v>
-      </c>
-      <c r="H58" s="32">
-        <v>1</v>
-      </c>
-      <c r="I58" s="45">
-        <v>1</v>
-      </c>
-      <c r="J58" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K58" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L58" s="13">
-        <v>0</v>
-      </c>
-      <c r="M58" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="N58" s="45">
-        <v>120</v>
-      </c>
-      <c r="O58" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P58" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q58" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R58" s="45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C59" s="27">
-        <v>1</v>
-      </c>
-      <c r="D59" s="28">
-        <v>0</v>
-      </c>
-      <c r="E59" s="28">
-        <v>0</v>
-      </c>
-      <c r="F59" s="28">
-        <v>0</v>
-      </c>
-      <c r="G59" s="37">
-        <v>4</v>
-      </c>
-      <c r="H59" s="29">
-        <v>1</v>
-      </c>
-      <c r="I59" s="44">
-        <v>1</v>
-      </c>
-      <c r="J59" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K59" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L59" s="4">
-        <v>0</v>
-      </c>
-      <c r="M59" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N59" s="44">
-        <v>60</v>
-      </c>
-      <c r="O59" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P59" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q59" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R59" s="44"/>
-    </row>
-    <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B60" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C60" s="27">
-        <v>1</v>
-      </c>
-      <c r="D60" s="28">
-        <v>0</v>
-      </c>
-      <c r="E60" s="28">
-        <v>0</v>
-      </c>
-      <c r="F60" s="28">
-        <v>0</v>
-      </c>
-      <c r="G60" s="37">
-        <v>4</v>
-      </c>
-      <c r="H60" s="29">
-        <v>1</v>
-      </c>
-      <c r="I60" s="44">
-        <v>1</v>
-      </c>
-      <c r="J60" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K60" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L60" s="4">
-        <v>0</v>
-      </c>
-      <c r="M60" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="N60" s="44">
-        <v>20</v>
-      </c>
-      <c r="O60" s="18"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="44"/>
-    </row>
-    <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C61" s="27">
-        <v>1</v>
-      </c>
-      <c r="D61" s="28">
-        <v>0</v>
-      </c>
-      <c r="E61" s="28">
-        <v>0</v>
-      </c>
-      <c r="F61" s="28">
-        <v>0</v>
-      </c>
-      <c r="G61" s="37">
-        <v>4</v>
-      </c>
-      <c r="H61" s="29">
-        <v>1</v>
-      </c>
-      <c r="I61" s="44">
-        <v>1</v>
-      </c>
-      <c r="J61" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K61" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L61" s="4">
-        <v>0</v>
-      </c>
-      <c r="M61" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N61" s="44">
-        <v>1</v>
-      </c>
-      <c r="O61" s="18"/>
-      <c r="P61" s="5"/>
-      <c r="Q61" s="5"/>
-      <c r="R61" s="44"/>
-    </row>
-    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B62" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62" s="30">
-        <v>2</v>
-      </c>
-      <c r="D62" s="31">
-        <v>0</v>
-      </c>
-      <c r="E62" s="31">
-        <v>0</v>
-      </c>
-      <c r="F62" s="31">
-        <v>0</v>
-      </c>
-      <c r="G62" s="36">
-        <v>4</v>
-      </c>
-      <c r="H62" s="32">
-        <v>1</v>
-      </c>
-      <c r="I62" s="45">
-        <v>1</v>
-      </c>
-      <c r="J62" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K62" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L62" s="13">
-        <v>0</v>
-      </c>
-      <c r="M62" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="N62" s="45">
-        <v>120</v>
-      </c>
-      <c r="O62" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P62" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q62" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R62" s="45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C63" s="27">
-        <v>2</v>
-      </c>
-      <c r="D63" s="28">
-        <v>0</v>
-      </c>
-      <c r="E63" s="28">
-        <v>0</v>
-      </c>
-      <c r="F63" s="28">
-        <v>0</v>
-      </c>
-      <c r="G63" s="37">
-        <v>4</v>
-      </c>
-      <c r="H63" s="29">
-        <v>1</v>
-      </c>
-      <c r="I63" s="44">
-        <v>1</v>
-      </c>
-      <c r="J63" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K63" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L63" s="4">
-        <v>0</v>
-      </c>
-      <c r="M63" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N63" s="44">
-        <v>60</v>
-      </c>
-      <c r="O63" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P63" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q63" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R63" s="44"/>
-    </row>
-    <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C64" s="27">
-        <v>2</v>
-      </c>
-      <c r="D64" s="28">
-        <v>0</v>
-      </c>
-      <c r="E64" s="28">
-        <v>0</v>
-      </c>
-      <c r="F64" s="28">
-        <v>0</v>
-      </c>
-      <c r="G64" s="37">
-        <v>4</v>
-      </c>
-      <c r="H64" s="29">
-        <v>1</v>
-      </c>
-      <c r="I64" s="44">
-        <v>1</v>
-      </c>
-      <c r="J64" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K64" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L64" s="4">
-        <v>0</v>
-      </c>
-      <c r="M64" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="N64" s="44">
-        <v>20</v>
-      </c>
-      <c r="O64" s="18"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="44"/>
-    </row>
-    <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B65" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C65" s="27">
-        <v>2</v>
-      </c>
-      <c r="D65" s="28">
-        <v>0</v>
-      </c>
-      <c r="E65" s="28">
-        <v>0</v>
-      </c>
-      <c r="F65" s="28">
-        <v>0</v>
-      </c>
-      <c r="G65" s="37">
-        <v>4</v>
-      </c>
-      <c r="H65" s="29">
-        <v>1</v>
-      </c>
-      <c r="I65" s="44">
-        <v>1</v>
-      </c>
-      <c r="J65" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K65" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L65" s="4">
-        <v>0</v>
-      </c>
-      <c r="M65" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="N65" s="44">
-        <v>2</v>
-      </c>
-      <c r="O65" s="18"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="44"/>
-    </row>
-    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C66" s="30">
-        <v>1</v>
-      </c>
-      <c r="D66" s="31">
-        <v>0</v>
-      </c>
-      <c r="E66" s="31">
-        <v>0</v>
-      </c>
-      <c r="F66" s="31">
-        <v>0</v>
-      </c>
-      <c r="G66" s="36">
-        <v>2</v>
-      </c>
-      <c r="H66" s="32">
-        <v>0</v>
-      </c>
-      <c r="I66" s="45">
-        <v>1</v>
-      </c>
-      <c r="J66" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K66" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L66" s="13">
-        <v>0</v>
-      </c>
-      <c r="M66" s="13">
-        <v>1</v>
-      </c>
-      <c r="N66" s="45">
-        <v>120</v>
-      </c>
-      <c r="O66" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P66" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q66" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R66" s="45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C67" s="27">
-        <v>1</v>
-      </c>
-      <c r="D67" s="28">
-        <v>0</v>
-      </c>
-      <c r="E67" s="28">
-        <v>0</v>
-      </c>
-      <c r="F67" s="28">
-        <v>0</v>
-      </c>
-      <c r="G67" s="37">
-        <v>2</v>
-      </c>
-      <c r="H67" s="29">
-        <v>0</v>
-      </c>
-      <c r="I67" s="44">
-        <v>1</v>
-      </c>
-      <c r="J67" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K67" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L67" s="4">
-        <v>0</v>
-      </c>
-      <c r="M67" s="4">
-        <v>1</v>
-      </c>
-      <c r="N67" s="44">
-        <v>60</v>
-      </c>
-      <c r="O67" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P67" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q67" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R67" s="44"/>
-    </row>
-    <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B68" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C68" s="27">
-        <v>1</v>
-      </c>
-      <c r="D68" s="28">
-        <v>0</v>
-      </c>
-      <c r="E68" s="28">
-        <v>0</v>
-      </c>
-      <c r="F68" s="28">
-        <v>0</v>
-      </c>
-      <c r="G68" s="37">
-        <v>2</v>
-      </c>
-      <c r="H68" s="29">
-        <v>0</v>
-      </c>
-      <c r="I68" s="44">
-        <v>1</v>
-      </c>
-      <c r="J68" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K68" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L68" s="4">
-        <v>0</v>
-      </c>
-      <c r="M68" s="4">
-        <v>1</v>
-      </c>
-      <c r="N68" s="44">
-        <v>20</v>
-      </c>
-      <c r="O68" s="18"/>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="5"/>
-      <c r="R68" s="44"/>
-    </row>
-    <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B69" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C69" s="27">
-        <v>1</v>
-      </c>
-      <c r="D69" s="28">
-        <v>0</v>
-      </c>
-      <c r="E69" s="28">
-        <v>0</v>
-      </c>
-      <c r="F69" s="28">
-        <v>0</v>
-      </c>
-      <c r="G69" s="37">
-        <v>2</v>
-      </c>
-      <c r="H69" s="29">
-        <v>0</v>
-      </c>
-      <c r="I69" s="44">
-        <v>1</v>
-      </c>
-      <c r="J69" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K69" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L69" s="4">
-        <v>0</v>
-      </c>
-      <c r="M69" s="4">
-        <v>1</v>
-      </c>
-      <c r="N69" s="44">
-        <v>2</v>
-      </c>
-      <c r="O69" s="18"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="44"/>
-    </row>
-    <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C70" s="30">
-        <v>2</v>
-      </c>
-      <c r="D70" s="31">
-        <v>0</v>
-      </c>
-      <c r="E70" s="31">
-        <v>0</v>
-      </c>
-      <c r="F70" s="31">
-        <v>0</v>
-      </c>
-      <c r="G70" s="36">
-        <v>2</v>
-      </c>
-      <c r="H70" s="32">
-        <v>0</v>
-      </c>
-      <c r="I70" s="45">
-        <v>1</v>
-      </c>
-      <c r="J70" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K70" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L70" s="19">
-        <v>0</v>
-      </c>
-      <c r="M70" s="14">
-        <v>1</v>
-      </c>
-      <c r="N70" s="45">
-        <v>120</v>
-      </c>
-      <c r="O70" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P70" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q70" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R70" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C71" s="27">
-        <v>2</v>
-      </c>
-      <c r="D71" s="28">
-        <v>0</v>
-      </c>
-      <c r="E71" s="28">
-        <v>0</v>
-      </c>
-      <c r="F71" s="28">
-        <v>0</v>
-      </c>
-      <c r="G71" s="37">
-        <v>2</v>
-      </c>
-      <c r="H71" s="29">
-        <v>0</v>
-      </c>
-      <c r="I71" s="44">
-        <v>1</v>
-      </c>
-      <c r="J71" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K71" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L71" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="M71" s="5">
-        <v>1</v>
-      </c>
-      <c r="N71" s="44">
-        <v>60</v>
-      </c>
-      <c r="O71" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P71" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q71" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R71" s="44"/>
-    </row>
-    <row r="72" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C72" s="27">
-        <v>2</v>
-      </c>
-      <c r="D72" s="28">
-        <v>0</v>
-      </c>
-      <c r="E72" s="28">
-        <v>0</v>
-      </c>
-      <c r="F72" s="28">
-        <v>0</v>
-      </c>
-      <c r="G72" s="37">
-        <v>2</v>
-      </c>
-      <c r="H72" s="29">
-        <v>0</v>
-      </c>
-      <c r="I72" s="44">
-        <v>1</v>
-      </c>
-      <c r="J72" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L72" s="18">
-        <v>0</v>
-      </c>
-      <c r="M72" s="5">
-        <v>1</v>
-      </c>
-      <c r="N72" s="44">
-        <v>20</v>
-      </c>
-      <c r="O72" s="18"/>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-      <c r="R72" s="44"/>
-    </row>
-    <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C73" s="27">
-        <v>2</v>
-      </c>
-      <c r="D73" s="28">
-        <v>0</v>
-      </c>
-      <c r="E73" s="28">
-        <v>0</v>
-      </c>
-      <c r="F73" s="28">
-        <v>0</v>
-      </c>
-      <c r="G73" s="37">
-        <v>2</v>
-      </c>
-      <c r="H73" s="29">
-        <v>0</v>
-      </c>
-      <c r="I73" s="44">
-        <v>1</v>
-      </c>
-      <c r="J73" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="K73" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L73" s="18">
-        <v>0</v>
-      </c>
-      <c r="M73" s="5">
-        <v>1</v>
-      </c>
-      <c r="N73" s="44">
-        <v>2</v>
-      </c>
-      <c r="O73" s="18"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="44"/>
-    </row>
-    <row r="74" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B74" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C74" s="30">
-        <v>2</v>
-      </c>
-      <c r="D74" s="31">
-        <v>0</v>
-      </c>
-      <c r="E74" s="31">
-        <v>3</v>
-      </c>
-      <c r="F74" s="31">
-        <v>0</v>
-      </c>
-      <c r="G74" s="36">
-        <v>2</v>
-      </c>
-      <c r="H74" s="32">
-        <v>0</v>
-      </c>
-      <c r="I74" s="45">
-        <v>1</v>
-      </c>
-      <c r="J74" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="K74" s="45">
-        <v>212.5</v>
-      </c>
-      <c r="L74" s="19">
-        <v>0</v>
-      </c>
-      <c r="M74" s="14">
-        <v>1</v>
-      </c>
-      <c r="N74" s="45">
-        <v>120</v>
-      </c>
-      <c r="O74" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="P74" s="14">
-        <v>-240</v>
-      </c>
-      <c r="Q74" s="14">
-        <v>210.5</v>
-      </c>
-      <c r="R74" s="45" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C75" s="27">
-        <v>2</v>
-      </c>
-      <c r="D75" s="28">
-        <v>0</v>
-      </c>
-      <c r="E75" s="28">
-        <v>3</v>
-      </c>
-      <c r="F75" s="28">
-        <v>0</v>
-      </c>
-      <c r="G75" s="37">
-        <v>2</v>
-      </c>
-      <c r="H75" s="29">
-        <v>0</v>
-      </c>
-      <c r="I75" s="44">
-        <v>1</v>
-      </c>
-      <c r="J75" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K75" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L75" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="M75" s="5">
-        <v>1</v>
-      </c>
-      <c r="N75" s="44">
-        <v>60</v>
-      </c>
-      <c r="O75" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P75" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q75" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R75" s="44"/>
-    </row>
-    <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B76" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C76" s="27">
-        <v>2</v>
-      </c>
-      <c r="D76" s="28">
-        <v>0</v>
-      </c>
-      <c r="E76" s="28">
-        <v>3</v>
-      </c>
-      <c r="F76" s="28">
-        <v>0</v>
-      </c>
-      <c r="G76" s="37">
-        <v>2</v>
-      </c>
-      <c r="H76" s="29">
-        <v>0</v>
-      </c>
-      <c r="I76" s="44">
-        <v>1</v>
-      </c>
-      <c r="J76" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K76" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L76" s="18">
-        <v>0</v>
-      </c>
-      <c r="M76" s="5">
-        <v>1</v>
-      </c>
-      <c r="N76" s="44">
-        <v>20</v>
-      </c>
-      <c r="O76" s="18"/>
-      <c r="P76" s="5"/>
-      <c r="Q76" s="5"/>
-      <c r="R76" s="44"/>
-    </row>
-    <row r="77" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B77" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="C77" s="33">
-        <v>2</v>
-      </c>
-      <c r="D77" s="34">
-        <v>0</v>
-      </c>
-      <c r="E77" s="34">
-        <v>3</v>
-      </c>
-      <c r="F77" s="34">
-        <v>0</v>
-      </c>
-      <c r="G77" s="49">
-        <v>2</v>
-      </c>
-      <c r="H77" s="35">
-        <v>0</v>
-      </c>
-      <c r="I77" s="46">
-        <v>1</v>
-      </c>
-      <c r="J77" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="K77" s="46">
-        <v>212.5</v>
-      </c>
-      <c r="L77" s="20">
-        <v>0</v>
-      </c>
-      <c r="M77" s="17">
-        <v>1</v>
-      </c>
-      <c r="N77" s="46">
-        <v>2</v>
-      </c>
-      <c r="O77" s="20"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="17"/>
-      <c r="R77" s="46"/>
-    </row>
-    <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B78" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C78" s="27">
-        <v>3</v>
-      </c>
-      <c r="D78" s="28">
-        <v>0</v>
-      </c>
-      <c r="E78" s="28">
-        <v>0</v>
-      </c>
-      <c r="F78" s="28">
-        <v>0</v>
-      </c>
-      <c r="G78" s="37">
-        <v>2</v>
-      </c>
-      <c r="H78" s="29">
-        <v>0</v>
-      </c>
-      <c r="I78" s="44">
-        <v>1</v>
-      </c>
-      <c r="J78" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="K78" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L78" s="4">
-        <v>0</v>
-      </c>
-      <c r="M78" s="4">
-        <v>1</v>
-      </c>
-      <c r="N78" s="44">
-        <v>120</v>
-      </c>
-      <c r="O78" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="P78" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q78" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R78" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C79" s="27">
-        <v>3</v>
-      </c>
-      <c r="D79" s="28">
-        <v>0</v>
-      </c>
-      <c r="E79" s="28">
-        <v>0</v>
-      </c>
-      <c r="F79" s="28">
-        <v>0</v>
-      </c>
-      <c r="G79" s="37">
-        <v>2</v>
-      </c>
-      <c r="H79" s="29">
-        <v>0</v>
-      </c>
-      <c r="I79" s="44">
-        <v>1</v>
-      </c>
-      <c r="J79" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="K79" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L79" s="4">
-        <v>0</v>
-      </c>
-      <c r="M79" s="4">
-        <v>1</v>
-      </c>
-      <c r="N79" s="44">
-        <v>60</v>
-      </c>
-      <c r="O79" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="P79" s="5">
-        <v>-240</v>
-      </c>
-      <c r="Q79" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="R79" s="5"/>
-    </row>
-    <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B80" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C80" s="27">
-        <v>3</v>
-      </c>
-      <c r="D80" s="28">
-        <v>0</v>
-      </c>
-      <c r="E80" s="28">
-        <v>0</v>
-      </c>
-      <c r="F80" s="28">
-        <v>0</v>
-      </c>
-      <c r="G80" s="37">
-        <v>2</v>
-      </c>
-      <c r="H80" s="29">
-        <v>0</v>
-      </c>
-      <c r="I80" s="44">
-        <v>1</v>
-      </c>
-      <c r="J80" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="K80" s="44">
-        <v>212.5</v>
-      </c>
-      <c r="L80" s="4">
-        <v>0</v>
-      </c>
-      <c r="M80" s="4">
-        <v>1</v>
-      </c>
-      <c r="N80" s="44">
-        <v>20</v>
-      </c>
-      <c r="O80" s="18"/>
-      <c r="P80" s="5"/>
-      <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-    </row>
-    <row r="81" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B81" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="C81" s="38">
-        <v>3</v>
-      </c>
-      <c r="D81" s="39">
-        <v>0</v>
-      </c>
-      <c r="E81" s="39">
-        <v>0</v>
-      </c>
-      <c r="F81" s="39">
-        <v>0</v>
-      </c>
-      <c r="G81" s="40">
-        <v>2</v>
-      </c>
-      <c r="H81" s="41">
-        <v>0</v>
-      </c>
-      <c r="I81" s="47">
-        <v>1</v>
-      </c>
-      <c r="J81" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="K81" s="47">
-        <v>212.5</v>
-      </c>
-      <c r="L81" s="7">
-        <v>0</v>
-      </c>
-      <c r="M81" s="7">
-        <v>1</v>
-      </c>
-      <c r="N81" s="47">
-        <v>2</v>
-      </c>
-      <c r="O81" s="21"/>
-      <c r="P81" s="8"/>
-      <c r="Q81" s="8"/>
-      <c r="R81" s="8"/>
+      <c r="D49" s="39">
+        <v>0</v>
+      </c>
+      <c r="E49" s="39">
+        <v>0</v>
+      </c>
+      <c r="F49" s="39">
+        <v>0</v>
+      </c>
+      <c r="G49" s="40">
+        <v>2</v>
+      </c>
+      <c r="H49" s="41">
+        <v>0</v>
+      </c>
+      <c r="I49" s="47">
+        <v>1</v>
+      </c>
+      <c r="J49" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="K49" s="47">
+        <v>212.5</v>
+      </c>
+      <c r="L49" s="7">
+        <v>0</v>
+      </c>
+      <c r="M49" s="7">
+        <v>1</v>
+      </c>
+      <c r="N49" s="47">
+        <v>2</v>
+      </c>
+      <c r="O49" s="21"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
     </row>
   </sheetData>
   <sortState ref="A3:P76">
@@ -5536,7 +3770,7 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="O1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="R4:R5 J4:P5 J6:R6 A7:R81 A4:I6">
+  <conditionalFormatting sqref="R4:R5 J4:P5 J6:R6 A4:I6 A7:R49">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
@@ -5557,7 +3791,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B49">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Correcting minor error in scenario numbering
git-svn-id: http://svn.niwa.co.nz/repos/SedimentProcesses/delft3d/Research/BankErosionMatlab/Trunk@234 d29393a4-73d2-11e2-8554-73eba5050919
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Sediment_processes\MarieCurie\BankErosionPaper\model\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NIWA-36404-Projects\BankErosion\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -356,7 +356,7 @@
     <t>1c</t>
   </si>
   <si>
-    <t>96c</t>
+    <t>9c</t>
   </si>
 </sst>
 </file>
@@ -1229,10 +1229,10 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Re-run with original Meyer-Peter-Muller
Re-run of the Selwyn based bank erosion sensitivity analysis using the original Meyer-Peter-Muller transport formula (i.e. original coefficients).
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NIWA-36404-Projects\BankErosion\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\XChannel\trunk\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,7 +52,103 @@
         </r>
       </text>
     </comment>
+    <comment ref="N13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard Measures:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Timestep reduced to try and improve stability</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard Measures:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Timestep reduced to try and improve stability</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard Measures:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Timestep reduced to try and improve stability</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="N33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Richard Measures:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Timestep reduced to try and improve stability</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -921,7 +1017,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1229,10 +1353,10 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1474,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="27">
         <v>0</v>
@@ -1406,7 +1530,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="27">
         <v>0</v>
@@ -1460,7 +1584,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1508,7 +1632,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -1556,7 +1680,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="27">
         <v>0</v>
@@ -1606,7 +1730,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="27">
         <v>0</v>
@@ -1656,7 +1780,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="33">
         <v>0</v>
@@ -1706,7 +1830,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="30">
         <v>4</v>
@@ -1762,7 +1886,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="27">
         <v>4</v>
@@ -1816,7 +1940,7 @@
         <v>80</v>
       </c>
       <c r="B12" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="27">
         <v>4</v>
@@ -1864,7 +1988,7 @@
         <v>81</v>
       </c>
       <c r="B13" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="27">
         <v>4</v>
@@ -1900,7 +2024,7 @@
         <v>0.01</v>
       </c>
       <c r="N13" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13" s="18"/>
       <c r="P13" s="5"/>
@@ -1912,7 +2036,7 @@
         <v>43</v>
       </c>
       <c r="B14" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="30">
         <v>3</v>
@@ -1968,7 +2092,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="27">
         <v>3</v>
@@ -2022,7 +2146,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="27">
         <v>3</v>
@@ -2070,7 +2194,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="27">
         <v>3</v>
@@ -2106,7 +2230,7 @@
         <v>0.02</v>
       </c>
       <c r="N17" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="5"/>
@@ -2118,7 +2242,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="30">
         <v>1</v>
@@ -2174,7 +2298,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="27">
         <v>1</v>
@@ -2228,7 +2352,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="27">
         <v>1</v>
@@ -2276,7 +2400,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="27">
         <v>1</v>
@@ -2324,7 +2448,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="30">
         <v>2</v>
@@ -2380,7 +2504,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="27">
         <v>2</v>
@@ -2434,7 +2558,7 @@
         <v>55</v>
       </c>
       <c r="B24" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="27">
         <v>2</v>
@@ -2515,10 +2639,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="4">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="N25" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O25" s="18"/>
       <c r="P25" s="5"/>
@@ -2530,7 +2654,7 @@
         <v>57</v>
       </c>
       <c r="B26" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="30">
         <v>1</v>
@@ -2586,7 +2710,7 @@
         <v>58</v>
       </c>
       <c r="B27" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="27">
         <v>1</v>
@@ -2640,7 +2764,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="27">
         <v>1</v>
@@ -2688,7 +2812,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="27">
         <v>1</v>
@@ -2736,7 +2860,7 @@
         <v>59</v>
       </c>
       <c r="B30" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="30">
         <v>1</v>
@@ -2792,7 +2916,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="27">
         <v>1</v>
@@ -2846,7 +2970,7 @@
         <v>78</v>
       </c>
       <c r="B32" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="27">
         <v>1</v>
@@ -2894,7 +3018,7 @@
         <v>79</v>
       </c>
       <c r="B33" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="27">
         <v>1</v>
@@ -2942,7 +3066,7 @@
         <v>61</v>
       </c>
       <c r="B34" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="30">
         <v>2</v>
@@ -2998,7 +3122,7 @@
         <v>62</v>
       </c>
       <c r="B35" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="27">
         <v>2</v>
@@ -3052,7 +3176,7 @@
         <v>76</v>
       </c>
       <c r="B36" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="27">
         <v>2</v>
@@ -3136,7 +3260,7 @@
         <v>0.1</v>
       </c>
       <c r="N37" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O37" s="18"/>
       <c r="P37" s="5"/>
@@ -3148,7 +3272,7 @@
         <v>63</v>
       </c>
       <c r="B38" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" s="30">
         <v>1</v>
@@ -3204,7 +3328,7 @@
         <v>64</v>
       </c>
       <c r="B39" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" s="27">
         <v>1</v>
@@ -3258,7 +3382,7 @@
         <v>91</v>
       </c>
       <c r="B40" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="27">
         <v>1</v>
@@ -3306,7 +3430,7 @@
         <v>75</v>
       </c>
       <c r="B41" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="27">
         <v>1</v>
@@ -3354,7 +3478,7 @@
         <v>65</v>
       </c>
       <c r="B42" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="30">
         <v>2</v>
@@ -3410,7 +3534,7 @@
         <v>66</v>
       </c>
       <c r="B43" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" s="27">
         <v>2</v>
@@ -3464,7 +3588,7 @@
         <v>73</v>
       </c>
       <c r="B44" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="27">
         <v>2</v>
@@ -3512,7 +3636,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="27">
         <v>2</v>
@@ -3560,7 +3684,7 @@
         <v>67</v>
       </c>
       <c r="B46" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" s="30">
         <v>3</v>
@@ -3616,7 +3740,7 @@
         <v>68</v>
       </c>
       <c r="B47" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="27">
         <v>3</v>
@@ -3670,7 +3794,7 @@
         <v>71</v>
       </c>
       <c r="B48" s="44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" s="27">
         <v>3</v>
@@ -3718,7 +3842,7 @@
         <v>72</v>
       </c>
       <c r="B49" s="47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" s="38">
         <v>3</v>
@@ -3771,22 +3895,22 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="R4:R5 J4:P5 J6:R6 A4:I6 A7:R49">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:R3">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$B5&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Minor tweak to optimisation bounds to improve calibration
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1017,35 +1017,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1353,10 +1325,10 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1446,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="27">
         <v>0</v>
@@ -1530,7 +1502,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="27">
         <v>0</v>
@@ -1584,7 +1556,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -1632,7 +1604,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -1680,7 +1652,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="27">
         <v>0</v>
@@ -1730,7 +1702,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="27">
         <v>0</v>
@@ -1780,7 +1752,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="33">
         <v>0</v>
@@ -1830,7 +1802,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="30">
         <v>4</v>
@@ -1886,7 +1858,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="27">
         <v>4</v>
@@ -1940,7 +1912,7 @@
         <v>80</v>
       </c>
       <c r="B12" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="27">
         <v>4</v>
@@ -1988,7 +1960,7 @@
         <v>81</v>
       </c>
       <c r="B13" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="27">
         <v>4</v>
@@ -2036,7 +2008,7 @@
         <v>43</v>
       </c>
       <c r="B14" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="30">
         <v>3</v>
@@ -2092,7 +2064,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="27">
         <v>3</v>
@@ -2146,7 +2118,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="27">
         <v>3</v>
@@ -2194,7 +2166,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="27">
         <v>3</v>
@@ -2242,7 +2214,7 @@
         <v>46</v>
       </c>
       <c r="B18" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="30">
         <v>1</v>
@@ -2298,7 +2270,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="27">
         <v>1</v>
@@ -2352,7 +2324,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="27">
         <v>1</v>
@@ -2400,7 +2372,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="27">
         <v>1</v>
@@ -2448,7 +2420,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="30">
         <v>2</v>
@@ -2504,7 +2476,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="27">
         <v>2</v>
@@ -2558,7 +2530,7 @@
         <v>55</v>
       </c>
       <c r="B24" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="27">
         <v>2</v>
@@ -2654,7 +2626,7 @@
         <v>57</v>
       </c>
       <c r="B26" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="30">
         <v>1</v>
@@ -2710,7 +2682,7 @@
         <v>58</v>
       </c>
       <c r="B27" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="27">
         <v>1</v>
@@ -2764,7 +2736,7 @@
         <v>69</v>
       </c>
       <c r="B28" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="27">
         <v>1</v>
@@ -2812,7 +2784,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="27">
         <v>1</v>
@@ -2860,7 +2832,7 @@
         <v>59</v>
       </c>
       <c r="B30" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="30">
         <v>1</v>
@@ -2916,7 +2888,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="27">
         <v>1</v>
@@ -2970,7 +2942,7 @@
         <v>78</v>
       </c>
       <c r="B32" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="27">
         <v>1</v>
@@ -3018,7 +2990,7 @@
         <v>79</v>
       </c>
       <c r="B33" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="27">
         <v>1</v>
@@ -3051,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="4">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="N33" s="44">
         <v>1</v>
@@ -3066,7 +3038,7 @@
         <v>61</v>
       </c>
       <c r="B34" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="30">
         <v>2</v>
@@ -3122,7 +3094,7 @@
         <v>62</v>
       </c>
       <c r="B35" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="27">
         <v>2</v>
@@ -3176,7 +3148,7 @@
         <v>76</v>
       </c>
       <c r="B36" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="27">
         <v>2</v>
@@ -3272,7 +3244,7 @@
         <v>63</v>
       </c>
       <c r="B38" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="30">
         <v>1</v>
@@ -3328,7 +3300,7 @@
         <v>64</v>
       </c>
       <c r="B39" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="27">
         <v>1</v>
@@ -3382,7 +3354,7 @@
         <v>91</v>
       </c>
       <c r="B40" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="27">
         <v>1</v>
@@ -3430,7 +3402,7 @@
         <v>75</v>
       </c>
       <c r="B41" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="27">
         <v>1</v>
@@ -3478,7 +3450,7 @@
         <v>65</v>
       </c>
       <c r="B42" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="30">
         <v>2</v>
@@ -3534,7 +3506,7 @@
         <v>66</v>
       </c>
       <c r="B43" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" s="27">
         <v>2</v>
@@ -3588,7 +3560,7 @@
         <v>73</v>
       </c>
       <c r="B44" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="27">
         <v>2</v>
@@ -3636,7 +3608,7 @@
         <v>74</v>
       </c>
       <c r="B45" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="27">
         <v>2</v>
@@ -3684,7 +3656,7 @@
         <v>67</v>
       </c>
       <c r="B46" s="45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="30">
         <v>3</v>
@@ -3740,7 +3712,7 @@
         <v>68</v>
       </c>
       <c r="B47" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="27">
         <v>3</v>
@@ -3794,7 +3766,7 @@
         <v>71</v>
       </c>
       <c r="B48" s="44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="27">
         <v>3</v>
@@ -3842,7 +3814,7 @@
         <v>72</v>
       </c>
       <c r="B49" s="47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="38">
         <v>3</v>
@@ -3895,22 +3867,22 @@
     <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="R4:R5 J4:P5 J6:R6 A4:I6 A7:R49">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:R3">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$B5&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Setting SlipRatio to 1
Setting SlipRatio to 1 for simplicity in the paper as SlipRatio<1 is only required in a 2D situation. Sensitivity analysis shows this does not have a big effect.
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -933,14 +933,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1251,7 +1244,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1367,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="23">
         <v>0</v>
@@ -1398,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K3" s="37" t="s">
         <v>85</v>
@@ -1457,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K4" s="37" t="s">
         <v>20</v>
@@ -1490,7 +1483,7 @@
         <v>90</v>
       </c>
       <c r="B5" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="23">
         <v>0</v>
@@ -1514,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K5" s="37" t="s">
         <v>27</v>
@@ -1541,7 +1534,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="23">
         <v>0</v>
@@ -1565,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K6" s="37" t="s">
         <v>33</v>
@@ -1592,7 +1585,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="23">
         <v>0</v>
@@ -1616,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K7" s="37" t="s">
         <v>20</v>
@@ -1645,7 +1638,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="23">
         <v>0</v>
@@ -1669,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K8" s="37" t="s">
         <v>20</v>
@@ -1698,7 +1691,7 @@
         <v>83</v>
       </c>
       <c r="B9" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="23">
         <v>0</v>
@@ -1722,7 +1715,7 @@
         <v>0.5</v>
       </c>
       <c r="J9" s="37">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K9" s="37" t="s">
         <v>20</v>
@@ -1775,7 +1768,7 @@
         <v>0.5</v>
       </c>
       <c r="J10" s="37">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K10" s="37" t="s">
         <v>20</v>
@@ -1804,7 +1797,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="26">
         <v>4</v>
@@ -1827,7 +1820,9 @@
       <c r="I11" s="38">
         <v>1</v>
       </c>
-      <c r="J11" s="38"/>
+      <c r="J11" s="38">
+        <v>1</v>
+      </c>
       <c r="K11" s="38" t="s">
         <v>85</v>
       </c>
@@ -1861,7 +1856,7 @@
         <v>48</v>
       </c>
       <c r="B12" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="23">
         <v>4</v>
@@ -1884,7 +1879,9 @@
       <c r="I12" s="37">
         <v>1</v>
       </c>
-      <c r="J12" s="37"/>
+      <c r="J12" s="37">
+        <v>1</v>
+      </c>
       <c r="K12" s="37" t="s">
         <v>20</v>
       </c>
@@ -1916,7 +1913,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="23">
         <v>4</v>
@@ -1939,7 +1936,9 @@
       <c r="I13" s="37">
         <v>1</v>
       </c>
-      <c r="J13" s="37"/>
+      <c r="J13" s="37">
+        <v>1</v>
+      </c>
       <c r="K13" s="37" t="s">
         <v>27</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="23">
         <v>4</v>
@@ -1988,7 +1987,9 @@
       <c r="I14" s="37">
         <v>1</v>
       </c>
-      <c r="J14" s="37"/>
+      <c r="J14" s="37">
+        <v>1</v>
+      </c>
       <c r="K14" s="37" t="s">
         <v>33</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="26">
         <v>3</v>
@@ -2037,7 +2038,9 @@
       <c r="I15" s="38">
         <v>1</v>
       </c>
-      <c r="J15" s="38"/>
+      <c r="J15" s="38">
+        <v>1</v>
+      </c>
       <c r="K15" s="38" t="s">
         <v>85</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="23">
         <v>3</v>
@@ -2094,7 +2097,9 @@
       <c r="I16" s="37">
         <v>1</v>
       </c>
-      <c r="J16" s="37"/>
+      <c r="J16" s="37">
+        <v>1</v>
+      </c>
       <c r="K16" s="37" t="s">
         <v>20</v>
       </c>
@@ -2126,7 +2131,7 @@
         <v>45</v>
       </c>
       <c r="B17" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="23">
         <v>3</v>
@@ -2149,7 +2154,9 @@
       <c r="I17" s="37">
         <v>1</v>
       </c>
-      <c r="J17" s="37"/>
+      <c r="J17" s="37">
+        <v>1</v>
+      </c>
       <c r="K17" s="37" t="s">
         <v>27</v>
       </c>
@@ -2175,7 +2182,7 @@
         <v>49</v>
       </c>
       <c r="B18" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="23">
         <v>3</v>
@@ -2198,7 +2205,9 @@
       <c r="I18" s="37">
         <v>1</v>
       </c>
-      <c r="J18" s="37"/>
+      <c r="J18" s="37">
+        <v>1</v>
+      </c>
       <c r="K18" s="37" t="s">
         <v>33</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="26">
         <v>1</v>
@@ -2247,7 +2256,9 @@
       <c r="I19" s="38">
         <v>1</v>
       </c>
-      <c r="J19" s="38"/>
+      <c r="J19" s="38">
+        <v>1</v>
+      </c>
       <c r="K19" s="38" t="s">
         <v>85</v>
       </c>
@@ -2281,7 +2292,7 @@
         <v>50</v>
       </c>
       <c r="B20" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="23">
         <v>1</v>
@@ -2304,7 +2315,9 @@
       <c r="I20" s="37">
         <v>1</v>
       </c>
-      <c r="J20" s="37"/>
+      <c r="J20" s="37">
+        <v>1</v>
+      </c>
       <c r="K20" s="37" t="s">
         <v>20</v>
       </c>
@@ -2336,7 +2349,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="23">
         <v>1</v>
@@ -2359,7 +2372,9 @@
       <c r="I21" s="37">
         <v>1</v>
       </c>
-      <c r="J21" s="37"/>
+      <c r="J21" s="37">
+        <v>1</v>
+      </c>
       <c r="K21" s="37" t="s">
         <v>27</v>
       </c>
@@ -2385,7 +2400,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="23">
         <v>1</v>
@@ -2408,7 +2423,9 @@
       <c r="I22" s="37">
         <v>1</v>
       </c>
-      <c r="J22" s="37"/>
+      <c r="J22" s="37">
+        <v>1</v>
+      </c>
       <c r="K22" s="37" t="s">
         <v>33</v>
       </c>
@@ -2434,7 +2451,7 @@
         <v>53</v>
       </c>
       <c r="B23" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="26">
         <v>2</v>
@@ -2457,7 +2474,9 @@
       <c r="I23" s="38">
         <v>1</v>
       </c>
-      <c r="J23" s="38"/>
+      <c r="J23" s="38">
+        <v>1</v>
+      </c>
       <c r="K23" s="38" t="s">
         <v>85</v>
       </c>
@@ -2491,7 +2510,7 @@
         <v>54</v>
       </c>
       <c r="B24" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="23">
         <v>2</v>
@@ -2514,7 +2533,9 @@
       <c r="I24" s="37">
         <v>1</v>
       </c>
-      <c r="J24" s="37"/>
+      <c r="J24" s="37">
+        <v>1</v>
+      </c>
       <c r="K24" s="37" t="s">
         <v>20</v>
       </c>
@@ -2546,7 +2567,7 @@
         <v>55</v>
       </c>
       <c r="B25" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="23">
         <v>2</v>
@@ -2569,7 +2590,9 @@
       <c r="I25" s="37">
         <v>1</v>
       </c>
-      <c r="J25" s="37"/>
+      <c r="J25" s="37">
+        <v>1</v>
+      </c>
       <c r="K25" s="37" t="s">
         <v>27</v>
       </c>
@@ -2595,7 +2618,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="23">
         <v>2</v>
@@ -2618,7 +2641,9 @@
       <c r="I26" s="37">
         <v>1</v>
       </c>
-      <c r="J26" s="37"/>
+      <c r="J26" s="37">
+        <v>1</v>
+      </c>
       <c r="K26" s="37" t="s">
         <v>33</v>
       </c>
@@ -2644,7 +2669,7 @@
         <v>57</v>
       </c>
       <c r="B27" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="26">
         <v>1</v>
@@ -2667,7 +2692,9 @@
       <c r="I27" s="38">
         <v>1</v>
       </c>
-      <c r="J27" s="38"/>
+      <c r="J27" s="38">
+        <v>1</v>
+      </c>
       <c r="K27" s="38" t="s">
         <v>85</v>
       </c>
@@ -2701,7 +2728,7 @@
         <v>58</v>
       </c>
       <c r="B28" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="23">
         <v>1</v>
@@ -2724,7 +2751,9 @@
       <c r="I28" s="37">
         <v>1</v>
       </c>
-      <c r="J28" s="37"/>
+      <c r="J28" s="37">
+        <v>1</v>
+      </c>
       <c r="K28" s="37" t="s">
         <v>20</v>
       </c>
@@ -2756,7 +2785,7 @@
         <v>69</v>
       </c>
       <c r="B29" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="23">
         <v>1</v>
@@ -2779,7 +2808,9 @@
       <c r="I29" s="37">
         <v>1</v>
       </c>
-      <c r="J29" s="37"/>
+      <c r="J29" s="37">
+        <v>1</v>
+      </c>
       <c r="K29" s="37" t="s">
         <v>27</v>
       </c>
@@ -2805,7 +2836,7 @@
         <v>70</v>
       </c>
       <c r="B30" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="23">
         <v>1</v>
@@ -2828,7 +2859,9 @@
       <c r="I30" s="37">
         <v>1</v>
       </c>
-      <c r="J30" s="37"/>
+      <c r="J30" s="37">
+        <v>1</v>
+      </c>
       <c r="K30" s="37" t="s">
         <v>33</v>
       </c>
@@ -2854,7 +2887,7 @@
         <v>59</v>
       </c>
       <c r="B31" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="26">
         <v>1</v>
@@ -2877,7 +2910,9 @@
       <c r="I31" s="38">
         <v>1</v>
       </c>
-      <c r="J31" s="38"/>
+      <c r="J31" s="38">
+        <v>1</v>
+      </c>
       <c r="K31" s="38" t="s">
         <v>85</v>
       </c>
@@ -2911,7 +2946,7 @@
         <v>60</v>
       </c>
       <c r="B32" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="23">
         <v>1</v>
@@ -2934,7 +2969,9 @@
       <c r="I32" s="37">
         <v>1</v>
       </c>
-      <c r="J32" s="37"/>
+      <c r="J32" s="37">
+        <v>1</v>
+      </c>
       <c r="K32" s="37" t="s">
         <v>20</v>
       </c>
@@ -2966,7 +3003,7 @@
         <v>78</v>
       </c>
       <c r="B33" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" s="23">
         <v>1</v>
@@ -2989,7 +3026,9 @@
       <c r="I33" s="37">
         <v>1</v>
       </c>
-      <c r="J33" s="37"/>
+      <c r="J33" s="37">
+        <v>1</v>
+      </c>
       <c r="K33" s="37" t="s">
         <v>27</v>
       </c>
@@ -3015,7 +3054,7 @@
         <v>79</v>
       </c>
       <c r="B34" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="23">
         <v>1</v>
@@ -3038,7 +3077,9 @@
       <c r="I34" s="37">
         <v>1</v>
       </c>
-      <c r="J34" s="37"/>
+      <c r="J34" s="37">
+        <v>1</v>
+      </c>
       <c r="K34" s="37" t="s">
         <v>33</v>
       </c>
@@ -3064,7 +3105,7 @@
         <v>61</v>
       </c>
       <c r="B35" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="26">
         <v>2</v>
@@ -3087,7 +3128,9 @@
       <c r="I35" s="38">
         <v>1</v>
       </c>
-      <c r="J35" s="38"/>
+      <c r="J35" s="38">
+        <v>1</v>
+      </c>
       <c r="K35" s="38" t="s">
         <v>85</v>
       </c>
@@ -3121,7 +3164,7 @@
         <v>62</v>
       </c>
       <c r="B36" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="23">
         <v>2</v>
@@ -3144,7 +3187,9 @@
       <c r="I36" s="37">
         <v>1</v>
       </c>
-      <c r="J36" s="37"/>
+      <c r="J36" s="37">
+        <v>1</v>
+      </c>
       <c r="K36" s="37" t="s">
         <v>20</v>
       </c>
@@ -3176,7 +3221,7 @@
         <v>76</v>
       </c>
       <c r="B37" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="23">
         <v>2</v>
@@ -3199,7 +3244,9 @@
       <c r="I37" s="37">
         <v>1</v>
       </c>
-      <c r="J37" s="37"/>
+      <c r="J37" s="37">
+        <v>1</v>
+      </c>
       <c r="K37" s="37" t="s">
         <v>27</v>
       </c>
@@ -3225,7 +3272,7 @@
         <v>77</v>
       </c>
       <c r="B38" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="23">
         <v>2</v>
@@ -3248,7 +3295,9 @@
       <c r="I38" s="37">
         <v>1</v>
       </c>
-      <c r="J38" s="37"/>
+      <c r="J38" s="37">
+        <v>1</v>
+      </c>
       <c r="K38" s="37" t="s">
         <v>33</v>
       </c>
@@ -3274,7 +3323,7 @@
         <v>63</v>
       </c>
       <c r="B39" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="26">
         <v>1</v>
@@ -3297,7 +3346,9 @@
       <c r="I39" s="38">
         <v>1</v>
       </c>
-      <c r="J39" s="38"/>
+      <c r="J39" s="38">
+        <v>1</v>
+      </c>
       <c r="K39" s="38" t="s">
         <v>85</v>
       </c>
@@ -3331,7 +3382,7 @@
         <v>64</v>
       </c>
       <c r="B40" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="23">
         <v>1</v>
@@ -3354,7 +3405,9 @@
       <c r="I40" s="37">
         <v>1</v>
       </c>
-      <c r="J40" s="37"/>
+      <c r="J40" s="37">
+        <v>1</v>
+      </c>
       <c r="K40" s="37" t="s">
         <v>20</v>
       </c>
@@ -3386,7 +3439,7 @@
         <v>91</v>
       </c>
       <c r="B41" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="23">
         <v>1</v>
@@ -3409,7 +3462,9 @@
       <c r="I41" s="37">
         <v>1</v>
       </c>
-      <c r="J41" s="37"/>
+      <c r="J41" s="37">
+        <v>1</v>
+      </c>
       <c r="K41" s="37" t="s">
         <v>27</v>
       </c>
@@ -3435,7 +3490,7 @@
         <v>75</v>
       </c>
       <c r="B42" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="23">
         <v>1</v>
@@ -3458,7 +3513,9 @@
       <c r="I42" s="37">
         <v>1</v>
       </c>
-      <c r="J42" s="37"/>
+      <c r="J42" s="37">
+        <v>1</v>
+      </c>
       <c r="K42" s="37" t="s">
         <v>33</v>
       </c>
@@ -3484,7 +3541,7 @@
         <v>65</v>
       </c>
       <c r="B43" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" s="26">
         <v>2</v>
@@ -3507,7 +3564,9 @@
       <c r="I43" s="38">
         <v>1</v>
       </c>
-      <c r="J43" s="38"/>
+      <c r="J43" s="38">
+        <v>1</v>
+      </c>
       <c r="K43" s="38" t="s">
         <v>85</v>
       </c>
@@ -3541,7 +3600,7 @@
         <v>66</v>
       </c>
       <c r="B44" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="23">
         <v>2</v>
@@ -3564,7 +3623,9 @@
       <c r="I44" s="37">
         <v>1</v>
       </c>
-      <c r="J44" s="37"/>
+      <c r="J44" s="37">
+        <v>1</v>
+      </c>
       <c r="K44" s="37" t="s">
         <v>20</v>
       </c>
@@ -3596,7 +3657,7 @@
         <v>73</v>
       </c>
       <c r="B45" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" s="23">
         <v>2</v>
@@ -3619,7 +3680,9 @@
       <c r="I45" s="37">
         <v>1</v>
       </c>
-      <c r="J45" s="37"/>
+      <c r="J45" s="37">
+        <v>1</v>
+      </c>
       <c r="K45" s="37" t="s">
         <v>27</v>
       </c>
@@ -3645,7 +3708,7 @@
         <v>74</v>
       </c>
       <c r="B46" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="23">
         <v>2</v>
@@ -3668,7 +3731,9 @@
       <c r="I46" s="37">
         <v>1</v>
       </c>
-      <c r="J46" s="37"/>
+      <c r="J46" s="37">
+        <v>1</v>
+      </c>
       <c r="K46" s="37" t="s">
         <v>33</v>
       </c>
@@ -3694,7 +3759,7 @@
         <v>67</v>
       </c>
       <c r="B47" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="26">
         <v>3</v>
@@ -3717,7 +3782,9 @@
       <c r="I47" s="38">
         <v>1</v>
       </c>
-      <c r="J47" s="38"/>
+      <c r="J47" s="38">
+        <v>1</v>
+      </c>
       <c r="K47" s="38" t="s">
         <v>85</v>
       </c>
@@ -3751,7 +3818,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="23">
         <v>3</v>
@@ -3774,7 +3841,9 @@
       <c r="I48" s="37">
         <v>1</v>
       </c>
-      <c r="J48" s="37"/>
+      <c r="J48" s="37">
+        <v>1</v>
+      </c>
       <c r="K48" s="37" t="s">
         <v>20</v>
       </c>
@@ -3806,7 +3875,7 @@
         <v>71</v>
       </c>
       <c r="B49" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="23">
         <v>3</v>
@@ -3829,7 +3898,9 @@
       <c r="I49" s="37">
         <v>1</v>
       </c>
-      <c r="J49" s="37"/>
+      <c r="J49" s="37">
+        <v>1</v>
+      </c>
       <c r="K49" s="37" t="s">
         <v>27</v>
       </c>
@@ -3855,7 +3926,7 @@
         <v>72</v>
       </c>
       <c r="B50" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" s="31">
         <v>3</v>
@@ -3878,7 +3949,9 @@
       <c r="I50" s="39">
         <v>1</v>
       </c>
-      <c r="J50" s="39"/>
+      <c r="J50" s="39">
+        <v>1</v>
+      </c>
       <c r="K50" s="39" t="s">
         <v>33</v>
       </c>
@@ -3909,22 +3982,22 @@
     <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="S4:S5 K4:Q5 K6:S6 A4:J6 A7:S50">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:S3">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B5&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding sensitivity test for varying bend radius across cross-section (scenario 1i)
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
     <author>Richard Measures</author>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O14" authorId="0" shapeId="0">
+    <comment ref="Q15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O18" authorId="0" shapeId="0">
+    <comment ref="Q19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O26" authorId="0" shapeId="0">
+    <comment ref="Q27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O34" authorId="0" shapeId="0">
+    <comment ref="Q35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O38" authorId="0" shapeId="0">
+    <comment ref="Q39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="99">
   <si>
     <t>Stencil</t>
   </si>
@@ -462,12 +462,24 @@
   </si>
   <si>
     <t>SlipRatio</t>
+  </si>
+  <si>
+    <t>ConstBend</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>1i</t>
+  </si>
+  <si>
+    <t>Slope - ConstBend sensitivity check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1051,6 +1063,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1086,6 +1115,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1238,13 +1284,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S10" sqref="S10"/>
+      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,17 +1300,19 @@
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.5703125" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42"/>
       <c r="B1" s="35"/>
       <c r="C1" s="18" t="s">
@@ -1285,25 +1333,27 @@
       </c>
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="45" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="35" t="s">
+      <c r="P1" s="45"/>
+      <c r="Q1" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="R1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S1" s="47"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
@@ -1335,34 +1385,40 @@
         <v>94</v>
       </c>
       <c r="K2" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="N2" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="O2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="P2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="Q2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -1393,35 +1449,41 @@
       <c r="J3" s="37">
         <v>1</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="37">
+        <v>1</v>
+      </c>
+      <c r="L3" s="37">
+        <v>185</v>
+      </c>
+      <c r="M3" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="N3" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O3" s="4">
         <v>0.1</v>
       </c>
-      <c r="N3" s="4">
+      <c r="P3" s="4">
         <v>0.5</v>
       </c>
-      <c r="O3" s="37">
+      <c r="Q3" s="37">
         <v>120</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="R3" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="S3" s="5">
         <v>-240</v>
       </c>
-      <c r="R3" s="5">
+      <c r="T3" s="5">
         <v>210.5</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
@@ -1452,33 +1514,39 @@
       <c r="J4" s="37">
         <v>1</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="37">
+        <v>1</v>
+      </c>
+      <c r="L4" s="37">
+        <v>185</v>
+      </c>
+      <c r="M4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="N4" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O4" s="4">
         <v>0.1</v>
       </c>
-      <c r="N4" s="4">
+      <c r="P4" s="4">
         <v>2</v>
       </c>
-      <c r="O4" s="37">
+      <c r="Q4" s="37">
         <v>60</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="R4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="S4" s="5">
         <v>-240</v>
       </c>
-      <c r="R4" s="5">
+      <c r="T4" s="5">
         <v>210.5</v>
       </c>
-      <c r="S4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>90</v>
       </c>
@@ -1509,27 +1577,33 @@
       <c r="J5" s="37">
         <v>1</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="37">
+        <v>1</v>
+      </c>
+      <c r="L5" s="37">
+        <v>185</v>
+      </c>
+      <c r="M5" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M5" s="4">
+      <c r="N5" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O5" s="4">
         <v>0.1</v>
       </c>
-      <c r="N5" s="4">
+      <c r="P5" s="4">
         <v>2</v>
       </c>
-      <c r="O5" s="37">
+      <c r="Q5" s="37">
         <v>20</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
+      <c r="R5" s="15"/>
       <c r="S5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
@@ -1560,27 +1634,33 @@
       <c r="J6" s="37">
         <v>1</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="37">
+        <v>1</v>
+      </c>
+      <c r="L6" s="37">
+        <v>185</v>
+      </c>
+      <c r="M6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="N6" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O6" s="4">
         <v>2</v>
       </c>
-      <c r="N6" s="4">
+      <c r="P6" s="4">
         <v>8</v>
       </c>
-      <c r="O6" s="37">
+      <c r="Q6" s="37">
         <v>2</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
+      <c r="R6" s="15"/>
       <c r="S6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
@@ -1611,29 +1691,35 @@
       <c r="J7" s="37">
         <v>1</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="37">
+        <v>1</v>
+      </c>
+      <c r="L7" s="37">
+        <v>185</v>
+      </c>
+      <c r="M7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M7" s="4">
+      <c r="N7" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O7" s="4">
         <v>0.1</v>
       </c>
-      <c r="N7" s="4">
+      <c r="P7" s="4">
         <v>2</v>
       </c>
-      <c r="O7" s="37">
+      <c r="Q7" s="37">
         <v>120</v>
       </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5" t="s">
+      <c r="R7" s="15"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -1664,29 +1750,35 @@
       <c r="J8" s="37">
         <v>1</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="37">
+        <v>1</v>
+      </c>
+      <c r="L8" s="37">
+        <v>185</v>
+      </c>
+      <c r="M8" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M8" s="4">
+      <c r="N8" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O8" s="4">
         <v>0.1</v>
       </c>
-      <c r="N8" s="4">
+      <c r="P8" s="4">
         <v>2</v>
       </c>
-      <c r="O8" s="37">
+      <c r="Q8" s="37">
         <v>2</v>
       </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5" t="s">
+      <c r="R8" s="15"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
@@ -1717,29 +1809,35 @@
       <c r="J9" s="37">
         <v>1</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="37">
+        <v>1</v>
+      </c>
+      <c r="L9" s="37">
+        <v>185</v>
+      </c>
+      <c r="M9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M9" s="4">
+      <c r="N9" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O9" s="4">
         <v>0.1</v>
       </c>
-      <c r="N9" s="4">
+      <c r="P9" s="4">
         <v>2</v>
       </c>
-      <c r="O9" s="37">
+      <c r="Q9" s="37">
         <v>60</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5" t="s">
+      <c r="R9" s="15"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>92</v>
       </c>
@@ -1765,152 +1863,172 @@
         <v>0</v>
       </c>
       <c r="I10" s="37">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J10" s="37">
         <v>0.25</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="37">
+        <v>1</v>
+      </c>
+      <c r="L10" s="37">
+        <v>185</v>
+      </c>
+      <c r="M10" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M10" s="4">
+      <c r="N10" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O10" s="4">
         <v>0.1</v>
       </c>
-      <c r="N10" s="4">
+      <c r="P10" s="4">
         <v>2</v>
       </c>
-      <c r="O10" s="37">
+      <c r="Q10" s="37">
         <v>60</v>
       </c>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5" t="s">
+      <c r="R10" s="15"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:21" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="23">
+        <v>0</v>
+      </c>
+      <c r="D11" s="24">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0</v>
+      </c>
+      <c r="F11" s="24">
+        <v>0</v>
+      </c>
+      <c r="G11" s="24">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25">
+        <v>0</v>
+      </c>
+      <c r="I11" s="37">
+        <v>1</v>
+      </c>
+      <c r="J11" s="37">
+        <v>1</v>
+      </c>
+      <c r="K11" s="37">
+        <v>0</v>
+      </c>
+      <c r="L11" s="37">
+        <v>115</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="P11" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="37">
+        <v>60</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T11" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="26">
+      <c r="B12" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="26">
         <v>4</v>
       </c>
-      <c r="D11" s="27">
-        <v>0</v>
-      </c>
-      <c r="E11" s="27">
-        <v>0</v>
-      </c>
-      <c r="F11" s="27">
-        <v>0</v>
-      </c>
-      <c r="G11" s="29">
+      <c r="D12" s="27">
+        <v>0</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="29">
         <v>3</v>
       </c>
-      <c r="H11" s="28">
-        <v>0</v>
-      </c>
-      <c r="I11" s="38">
-        <v>1</v>
-      </c>
-      <c r="J11" s="38">
-        <v>1</v>
-      </c>
-      <c r="K11" s="38" t="s">
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="38">
+        <v>1</v>
+      </c>
+      <c r="J12" s="38">
+        <v>1</v>
+      </c>
+      <c r="K12" s="38">
+        <v>1</v>
+      </c>
+      <c r="L12" s="38">
+        <v>185</v>
+      </c>
+      <c r="M12" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L11" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M11" s="13">
-        <v>0</v>
-      </c>
-      <c r="N11" s="13">
+      <c r="N12" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O12" s="13">
+        <v>0</v>
+      </c>
+      <c r="P12" s="13">
         <v>0.1</v>
       </c>
-      <c r="O11" s="38">
+      <c r="Q12" s="38">
         <v>120</v>
       </c>
-      <c r="P11" s="16" t="s">
+      <c r="R12" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="S12" s="14">
         <v>-240</v>
       </c>
-      <c r="R11" s="14">
+      <c r="T12" s="14">
         <v>210.5</v>
       </c>
-      <c r="S11" s="38" t="s">
+      <c r="U12" s="38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="23">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24">
-        <v>0</v>
-      </c>
-      <c r="E12" s="24">
-        <v>0</v>
-      </c>
-      <c r="F12" s="24">
-        <v>0</v>
-      </c>
-      <c r="G12" s="30">
-        <v>3</v>
-      </c>
-      <c r="H12" s="25">
-        <v>0</v>
-      </c>
-      <c r="I12" s="37">
-        <v>1</v>
-      </c>
-      <c r="J12" s="37">
-        <v>1</v>
-      </c>
-      <c r="K12" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O12" s="37">
-        <v>60</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R12" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S12" s="37"/>
-    </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="B13" s="37" t="b">
         <v>1</v>
@@ -1939,29 +2057,41 @@
       <c r="J13" s="37">
         <v>1</v>
       </c>
-      <c r="K13" s="37" t="s">
-        <v>27</v>
+      <c r="K13" s="37">
+        <v>1</v>
       </c>
       <c r="L13" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
+        <v>185</v>
+      </c>
+      <c r="M13" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
         <v>0.1</v>
       </c>
-      <c r="O13" s="37">
-        <v>20</v>
-      </c>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="37"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q13" s="37">
+        <v>60</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T13" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U13" s="37"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="37" t="b">
         <v>1</v>
@@ -1990,145 +2120,157 @@
       <c r="J14" s="37">
         <v>1</v>
       </c>
-      <c r="K14" s="37" t="s">
+      <c r="K14" s="37">
+        <v>1</v>
+      </c>
+      <c r="L14" s="37">
+        <v>185</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q14" s="37">
+        <v>20</v>
+      </c>
+      <c r="R14" s="15"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="37"/>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="23">
+        <v>4</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30">
+        <v>3</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0</v>
+      </c>
+      <c r="I15" s="37">
+        <v>1</v>
+      </c>
+      <c r="J15" s="37">
+        <v>1</v>
+      </c>
+      <c r="K15" s="37">
+        <v>1</v>
+      </c>
+      <c r="L15" s="37">
+        <v>185</v>
+      </c>
+      <c r="M15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
+      <c r="N15" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
         <v>0.01</v>
       </c>
-      <c r="O14" s="37">
-        <v>1</v>
-      </c>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="37"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="Q15" s="37">
+        <v>1</v>
+      </c>
+      <c r="R15" s="15"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="37"/>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="26">
+      <c r="B16" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="26">
         <v>3</v>
       </c>
-      <c r="D15" s="27">
-        <v>0</v>
-      </c>
-      <c r="E15" s="27">
-        <v>0</v>
-      </c>
-      <c r="F15" s="27">
-        <v>0</v>
-      </c>
-      <c r="G15" s="29">
+      <c r="D16" s="27">
+        <v>0</v>
+      </c>
+      <c r="E16" s="27">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>0</v>
+      </c>
+      <c r="G16" s="29">
         <v>3</v>
       </c>
-      <c r="H15" s="28">
-        <v>0</v>
-      </c>
-      <c r="I15" s="38">
-        <v>1</v>
-      </c>
-      <c r="J15" s="38">
-        <v>1</v>
-      </c>
-      <c r="K15" s="38" t="s">
+      <c r="H16" s="28">
+        <v>0</v>
+      </c>
+      <c r="I16" s="38">
+        <v>1</v>
+      </c>
+      <c r="J16" s="38">
+        <v>1</v>
+      </c>
+      <c r="K16" s="38">
+        <v>1</v>
+      </c>
+      <c r="L16" s="38">
+        <v>185</v>
+      </c>
+      <c r="M16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L15" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M15" s="13">
-        <v>0</v>
-      </c>
-      <c r="N15" s="13">
+      <c r="N16" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O16" s="13">
+        <v>0</v>
+      </c>
+      <c r="P16" s="13">
         <v>0.1</v>
       </c>
-      <c r="O15" s="38">
+      <c r="Q16" s="38">
         <v>120</v>
       </c>
-      <c r="P15" s="16" t="s">
+      <c r="R16" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="S16" s="14">
         <v>-240</v>
       </c>
-      <c r="R15" s="14">
+      <c r="T16" s="14">
         <v>210.5</v>
       </c>
-      <c r="S15" s="38" t="s">
+      <c r="U16" s="38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="23">
-        <v>3</v>
-      </c>
-      <c r="D16" s="24">
-        <v>0</v>
-      </c>
-      <c r="E16" s="24">
-        <v>0</v>
-      </c>
-      <c r="F16" s="24">
-        <v>0</v>
-      </c>
-      <c r="G16" s="30">
-        <v>3</v>
-      </c>
-      <c r="H16" s="25">
-        <v>0</v>
-      </c>
-      <c r="I16" s="37">
-        <v>1</v>
-      </c>
-      <c r="J16" s="37">
-        <v>1</v>
-      </c>
-      <c r="K16" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O16" s="37">
-        <v>60</v>
-      </c>
-      <c r="P16" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R16" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S16" s="37"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="B17" s="37" t="b">
         <v>1</v>
@@ -2157,29 +2299,41 @@
       <c r="J17" s="37">
         <v>1</v>
       </c>
-      <c r="K17" s="37" t="s">
-        <v>27</v>
+      <c r="K17" s="37">
+        <v>1</v>
       </c>
       <c r="L17" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
+        <v>185</v>
+      </c>
+      <c r="M17" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
         <v>0.1</v>
       </c>
-      <c r="O17" s="37">
-        <v>20</v>
-      </c>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="37"/>
-    </row>
-    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q17" s="37">
+        <v>60</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T17" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U17" s="37"/>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="37" t="b">
         <v>1</v>
@@ -2208,145 +2362,157 @@
       <c r="J18" s="37">
         <v>1</v>
       </c>
-      <c r="K18" s="37" t="s">
+      <c r="K18" s="37">
+        <v>1</v>
+      </c>
+      <c r="L18" s="37">
+        <v>185</v>
+      </c>
+      <c r="M18" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q18" s="37">
+        <v>20</v>
+      </c>
+      <c r="R18" s="15"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="37"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="23">
+        <v>3</v>
+      </c>
+      <c r="D19" s="24">
+        <v>0</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0</v>
+      </c>
+      <c r="F19" s="24">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30">
+        <v>3</v>
+      </c>
+      <c r="H19" s="25">
+        <v>0</v>
+      </c>
+      <c r="I19" s="37">
+        <v>1</v>
+      </c>
+      <c r="J19" s="37">
+        <v>1</v>
+      </c>
+      <c r="K19" s="37">
+        <v>1</v>
+      </c>
+      <c r="L19" s="37">
+        <v>185</v>
+      </c>
+      <c r="M19" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-      <c r="N18" s="4">
+      <c r="N19" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
         <v>0.02</v>
       </c>
-      <c r="O18" s="37">
-        <v>1</v>
-      </c>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="37"/>
-    </row>
-    <row r="19" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="Q19" s="37">
+        <v>1</v>
+      </c>
+      <c r="R19" s="15"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="37"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" s="26">
-        <v>1</v>
-      </c>
-      <c r="D19" s="27">
-        <v>0</v>
-      </c>
-      <c r="E19" s="27">
-        <v>0</v>
-      </c>
-      <c r="F19" s="27">
-        <v>0</v>
-      </c>
-      <c r="G19" s="29">
+      <c r="B20" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" s="26">
+        <v>1</v>
+      </c>
+      <c r="D20" s="27">
+        <v>0</v>
+      </c>
+      <c r="E20" s="27">
+        <v>0</v>
+      </c>
+      <c r="F20" s="27">
+        <v>0</v>
+      </c>
+      <c r="G20" s="29">
         <v>3</v>
       </c>
-      <c r="H19" s="28">
-        <v>0</v>
-      </c>
-      <c r="I19" s="38">
-        <v>1</v>
-      </c>
-      <c r="J19" s="38">
-        <v>1</v>
-      </c>
-      <c r="K19" s="38" t="s">
+      <c r="H20" s="28">
+        <v>0</v>
+      </c>
+      <c r="I20" s="38">
+        <v>1</v>
+      </c>
+      <c r="J20" s="38">
+        <v>1</v>
+      </c>
+      <c r="K20" s="38">
+        <v>1</v>
+      </c>
+      <c r="L20" s="38">
+        <v>185</v>
+      </c>
+      <c r="M20" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L19" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M19" s="13">
-        <v>0</v>
-      </c>
-      <c r="N19" s="13">
+      <c r="N20" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O20" s="13">
+        <v>0</v>
+      </c>
+      <c r="P20" s="13">
         <v>0.1</v>
       </c>
-      <c r="O19" s="38">
+      <c r="Q20" s="38">
         <v>120</v>
       </c>
-      <c r="P19" s="16" t="s">
+      <c r="R20" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="S20" s="14">
         <v>-240</v>
       </c>
-      <c r="R19" s="14">
+      <c r="T20" s="14">
         <v>210.5</v>
       </c>
-      <c r="S19" s="38" t="s">
+      <c r="U20" s="38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="23">
-        <v>1</v>
-      </c>
-      <c r="D20" s="24">
-        <v>0</v>
-      </c>
-      <c r="E20" s="24">
-        <v>0</v>
-      </c>
-      <c r="F20" s="24">
-        <v>0</v>
-      </c>
-      <c r="G20" s="30">
-        <v>3</v>
-      </c>
-      <c r="H20" s="25">
-        <v>0</v>
-      </c>
-      <c r="I20" s="37">
-        <v>1</v>
-      </c>
-      <c r="J20" s="37">
-        <v>1</v>
-      </c>
-      <c r="K20" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M20" s="4">
-        <v>0</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O20" s="37">
-        <v>60</v>
-      </c>
-      <c r="P20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R20" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S20" s="37"/>
-    </row>
-    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="B21" s="37" t="b">
         <v>1</v>
@@ -2375,29 +2541,41 @@
       <c r="J21" s="37">
         <v>1</v>
       </c>
-      <c r="K21" s="37" t="s">
-        <v>27</v>
+      <c r="K21" s="37">
+        <v>1</v>
       </c>
       <c r="L21" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0</v>
-      </c>
-      <c r="N21" s="4">
+        <v>185</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
         <v>0.1</v>
       </c>
-      <c r="O21" s="37">
-        <v>20</v>
-      </c>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="37"/>
-    </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q21" s="37">
+        <v>60</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S21" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T21" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U21" s="37"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="37" t="b">
         <v>1</v>
@@ -2426,145 +2604,157 @@
       <c r="J22" s="37">
         <v>1</v>
       </c>
-      <c r="K22" s="37" t="s">
+      <c r="K22" s="37">
+        <v>1</v>
+      </c>
+      <c r="L22" s="37">
+        <v>185</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q22" s="37">
+        <v>20</v>
+      </c>
+      <c r="R22" s="15"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="37"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0</v>
+      </c>
+      <c r="G23" s="30">
+        <v>3</v>
+      </c>
+      <c r="H23" s="25">
+        <v>0</v>
+      </c>
+      <c r="I23" s="37">
+        <v>1</v>
+      </c>
+      <c r="J23" s="37">
+        <v>1</v>
+      </c>
+      <c r="K23" s="37">
+        <v>1</v>
+      </c>
+      <c r="L23" s="37">
+        <v>185</v>
+      </c>
+      <c r="M23" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L22" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0</v>
-      </c>
-      <c r="N22" s="4">
+      <c r="N23" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
         <v>0.1</v>
       </c>
-      <c r="O22" s="37">
+      <c r="Q23" s="37">
         <v>2</v>
       </c>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="37"/>
-    </row>
-    <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="R23" s="15"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="37"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C23" s="26">
+      <c r="B24" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" s="26">
         <v>2</v>
       </c>
-      <c r="D23" s="27">
-        <v>0</v>
-      </c>
-      <c r="E23" s="27">
-        <v>0</v>
-      </c>
-      <c r="F23" s="27">
-        <v>0</v>
-      </c>
-      <c r="G23" s="29">
+      <c r="D24" s="27">
+        <v>0</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27">
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
         <v>3</v>
       </c>
-      <c r="H23" s="28">
-        <v>0</v>
-      </c>
-      <c r="I23" s="38">
-        <v>1</v>
-      </c>
-      <c r="J23" s="38">
-        <v>1</v>
-      </c>
-      <c r="K23" s="38" t="s">
+      <c r="H24" s="28">
+        <v>0</v>
+      </c>
+      <c r="I24" s="38">
+        <v>1</v>
+      </c>
+      <c r="J24" s="38">
+        <v>1</v>
+      </c>
+      <c r="K24" s="38">
+        <v>1</v>
+      </c>
+      <c r="L24" s="38">
+        <v>185</v>
+      </c>
+      <c r="M24" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L23" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M23" s="13">
-        <v>0</v>
-      </c>
-      <c r="N23" s="13">
+      <c r="N24" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O24" s="13">
+        <v>0</v>
+      </c>
+      <c r="P24" s="13">
         <v>0.1</v>
       </c>
-      <c r="O23" s="38">
+      <c r="Q24" s="38">
         <v>120</v>
       </c>
-      <c r="P23" s="16" t="s">
+      <c r="R24" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q23" s="14">
+      <c r="S24" s="14">
         <v>-240</v>
       </c>
-      <c r="R23" s="14">
+      <c r="T24" s="14">
         <v>210.5</v>
       </c>
-      <c r="S23" s="38" t="s">
+      <c r="U24" s="38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" s="23">
-        <v>2</v>
-      </c>
-      <c r="D24" s="24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="24">
-        <v>0</v>
-      </c>
-      <c r="F24" s="24">
-        <v>0</v>
-      </c>
-      <c r="G24" s="30">
-        <v>3</v>
-      </c>
-      <c r="H24" s="25">
-        <v>0</v>
-      </c>
-      <c r="I24" s="37">
-        <v>1</v>
-      </c>
-      <c r="J24" s="37">
-        <v>1</v>
-      </c>
-      <c r="K24" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O24" s="37">
-        <v>60</v>
-      </c>
-      <c r="P24" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q24" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R24" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S24" s="37"/>
-    </row>
-    <row r="25" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="B25" s="37" t="b">
         <v>1</v>
@@ -2593,29 +2783,41 @@
       <c r="J25" s="37">
         <v>1</v>
       </c>
-      <c r="K25" s="37" t="s">
-        <v>27</v>
+      <c r="K25" s="37">
+        <v>1</v>
       </c>
       <c r="L25" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M25" s="4">
-        <v>0</v>
-      </c>
-      <c r="N25" s="4">
+        <v>185</v>
+      </c>
+      <c r="M25" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0</v>
+      </c>
+      <c r="P25" s="4">
         <v>0.1</v>
       </c>
-      <c r="O25" s="37">
-        <v>20</v>
-      </c>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="37"/>
-    </row>
-    <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q25" s="37">
+        <v>60</v>
+      </c>
+      <c r="R25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S25" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T25" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U25" s="37"/>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="37" t="b">
         <v>1</v>
@@ -2644,145 +2846,157 @@
       <c r="J26" s="37">
         <v>1</v>
       </c>
-      <c r="K26" s="37" t="s">
+      <c r="K26" s="37">
+        <v>1</v>
+      </c>
+      <c r="L26" s="37">
+        <v>185</v>
+      </c>
+      <c r="M26" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0</v>
+      </c>
+      <c r="P26" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q26" s="37">
+        <v>20</v>
+      </c>
+      <c r="R26" s="15"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="37"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="23">
+        <v>2</v>
+      </c>
+      <c r="D27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="24">
+        <v>0</v>
+      </c>
+      <c r="F27" s="24">
+        <v>0</v>
+      </c>
+      <c r="G27" s="30">
+        <v>3</v>
+      </c>
+      <c r="H27" s="25">
+        <v>0</v>
+      </c>
+      <c r="I27" s="37">
+        <v>1</v>
+      </c>
+      <c r="J27" s="37">
+        <v>1</v>
+      </c>
+      <c r="K27" s="37">
+        <v>1</v>
+      </c>
+      <c r="L27" s="37">
+        <v>185</v>
+      </c>
+      <c r="M27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L26" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0</v>
-      </c>
-      <c r="N26" s="4">
+      <c r="N27" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
         <v>0.02</v>
       </c>
-      <c r="O26" s="37">
-        <v>1</v>
-      </c>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="37"/>
-    </row>
-    <row r="27" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="Q27" s="37">
+        <v>1</v>
+      </c>
+      <c r="R27" s="15"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="37"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C27" s="26">
-        <v>1</v>
-      </c>
-      <c r="D27" s="27">
-        <v>0</v>
-      </c>
-      <c r="E27" s="27">
-        <v>0</v>
-      </c>
-      <c r="F27" s="27">
-        <v>0</v>
-      </c>
-      <c r="G27" s="29">
+      <c r="B28" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C28" s="26">
+        <v>1</v>
+      </c>
+      <c r="D28" s="27">
+        <v>0</v>
+      </c>
+      <c r="E28" s="27">
+        <v>0</v>
+      </c>
+      <c r="F28" s="27">
+        <v>0</v>
+      </c>
+      <c r="G28" s="29">
         <v>4</v>
       </c>
-      <c r="H27" s="28">
-        <v>0</v>
-      </c>
-      <c r="I27" s="38">
-        <v>1</v>
-      </c>
-      <c r="J27" s="38">
-        <v>1</v>
-      </c>
-      <c r="K27" s="38" t="s">
+      <c r="H28" s="28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="38">
+        <v>1</v>
+      </c>
+      <c r="J28" s="38">
+        <v>1</v>
+      </c>
+      <c r="K28" s="38">
+        <v>1</v>
+      </c>
+      <c r="L28" s="38">
+        <v>185</v>
+      </c>
+      <c r="M28" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L27" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M27" s="13">
-        <v>0</v>
-      </c>
-      <c r="N27" s="13">
+      <c r="N28" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O28" s="13">
+        <v>0</v>
+      </c>
+      <c r="P28" s="13">
         <v>0.1</v>
       </c>
-      <c r="O27" s="38">
+      <c r="Q28" s="38">
         <v>120</v>
       </c>
-      <c r="P27" s="16" t="s">
+      <c r="R28" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q27" s="14">
+      <c r="S28" s="14">
         <v>-240</v>
       </c>
-      <c r="R27" s="14">
+      <c r="T28" s="14">
         <v>210.5</v>
       </c>
-      <c r="S27" s="38" t="s">
+      <c r="U28" s="38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B28" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" s="23">
-        <v>1</v>
-      </c>
-      <c r="D28" s="24">
-        <v>0</v>
-      </c>
-      <c r="E28" s="24">
-        <v>0</v>
-      </c>
-      <c r="F28" s="24">
-        <v>0</v>
-      </c>
-      <c r="G28" s="30">
-        <v>4</v>
-      </c>
-      <c r="H28" s="25">
-        <v>0</v>
-      </c>
-      <c r="I28" s="37">
-        <v>1</v>
-      </c>
-      <c r="J28" s="37">
-        <v>1</v>
-      </c>
-      <c r="K28" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0</v>
-      </c>
-      <c r="N28" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O28" s="37">
-        <v>60</v>
-      </c>
-      <c r="P28" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q28" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R28" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S28" s="37"/>
-    </row>
-    <row r="29" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="B29" s="37" t="b">
         <v>1</v>
@@ -2811,29 +3025,41 @@
       <c r="J29" s="37">
         <v>1</v>
       </c>
-      <c r="K29" s="37" t="s">
-        <v>27</v>
+      <c r="K29" s="37">
+        <v>1</v>
       </c>
       <c r="L29" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M29" s="4">
-        <v>0</v>
-      </c>
-      <c r="N29" s="4">
+        <v>185</v>
+      </c>
+      <c r="M29" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N29" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4">
         <v>0.1</v>
       </c>
-      <c r="O29" s="37">
-        <v>20</v>
-      </c>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="37"/>
-    </row>
-    <row r="30" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q29" s="37">
+        <v>60</v>
+      </c>
+      <c r="R29" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S29" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T29" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U29" s="37"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="37" t="b">
         <v>1</v>
@@ -2862,145 +3088,157 @@
       <c r="J30" s="37">
         <v>1</v>
       </c>
-      <c r="K30" s="37" t="s">
+      <c r="K30" s="37">
+        <v>1</v>
+      </c>
+      <c r="L30" s="37">
+        <v>185</v>
+      </c>
+      <c r="M30" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q30" s="37">
+        <v>20</v>
+      </c>
+      <c r="R30" s="15"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="37"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="23">
+        <v>1</v>
+      </c>
+      <c r="D31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0</v>
+      </c>
+      <c r="G31" s="30">
+        <v>4</v>
+      </c>
+      <c r="H31" s="25">
+        <v>0</v>
+      </c>
+      <c r="I31" s="37">
+        <v>1</v>
+      </c>
+      <c r="J31" s="37">
+        <v>1</v>
+      </c>
+      <c r="K31" s="37">
+        <v>1</v>
+      </c>
+      <c r="L31" s="37">
+        <v>185</v>
+      </c>
+      <c r="M31" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L30" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M30" s="4">
-        <v>0</v>
-      </c>
-      <c r="N30" s="4">
+      <c r="N31" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4">
         <v>0.1</v>
       </c>
-      <c r="O30" s="37">
+      <c r="Q31" s="37">
         <v>2</v>
       </c>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="37"/>
-    </row>
-    <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="R31" s="15"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="37"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" s="26">
-        <v>1</v>
-      </c>
-      <c r="D31" s="27">
-        <v>0</v>
-      </c>
-      <c r="E31" s="27">
-        <v>0</v>
-      </c>
-      <c r="F31" s="27">
-        <v>0</v>
-      </c>
-      <c r="G31" s="29">
+      <c r="B32" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" s="26">
+        <v>1</v>
+      </c>
+      <c r="D32" s="27">
+        <v>0</v>
+      </c>
+      <c r="E32" s="27">
+        <v>0</v>
+      </c>
+      <c r="F32" s="27">
+        <v>0</v>
+      </c>
+      <c r="G32" s="29">
         <v>4</v>
       </c>
-      <c r="H31" s="28">
-        <v>1</v>
-      </c>
-      <c r="I31" s="38">
-        <v>1</v>
-      </c>
-      <c r="J31" s="38">
-        <v>1</v>
-      </c>
-      <c r="K31" s="38" t="s">
+      <c r="H32" s="28">
+        <v>1</v>
+      </c>
+      <c r="I32" s="38">
+        <v>1</v>
+      </c>
+      <c r="J32" s="38">
+        <v>1</v>
+      </c>
+      <c r="K32" s="38">
+        <v>1</v>
+      </c>
+      <c r="L32" s="38">
+        <v>185</v>
+      </c>
+      <c r="M32" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L31" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M31" s="13">
-        <v>0</v>
-      </c>
-      <c r="N31" s="13">
+      <c r="N32" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O32" s="13">
+        <v>0</v>
+      </c>
+      <c r="P32" s="13">
         <v>0.1</v>
       </c>
-      <c r="O31" s="38">
+      <c r="Q32" s="38">
         <v>120</v>
       </c>
-      <c r="P31" s="16" t="s">
+      <c r="R32" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q31" s="14">
+      <c r="S32" s="14">
         <v>-240</v>
       </c>
-      <c r="R31" s="14">
+      <c r="T32" s="14">
         <v>210.5</v>
       </c>
-      <c r="S31" s="38" t="s">
+      <c r="U32" s="38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C32" s="23">
-        <v>1</v>
-      </c>
-      <c r="D32" s="24">
-        <v>0</v>
-      </c>
-      <c r="E32" s="24">
-        <v>0</v>
-      </c>
-      <c r="F32" s="24">
-        <v>0</v>
-      </c>
-      <c r="G32" s="30">
-        <v>4</v>
-      </c>
-      <c r="H32" s="25">
-        <v>1</v>
-      </c>
-      <c r="I32" s="37">
-        <v>1</v>
-      </c>
-      <c r="J32" s="37">
-        <v>1</v>
-      </c>
-      <c r="K32" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M32" s="4">
-        <v>0</v>
-      </c>
-      <c r="N32" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O32" s="37">
-        <v>60</v>
-      </c>
-      <c r="P32" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q32" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R32" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S32" s="37"/>
-    </row>
-    <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="B33" s="37" t="b">
         <v>1</v>
@@ -3029,29 +3267,41 @@
       <c r="J33" s="37">
         <v>1</v>
       </c>
-      <c r="K33" s="37" t="s">
-        <v>27</v>
+      <c r="K33" s="37">
+        <v>1</v>
       </c>
       <c r="L33" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0</v>
-      </c>
-      <c r="N33" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="O33" s="37">
+        <v>185</v>
+      </c>
+      <c r="M33" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="37"/>
-    </row>
-    <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N33" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0</v>
+      </c>
+      <c r="P33" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q33" s="37">
+        <v>60</v>
+      </c>
+      <c r="R33" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S33" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T33" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U33" s="37"/>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="37" t="b">
         <v>1</v>
@@ -3080,145 +3330,157 @@
       <c r="J34" s="37">
         <v>1</v>
       </c>
-      <c r="K34" s="37" t="s">
+      <c r="K34" s="37">
+        <v>1</v>
+      </c>
+      <c r="L34" s="37">
+        <v>185</v>
+      </c>
+      <c r="M34" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N34" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O34" s="4">
+        <v>0</v>
+      </c>
+      <c r="P34" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="Q34" s="37">
+        <v>20</v>
+      </c>
+      <c r="R34" s="15"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="37"/>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="23">
+        <v>1</v>
+      </c>
+      <c r="D35" s="24">
+        <v>0</v>
+      </c>
+      <c r="E35" s="24">
+        <v>0</v>
+      </c>
+      <c r="F35" s="24">
+        <v>0</v>
+      </c>
+      <c r="G35" s="30">
+        <v>4</v>
+      </c>
+      <c r="H35" s="25">
+        <v>1</v>
+      </c>
+      <c r="I35" s="37">
+        <v>1</v>
+      </c>
+      <c r="J35" s="37">
+        <v>1</v>
+      </c>
+      <c r="K35" s="37">
+        <v>1</v>
+      </c>
+      <c r="L35" s="37">
+        <v>185</v>
+      </c>
+      <c r="M35" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L34" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0</v>
-      </c>
-      <c r="N34" s="4">
+      <c r="N35" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O35" s="4">
+        <v>0</v>
+      </c>
+      <c r="P35" s="4">
         <v>0.03</v>
       </c>
-      <c r="O34" s="37">
-        <v>1</v>
-      </c>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="37"/>
-    </row>
-    <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="Q35" s="37">
+        <v>1</v>
+      </c>
+      <c r="R35" s="15"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="37"/>
+    </row>
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C35" s="26">
+      <c r="B36" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" s="26">
         <v>2</v>
       </c>
-      <c r="D35" s="27">
-        <v>0</v>
-      </c>
-      <c r="E35" s="27">
-        <v>0</v>
-      </c>
-      <c r="F35" s="27">
-        <v>0</v>
-      </c>
-      <c r="G35" s="29">
+      <c r="D36" s="27">
+        <v>0</v>
+      </c>
+      <c r="E36" s="27">
+        <v>0</v>
+      </c>
+      <c r="F36" s="27">
+        <v>0</v>
+      </c>
+      <c r="G36" s="29">
         <v>4</v>
       </c>
-      <c r="H35" s="28">
-        <v>1</v>
-      </c>
-      <c r="I35" s="38">
-        <v>1</v>
-      </c>
-      <c r="J35" s="38">
-        <v>1</v>
-      </c>
-      <c r="K35" s="38" t="s">
+      <c r="H36" s="28">
+        <v>1</v>
+      </c>
+      <c r="I36" s="38">
+        <v>1</v>
+      </c>
+      <c r="J36" s="38">
+        <v>1</v>
+      </c>
+      <c r="K36" s="38">
+        <v>1</v>
+      </c>
+      <c r="L36" s="38">
+        <v>185</v>
+      </c>
+      <c r="M36" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L35" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M35" s="13">
-        <v>0</v>
-      </c>
-      <c r="N35" s="13">
+      <c r="N36" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O36" s="13">
+        <v>0</v>
+      </c>
+      <c r="P36" s="13">
         <v>0.1</v>
       </c>
-      <c r="O35" s="38">
+      <c r="Q36" s="38">
         <v>120</v>
       </c>
-      <c r="P35" s="16" t="s">
+      <c r="R36" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q35" s="14">
+      <c r="S36" s="14">
         <v>-240</v>
       </c>
-      <c r="R35" s="14">
+      <c r="T36" s="14">
         <v>210.5</v>
       </c>
-      <c r="S35" s="38" t="s">
+      <c r="U36" s="38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B36" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C36" s="23">
-        <v>2</v>
-      </c>
-      <c r="D36" s="24">
-        <v>0</v>
-      </c>
-      <c r="E36" s="24">
-        <v>0</v>
-      </c>
-      <c r="F36" s="24">
-        <v>0</v>
-      </c>
-      <c r="G36" s="30">
-        <v>4</v>
-      </c>
-      <c r="H36" s="25">
-        <v>1</v>
-      </c>
-      <c r="I36" s="37">
-        <v>1</v>
-      </c>
-      <c r="J36" s="37">
-        <v>1</v>
-      </c>
-      <c r="K36" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M36" s="4">
-        <v>0</v>
-      </c>
-      <c r="N36" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="O36" s="37">
-        <v>60</v>
-      </c>
-      <c r="P36" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q36" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R36" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S36" s="37"/>
-    </row>
-    <row r="37" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="B37" s="37" t="b">
         <v>1</v>
@@ -3247,29 +3509,41 @@
       <c r="J37" s="37">
         <v>1</v>
       </c>
-      <c r="K37" s="37" t="s">
-        <v>27</v>
+      <c r="K37" s="37">
+        <v>1</v>
       </c>
       <c r="L37" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M37" s="4">
-        <v>0</v>
-      </c>
-      <c r="N37" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="O37" s="37">
+        <v>185</v>
+      </c>
+      <c r="M37" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="37"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N37" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O37" s="4">
+        <v>0</v>
+      </c>
+      <c r="P37" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Q37" s="37">
+        <v>60</v>
+      </c>
+      <c r="R37" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S37" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T37" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U37" s="37"/>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="37" t="b">
         <v>1</v>
@@ -3298,145 +3572,157 @@
       <c r="J38" s="37">
         <v>1</v>
       </c>
-      <c r="K38" s="37" t="s">
+      <c r="K38" s="37">
+        <v>1</v>
+      </c>
+      <c r="L38" s="37">
+        <v>185</v>
+      </c>
+      <c r="M38" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O38" s="4">
+        <v>0</v>
+      </c>
+      <c r="P38" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="Q38" s="37">
+        <v>20</v>
+      </c>
+      <c r="R38" s="15"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="37"/>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="23">
+        <v>2</v>
+      </c>
+      <c r="D39" s="24">
+        <v>0</v>
+      </c>
+      <c r="E39" s="24">
+        <v>0</v>
+      </c>
+      <c r="F39" s="24">
+        <v>0</v>
+      </c>
+      <c r="G39" s="30">
+        <v>4</v>
+      </c>
+      <c r="H39" s="25">
+        <v>1</v>
+      </c>
+      <c r="I39" s="37">
+        <v>1</v>
+      </c>
+      <c r="J39" s="37">
+        <v>1</v>
+      </c>
+      <c r="K39" s="37">
+        <v>1</v>
+      </c>
+      <c r="L39" s="37">
+        <v>185</v>
+      </c>
+      <c r="M39" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L38" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
+      <c r="N39" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O39" s="4">
+        <v>0</v>
+      </c>
+      <c r="P39" s="4">
         <v>0.1</v>
       </c>
-      <c r="O38" s="37">
-        <v>1</v>
-      </c>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="37"/>
-    </row>
-    <row r="39" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="Q39" s="37">
+        <v>1</v>
+      </c>
+      <c r="R39" s="15"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="37"/>
+    </row>
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C39" s="26">
-        <v>1</v>
-      </c>
-      <c r="D39" s="27">
-        <v>0</v>
-      </c>
-      <c r="E39" s="27">
-        <v>0</v>
-      </c>
-      <c r="F39" s="27">
-        <v>0</v>
-      </c>
-      <c r="G39" s="29">
+      <c r="B40" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="26">
+        <v>1</v>
+      </c>
+      <c r="D40" s="27">
+        <v>0</v>
+      </c>
+      <c r="E40" s="27">
+        <v>0</v>
+      </c>
+      <c r="F40" s="27">
+        <v>0</v>
+      </c>
+      <c r="G40" s="29">
         <v>2</v>
       </c>
-      <c r="H39" s="28">
-        <v>0</v>
-      </c>
-      <c r="I39" s="38">
-        <v>1</v>
-      </c>
-      <c r="J39" s="38">
-        <v>1</v>
-      </c>
-      <c r="K39" s="38" t="s">
+      <c r="H40" s="28">
+        <v>0</v>
+      </c>
+      <c r="I40" s="38">
+        <v>1</v>
+      </c>
+      <c r="J40" s="38">
+        <v>1</v>
+      </c>
+      <c r="K40" s="38">
+        <v>1</v>
+      </c>
+      <c r="L40" s="38">
+        <v>185</v>
+      </c>
+      <c r="M40" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L39" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M39" s="13">
-        <v>0</v>
-      </c>
-      <c r="N39" s="13">
-        <v>1</v>
-      </c>
-      <c r="O39" s="38">
+      <c r="N40" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O40" s="13">
+        <v>0</v>
+      </c>
+      <c r="P40" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="38">
         <v>120</v>
       </c>
-      <c r="P39" s="16" t="s">
+      <c r="R40" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q39" s="14">
+      <c r="S40" s="14">
         <v>-240</v>
       </c>
-      <c r="R39" s="14">
+      <c r="T40" s="14">
         <v>210.5</v>
       </c>
-      <c r="S39" s="38" t="s">
+      <c r="U40" s="38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B40" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C40" s="23">
-        <v>1</v>
-      </c>
-      <c r="D40" s="24">
-        <v>0</v>
-      </c>
-      <c r="E40" s="24">
-        <v>0</v>
-      </c>
-      <c r="F40" s="24">
-        <v>0</v>
-      </c>
-      <c r="G40" s="30">
-        <v>2</v>
-      </c>
-      <c r="H40" s="25">
-        <v>0</v>
-      </c>
-      <c r="I40" s="37">
-        <v>1</v>
-      </c>
-      <c r="J40" s="37">
-        <v>1</v>
-      </c>
-      <c r="K40" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M40" s="4">
-        <v>0</v>
-      </c>
-      <c r="N40" s="4">
-        <v>1</v>
-      </c>
-      <c r="O40" s="37">
-        <v>60</v>
-      </c>
-      <c r="P40" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q40" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R40" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S40" s="37"/>
-    </row>
-    <row r="41" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="B41" s="37" t="b">
         <v>1</v>
@@ -3465,29 +3751,41 @@
       <c r="J41" s="37">
         <v>1</v>
       </c>
-      <c r="K41" s="37" t="s">
-        <v>27</v>
+      <c r="K41" s="37">
+        <v>1</v>
       </c>
       <c r="L41" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M41" s="4">
-        <v>0</v>
-      </c>
-      <c r="N41" s="4">
-        <v>1</v>
-      </c>
-      <c r="O41" s="37">
+        <v>185</v>
+      </c>
+      <c r="M41" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="37"/>
-    </row>
-    <row r="42" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N41" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O41" s="4">
+        <v>0</v>
+      </c>
+      <c r="P41" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="37">
+        <v>60</v>
+      </c>
+      <c r="R41" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S41" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T41" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U41" s="37"/>
+    </row>
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B42" s="37" t="b">
         <v>1</v>
@@ -3516,145 +3814,157 @@
       <c r="J42" s="37">
         <v>1</v>
       </c>
-      <c r="K42" s="37" t="s">
+      <c r="K42" s="37">
+        <v>1</v>
+      </c>
+      <c r="L42" s="37">
+        <v>185</v>
+      </c>
+      <c r="M42" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N42" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O42" s="4">
+        <v>0</v>
+      </c>
+      <c r="P42" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="37">
+        <v>20</v>
+      </c>
+      <c r="R42" s="15"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="37"/>
+    </row>
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" s="23">
+        <v>1</v>
+      </c>
+      <c r="D43" s="24">
+        <v>0</v>
+      </c>
+      <c r="E43" s="24">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
+        <v>0</v>
+      </c>
+      <c r="G43" s="30">
+        <v>2</v>
+      </c>
+      <c r="H43" s="25">
+        <v>0</v>
+      </c>
+      <c r="I43" s="37">
+        <v>1</v>
+      </c>
+      <c r="J43" s="37">
+        <v>1</v>
+      </c>
+      <c r="K43" s="37">
+        <v>1</v>
+      </c>
+      <c r="L43" s="37">
+        <v>185</v>
+      </c>
+      <c r="M43" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L42" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M42" s="4">
-        <v>0</v>
-      </c>
-      <c r="N42" s="4">
-        <v>1</v>
-      </c>
-      <c r="O42" s="37">
+      <c r="N43" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O43" s="4">
+        <v>0</v>
+      </c>
+      <c r="P43" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="37">
         <v>2</v>
       </c>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="37"/>
-    </row>
-    <row r="43" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="R43" s="15"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="37"/>
+    </row>
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C43" s="26">
+      <c r="B44" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="26">
         <v>2</v>
       </c>
-      <c r="D43" s="27">
-        <v>0</v>
-      </c>
-      <c r="E43" s="27">
-        <v>0</v>
-      </c>
-      <c r="F43" s="27">
-        <v>0</v>
-      </c>
-      <c r="G43" s="29">
+      <c r="D44" s="27">
+        <v>0</v>
+      </c>
+      <c r="E44" s="27">
+        <v>0</v>
+      </c>
+      <c r="F44" s="27">
+        <v>0</v>
+      </c>
+      <c r="G44" s="29">
         <v>2</v>
       </c>
-      <c r="H43" s="28">
-        <v>0</v>
-      </c>
-      <c r="I43" s="38">
-        <v>1</v>
-      </c>
-      <c r="J43" s="38">
-        <v>1</v>
-      </c>
-      <c r="K43" s="38" t="s">
+      <c r="H44" s="28">
+        <v>0</v>
+      </c>
+      <c r="I44" s="38">
+        <v>1</v>
+      </c>
+      <c r="J44" s="38">
+        <v>1</v>
+      </c>
+      <c r="K44" s="38">
+        <v>1</v>
+      </c>
+      <c r="L44" s="38">
+        <v>185</v>
+      </c>
+      <c r="M44" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L43" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M43" s="16">
-        <v>0</v>
-      </c>
-      <c r="N43" s="14">
-        <v>1</v>
-      </c>
-      <c r="O43" s="38">
+      <c r="N44" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O44" s="16">
+        <v>0</v>
+      </c>
+      <c r="P44" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="38">
         <v>120</v>
       </c>
-      <c r="P43" s="16" t="s">
+      <c r="R44" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q43" s="14">
+      <c r="S44" s="14">
         <v>-240</v>
       </c>
-      <c r="R43" s="14">
+      <c r="T44" s="14">
         <v>210.5</v>
       </c>
-      <c r="S43" s="38" t="s">
+      <c r="U44" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B44" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C44" s="23">
-        <v>2</v>
-      </c>
-      <c r="D44" s="24">
-        <v>0</v>
-      </c>
-      <c r="E44" s="24">
-        <v>0</v>
-      </c>
-      <c r="F44" s="24">
-        <v>0</v>
-      </c>
-      <c r="G44" s="30">
-        <v>2</v>
-      </c>
-      <c r="H44" s="25">
-        <v>0</v>
-      </c>
-      <c r="I44" s="37">
-        <v>1</v>
-      </c>
-      <c r="J44" s="37">
-        <v>1</v>
-      </c>
-      <c r="K44" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M44" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="N44" s="5">
-        <v>1</v>
-      </c>
-      <c r="O44" s="37">
-        <v>60</v>
-      </c>
-      <c r="P44" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q44" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R44" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S44" s="37"/>
-    </row>
-    <row r="45" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="B45" s="37" t="b">
         <v>1</v>
@@ -3683,29 +3993,41 @@
       <c r="J45" s="37">
         <v>1</v>
       </c>
-      <c r="K45" s="37" t="s">
-        <v>27</v>
+      <c r="K45" s="37">
+        <v>1</v>
       </c>
       <c r="L45" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M45" s="15">
-        <v>0</v>
-      </c>
-      <c r="N45" s="5">
-        <v>1</v>
-      </c>
-      <c r="O45" s="37">
+        <v>185</v>
+      </c>
+      <c r="M45" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="37"/>
-    </row>
-    <row r="46" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N45" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O45" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="P45" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="37">
+        <v>60</v>
+      </c>
+      <c r="R45" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S45" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T45" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U45" s="37"/>
+    </row>
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="37" t="b">
         <v>1</v>
@@ -3734,145 +4056,157 @@
       <c r="J46" s="37">
         <v>1</v>
       </c>
-      <c r="K46" s="37" t="s">
+      <c r="K46" s="37">
+        <v>1</v>
+      </c>
+      <c r="L46" s="37">
+        <v>185</v>
+      </c>
+      <c r="M46" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O46" s="15">
+        <v>0</v>
+      </c>
+      <c r="P46" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="37">
+        <v>20</v>
+      </c>
+      <c r="R46" s="15"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="37"/>
+    </row>
+    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" s="23">
+        <v>2</v>
+      </c>
+      <c r="D47" s="24">
+        <v>0</v>
+      </c>
+      <c r="E47" s="24">
+        <v>0</v>
+      </c>
+      <c r="F47" s="24">
+        <v>0</v>
+      </c>
+      <c r="G47" s="30">
+        <v>2</v>
+      </c>
+      <c r="H47" s="25">
+        <v>0</v>
+      </c>
+      <c r="I47" s="37">
+        <v>1</v>
+      </c>
+      <c r="J47" s="37">
+        <v>1</v>
+      </c>
+      <c r="K47" s="37">
+        <v>1</v>
+      </c>
+      <c r="L47" s="37">
+        <v>185</v>
+      </c>
+      <c r="M47" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L46" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M46" s="15">
-        <v>0</v>
-      </c>
-      <c r="N46" s="5">
-        <v>1</v>
-      </c>
-      <c r="O46" s="37">
+      <c r="N47" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O47" s="15">
+        <v>0</v>
+      </c>
+      <c r="P47" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="37">
         <v>2</v>
       </c>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="37"/>
-    </row>
-    <row r="47" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+      <c r="R47" s="15"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="37"/>
+    </row>
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C47" s="26">
+      <c r="B48" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" s="26">
         <v>3</v>
       </c>
-      <c r="D47" s="27">
-        <v>0</v>
-      </c>
-      <c r="E47" s="27">
-        <v>0</v>
-      </c>
-      <c r="F47" s="27">
-        <v>0</v>
-      </c>
-      <c r="G47" s="29">
+      <c r="D48" s="27">
+        <v>0</v>
+      </c>
+      <c r="E48" s="27">
+        <v>0</v>
+      </c>
+      <c r="F48" s="27">
+        <v>0</v>
+      </c>
+      <c r="G48" s="29">
         <v>2</v>
       </c>
-      <c r="H47" s="28">
-        <v>0</v>
-      </c>
-      <c r="I47" s="38">
-        <v>1</v>
-      </c>
-      <c r="J47" s="38">
-        <v>1</v>
-      </c>
-      <c r="K47" s="38" t="s">
+      <c r="H48" s="28">
+        <v>0</v>
+      </c>
+      <c r="I48" s="38">
+        <v>1</v>
+      </c>
+      <c r="J48" s="38">
+        <v>1</v>
+      </c>
+      <c r="K48" s="38">
+        <v>1</v>
+      </c>
+      <c r="L48" s="38">
+        <v>185</v>
+      </c>
+      <c r="M48" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L47" s="38">
-        <v>212.5</v>
-      </c>
-      <c r="M47" s="13">
-        <v>0</v>
-      </c>
-      <c r="N47" s="13">
-        <v>1</v>
-      </c>
-      <c r="O47" s="38">
+      <c r="N48" s="38">
+        <v>212.5</v>
+      </c>
+      <c r="O48" s="13">
+        <v>0</v>
+      </c>
+      <c r="P48" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="38">
         <v>120</v>
       </c>
-      <c r="P47" s="16" t="s">
+      <c r="R48" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Q47" s="14">
+      <c r="S48" s="14">
         <v>-240</v>
       </c>
-      <c r="R47" s="14">
+      <c r="T48" s="14">
         <v>210.5</v>
       </c>
-      <c r="S47" s="14" t="s">
+      <c r="U48" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B48" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C48" s="23">
-        <v>3</v>
-      </c>
-      <c r="D48" s="24">
-        <v>0</v>
-      </c>
-      <c r="E48" s="24">
-        <v>0</v>
-      </c>
-      <c r="F48" s="24">
-        <v>0</v>
-      </c>
-      <c r="G48" s="30">
-        <v>2</v>
-      </c>
-      <c r="H48" s="25">
-        <v>0</v>
-      </c>
-      <c r="I48" s="37">
-        <v>1</v>
-      </c>
-      <c r="J48" s="37">
-        <v>1</v>
-      </c>
-      <c r="K48" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M48" s="4">
-        <v>0</v>
-      </c>
-      <c r="N48" s="4">
-        <v>1</v>
-      </c>
-      <c r="O48" s="37">
-        <v>60</v>
-      </c>
-      <c r="P48" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q48" s="5">
-        <v>-240</v>
-      </c>
-      <c r="R48" s="5">
-        <v>210.5</v>
-      </c>
-      <c r="S48" s="5"/>
-    </row>
-    <row r="49" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="B49" s="37" t="b">
         <v>1</v>
@@ -3901,76 +4235,151 @@
       <c r="J49" s="37">
         <v>1</v>
       </c>
-      <c r="K49" s="37" t="s">
+      <c r="K49" s="37">
+        <v>1</v>
+      </c>
+      <c r="L49" s="37">
+        <v>185</v>
+      </c>
+      <c r="M49" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N49" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O49" s="4">
+        <v>0</v>
+      </c>
+      <c r="P49" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="37">
+        <v>60</v>
+      </c>
+      <c r="R49" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S49" s="5">
+        <v>-240</v>
+      </c>
+      <c r="T49" s="5">
+        <v>210.5</v>
+      </c>
+      <c r="U49" s="5"/>
+    </row>
+    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="23">
+        <v>3</v>
+      </c>
+      <c r="D50" s="24">
+        <v>0</v>
+      </c>
+      <c r="E50" s="24">
+        <v>0</v>
+      </c>
+      <c r="F50" s="24">
+        <v>0</v>
+      </c>
+      <c r="G50" s="30">
+        <v>2</v>
+      </c>
+      <c r="H50" s="25">
+        <v>0</v>
+      </c>
+      <c r="I50" s="37">
+        <v>1</v>
+      </c>
+      <c r="J50" s="37">
+        <v>1</v>
+      </c>
+      <c r="K50" s="37">
+        <v>1</v>
+      </c>
+      <c r="L50" s="37">
+        <v>185</v>
+      </c>
+      <c r="M50" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="L49" s="37">
-        <v>212.5</v>
-      </c>
-      <c r="M49" s="4">
-        <v>0</v>
-      </c>
-      <c r="N49" s="4">
-        <v>1</v>
-      </c>
-      <c r="O49" s="37">
+      <c r="N50" s="37">
+        <v>212.5</v>
+      </c>
+      <c r="O50" s="4">
+        <v>0</v>
+      </c>
+      <c r="P50" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="37">
         <v>20</v>
       </c>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="5"/>
-    </row>
-    <row r="50" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+      <c r="R50" s="15"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+    </row>
+    <row r="51" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="C50" s="31">
+      <c r="B51" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" s="31">
         <v>3</v>
       </c>
-      <c r="D50" s="32">
-        <v>0</v>
-      </c>
-      <c r="E50" s="32">
-        <v>0</v>
-      </c>
-      <c r="F50" s="32">
-        <v>0</v>
-      </c>
-      <c r="G50" s="33">
+      <c r="D51" s="32">
+        <v>0</v>
+      </c>
+      <c r="E51" s="32">
+        <v>0</v>
+      </c>
+      <c r="F51" s="32">
+        <v>0</v>
+      </c>
+      <c r="G51" s="33">
         <v>2</v>
       </c>
-      <c r="H50" s="34">
-        <v>0</v>
-      </c>
-      <c r="I50" s="39">
-        <v>1</v>
-      </c>
-      <c r="J50" s="39">
-        <v>1</v>
-      </c>
-      <c r="K50" s="39" t="s">
+      <c r="H51" s="34">
+        <v>0</v>
+      </c>
+      <c r="I51" s="39">
+        <v>1</v>
+      </c>
+      <c r="J51" s="39">
+        <v>1</v>
+      </c>
+      <c r="K51" s="39">
+        <v>1</v>
+      </c>
+      <c r="L51" s="39">
+        <v>185</v>
+      </c>
+      <c r="M51" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="L50" s="39">
-        <v>212.5</v>
-      </c>
-      <c r="M50" s="7">
-        <v>0</v>
-      </c>
-      <c r="N50" s="7">
-        <v>1</v>
-      </c>
-      <c r="O50" s="39">
+      <c r="N51" s="39">
+        <v>212.5</v>
+      </c>
+      <c r="O51" s="7">
+        <v>0</v>
+      </c>
+      <c r="P51" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="39">
         <v>2</v>
       </c>
-      <c r="P50" s="17"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
     </row>
   </sheetData>
   <sortState ref="A3:P76">
@@ -3978,31 +4387,31 @@
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
-  <conditionalFormatting sqref="S4:S5 K4:Q5 K6:S6 A4:J6 A7:S50">
-    <cfRule type="expression" dxfId="0" priority="5">
+  <conditionalFormatting sqref="U4:U5 M4:S5 M6:U6 A4:L6 A7:U51">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:S3">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="A3:U3">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$B3&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R4">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="T4">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$B4&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="T5">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$B5&lt;&gt;TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B51">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>